<commit_message>
Recalibrate TTS for passenger LDVs
</commit_message>
<xml_diff>
--- a/InputData/trans/TTS/Transportation Technology Shareweights.xlsx
+++ b/InputData/trans/TTS/Transportation Technology Shareweights.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\TTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951B494E-2243-4188-9826-6551E88F9560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E1B76E-8504-4262-9456-2423C1D1900C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -3259,94 +3259,94 @@
                   <c:v>2.4033772409275102E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.8452728387264615E-2</c:v>
+                  <c:v>3.0565768877676487E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.3397240750809356E-2</c:v>
+                  <c:v>3.4756657361210842E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.999153989574362E-2</c:v>
+                  <c:v>4.1587705894632315E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.8750051814605499E-2</c:v>
+                  <c:v>5.264151967794517E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>7.0319822944581098E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.5493641158949502E-2</c:v>
+                  <c:v>9.806879419650627E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.10520751524499683</c:v>
+                  <c:v>0.14037179853299253</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.13050858543369728</c:v>
+                  <c:v>0.20207492269482669</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.16247562109993127</c:v>
+                  <c:v>0.28651151686663684</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.20207492269482669</c:v>
+                  <c:v>0.39250071469828041</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.24994576623848519</c:v>
+                  <c:v>0.51201688620463759</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.30613729591557276</c:v>
+                  <c:v>0.63153305771099466</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.36986125049264856</c:v>
+                  <c:v>0.73752225554263828</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.43936350389960366</c:v>
+                  <c:v>0.82195884971444833</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.51201688620463759</c:v>
+                  <c:v>0.88366197387628254</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.58467026850967152</c:v>
+                  <c:v>0.92596497821276891</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.65417252191662656</c:v>
+                  <c:v>0.95371394946469412</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.71789647649370236</c:v>
+                  <c:v>0.9713922527313299</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.77408800617078988</c:v>
+                  <c:v>0.98244606651464272</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.82195884971444833</c:v>
+                  <c:v>0.98927711504806426</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.86155815130934388</c:v>
+                  <c:v>0.9934680035315987</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.89352518697557781</c:v>
+                  <c:v>0.99602768304764211</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.91882625716427835</c:v>
+                  <c:v>0.99758680330556582</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.93854013125032565</c:v>
+                  <c:v>0.9985348968159663</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.95371394946469412</c:v>
+                  <c:v>0.99911084480265877</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.9652837205946696</c:v>
+                  <c:v>0.99946050671902897</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.97404223251353139</c:v>
+                  <c:v>0.99967270959824672</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.98063653165846576</c:v>
+                  <c:v>0.99980146213963728</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.98558104402201052</c:v>
+                  <c:v>0.99987957106116954</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.98927711504806426</c:v>
+                  <c:v>0.99992695260968711</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4130,16 +4130,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>79374</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>67468</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>555624</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>111918</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>391320</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>130175</xdr:rowOff>
+      <xdr:colOff>226220</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4490,7 +4490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -51985,8 +51985,8 @@
   </sheetPr>
   <dimension ref="A1:AL93"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10:AL10"/>
+    <sheetView tabSelected="1" topLeftCell="G4" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -52052,7 +52052,7 @@
         <v>100</v>
       </c>
       <c r="O3" s="26">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="4" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -52069,7 +52069,7 @@
         <v>101</v>
       </c>
       <c r="O4" s="27">
-        <v>-5</v>
+        <v>-12</v>
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.35">
@@ -52101,7 +52101,7 @@
         <v>2020</v>
       </c>
       <c r="E7" s="2">
-        <v>2035</v>
+        <v>2050</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -52283,128 +52283,128 @@
         <v>s-curve</v>
       </c>
       <c r="H10" s="29">
-        <f t="shared" ref="H10:H40" si="1">D10</f>
+        <f t="shared" ref="H10" si="1">D10</f>
         <v>2.4033772409275102E-2</v>
       </c>
       <c r="I10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:I$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,I$9))</f>
-        <v>3.8452728387264615E-2</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:I$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,I$9))</f>
+        <v>3.0565768877676487E-2</v>
       </c>
       <c r="J10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:J$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,J$9))</f>
-        <v>4.3397240750809356E-2</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:J$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,J$9))</f>
+        <v>3.4756657361210842E-2</v>
       </c>
       <c r="K10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:K$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,K$9))</f>
-        <v>4.999153989574362E-2</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:K$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,K$9))</f>
+        <v>4.1587705894632315E-2</v>
       </c>
       <c r="L10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:L$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,L$9))</f>
-        <v>5.8750051814605499E-2</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:L$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,L$9))</f>
+        <v>5.264151967794517E-2</v>
       </c>
       <c r="M10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:M$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,M$9))</f>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:M$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,M$9))</f>
         <v>7.0319822944581098E-2</v>
       </c>
       <c r="N10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:N$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,N$9))</f>
-        <v>8.5493641158949502E-2</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:N$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,N$9))</f>
+        <v>9.806879419650627E-2</v>
       </c>
       <c r="O10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:O$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,O$9))</f>
-        <v>0.10520751524499683</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:O$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,O$9))</f>
+        <v>0.14037179853299253</v>
       </c>
       <c r="P10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:P$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,P$9))</f>
-        <v>0.13050858543369728</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:P$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,P$9))</f>
+        <v>0.20207492269482669</v>
       </c>
       <c r="Q10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:Q$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,Q$9))</f>
-        <v>0.16247562109993127</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:Q$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,Q$9))</f>
+        <v>0.28651151686663684</v>
       </c>
       <c r="R10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:R$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,R$9))</f>
-        <v>0.20207492269482669</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:R$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,R$9))</f>
+        <v>0.39250071469828041</v>
       </c>
       <c r="S10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:S$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,S$9))</f>
-        <v>0.24994576623848519</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:S$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,S$9))</f>
+        <v>0.51201688620463759</v>
       </c>
       <c r="T10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:T$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,T$9))</f>
-        <v>0.30613729591557276</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:T$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,T$9))</f>
+        <v>0.63153305771099466</v>
       </c>
       <c r="U10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:U$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,U$9))</f>
-        <v>0.36986125049264856</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:U$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,U$9))</f>
+        <v>0.73752225554263828</v>
       </c>
       <c r="V10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:V$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,V$9))</f>
-        <v>0.43936350389960366</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:V$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,V$9))</f>
+        <v>0.82195884971444833</v>
       </c>
       <c r="W10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:W$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,W$9))</f>
-        <v>0.51201688620463759</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:W$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,W$9))</f>
+        <v>0.88366197387628254</v>
       </c>
       <c r="X10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:X$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,X$9))</f>
-        <v>0.58467026850967152</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:X$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,X$9))</f>
+        <v>0.92596497821276891</v>
       </c>
       <c r="Y10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:Y$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,Y$9))</f>
-        <v>0.65417252191662656</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:Y$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,Y$9))</f>
+        <v>0.95371394946469412</v>
       </c>
       <c r="Z10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:Z$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,Z$9))</f>
-        <v>0.71789647649370236</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:Z$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,Z$9))</f>
+        <v>0.9713922527313299</v>
       </c>
       <c r="AA10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:AA$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,AA$9))</f>
-        <v>0.77408800617078988</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:AA$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,AA$9))</f>
+        <v>0.98244606651464272</v>
       </c>
       <c r="AB10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:AB$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,AB$9))</f>
-        <v>0.82195884971444833</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:AB$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,AB$9))</f>
+        <v>0.98927711504806426</v>
       </c>
       <c r="AC10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:AC$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,AC$9))</f>
-        <v>0.86155815130934388</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:AC$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,AC$9))</f>
+        <v>0.9934680035315987</v>
       </c>
       <c r="AD10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:AD$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,AD$9))</f>
-        <v>0.89352518697557781</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:AD$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,AD$9))</f>
+        <v>0.99602768304764211</v>
       </c>
       <c r="AE10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:AE$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,AE$9))</f>
-        <v>0.91882625716427835</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:AE$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,AE$9))</f>
+        <v>0.99758680330556582</v>
       </c>
       <c r="AF10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:AF$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,AF$9))</f>
-        <v>0.93854013125032565</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:AF$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,AF$9))</f>
+        <v>0.9985348968159663</v>
       </c>
       <c r="AG10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:AG$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,AG$9))</f>
-        <v>0.95371394946469412</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:AG$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,AG$9))</f>
+        <v>0.99911084480265877</v>
       </c>
       <c r="AH10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:AH$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,AH$9))</f>
-        <v>0.9652837205946696</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:AH$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,AH$9))</f>
+        <v>0.99946050671902897</v>
       </c>
       <c r="AI10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:AI$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,AI$9))</f>
-        <v>0.97404223251353139</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:AI$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,AI$9))</f>
+        <v>0.99967270959824672</v>
       </c>
       <c r="AJ10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:AJ$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,AJ$9))</f>
-        <v>0.98063653165846576</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:AJ$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,AJ$9))</f>
+        <v>0.99980146213963728</v>
       </c>
       <c r="AK10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:AK$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,AK$9))</f>
-        <v>0.98558104402201052</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:AK$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,AK$9))</f>
+        <v>0.99987957106116954</v>
       </c>
       <c r="AL10" s="15">
-        <f>IF($F10="s-curve",$D10+($E10-$D10)*$I$2/(1+EXP($I$3*(COUNT($H$9:AL$9)+$I$4))),TREND($D10:$E10,$D$9:$E$9,AL$9))</f>
-        <v>0.98927711504806426</v>
+        <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:AL$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,AL$9))</f>
+        <v>0.99992695260968711</v>
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.35">
@@ -52424,7 +52424,7 @@
         <v>s-curve</v>
       </c>
       <c r="H11" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="H11:H40" si="2">D11</f>
         <v>3.8057610451262282E-4</v>
       </c>
       <c r="I11" s="15">
@@ -52563,7 +52563,7 @@
         <v>n/a</v>
       </c>
       <c r="H12" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I12" s="15">
@@ -52704,7 +52704,7 @@
         <v>linear</v>
       </c>
       <c r="H13" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.2138566319580755E-3</v>
       </c>
       <c r="I13" s="15">
@@ -52845,7 +52845,7 @@
         <v>s-curve</v>
       </c>
       <c r="H14" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.731416359500128E-3</v>
       </c>
       <c r="I14" s="15">
@@ -52986,7 +52986,7 @@
         <v>linear</v>
       </c>
       <c r="H15" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.186067677034385E-4</v>
       </c>
       <c r="I15" s="15">
@@ -53129,7 +53129,7 @@
         <v>s-curve</v>
       </c>
       <c r="H16" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9671627040405578E-5</v>
       </c>
       <c r="I16" s="15">
@@ -53276,7 +53276,7 @@
         <v>s-curve</v>
       </c>
       <c r="H17" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.0163026481612729E-6</v>
       </c>
       <c r="I17" s="15">
@@ -53416,7 +53416,7 @@
         <v>123</v>
       </c>
       <c r="H18" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.2417684632922508E-3</v>
       </c>
       <c r="I18" s="15">
@@ -53555,7 +53555,7 @@
         <v>n/a</v>
       </c>
       <c r="H19" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I19" s="15">
@@ -53695,7 +53695,7 @@
         <v>linear</v>
       </c>
       <c r="H20" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.82010231357952423</v>
       </c>
       <c r="I20" s="15">
@@ -53836,7 +53836,7 @@
         <v>s-curve</v>
       </c>
       <c r="H21" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I21" s="15">
@@ -53977,7 +53977,7 @@
         <v>linear</v>
       </c>
       <c r="H22" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.5128616403477108E-4</v>
       </c>
       <c r="I22" s="15">
@@ -54120,7 +54120,7 @@
         <v>s-curve</v>
       </c>
       <c r="H23" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I23" s="15">
@@ -54266,7 +54266,7 @@
         <v>s-curve</v>
       </c>
       <c r="H24" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.0593729231944068E-4</v>
       </c>
       <c r="I24" s="15">
@@ -54407,7 +54407,7 @@
         <v>s-curve</v>
       </c>
       <c r="H25" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.9823199644587315E-2</v>
       </c>
       <c r="I25" s="15">
@@ -54548,7 +54548,7 @@
         <v>linear</v>
       </c>
       <c r="H26" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.9823199644587315E-2</v>
       </c>
       <c r="I26" s="15">
@@ -54687,7 +54687,7 @@
         <v>n/a</v>
       </c>
       <c r="H27" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I27" s="15">
@@ -54828,7 +54828,7 @@
         <v>s-curve</v>
       </c>
       <c r="H28" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I28" s="15">
@@ -54969,7 +54969,7 @@
         <v>linear</v>
       </c>
       <c r="H29" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.3987187287436543E-3</v>
       </c>
       <c r="I29" s="15">
@@ -55112,7 +55112,7 @@
         <v>s-curve</v>
       </c>
       <c r="H30" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.2919974477595432E-4</v>
       </c>
       <c r="I30" s="15">
@@ -55259,7 +55259,7 @@
         <v>s-curve</v>
       </c>
       <c r="H31" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.455517997108405E-4</v>
       </c>
       <c r="I31" s="15">
@@ -55400,7 +55400,7 @@
         <v>s-curve</v>
       </c>
       <c r="H32" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.2809767943268324E-3</v>
       </c>
       <c r="I32" s="15">
@@ -55539,7 +55539,7 @@
         <v>n/a</v>
       </c>
       <c r="H33" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I33" s="15">
@@ -55678,7 +55678,7 @@
         <v>n/a</v>
       </c>
       <c r="H34" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I34" s="15">
@@ -55819,7 +55819,7 @@
         <v>s-curve</v>
       </c>
       <c r="H35" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.1604589258675129E-3</v>
       </c>
       <c r="I35" s="15">
@@ -55960,7 +55960,7 @@
         <v>linear</v>
       </c>
       <c r="H36" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.9129793393846839E-4</v>
       </c>
       <c r="I36" s="15">
@@ -56103,7 +56103,7 @@
         <v>s-curve</v>
       </c>
       <c r="H37" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.2506977162920506E-5</v>
       </c>
       <c r="I37" s="15">
@@ -56248,7 +56248,7 @@
         <v>n/a</v>
       </c>
       <c r="H38" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I38" s="15">
@@ -56387,7 +56387,7 @@
         <v>n/a</v>
       </c>
       <c r="H39" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I39" s="15">
@@ -56526,7 +56526,7 @@
         <v>n/a</v>
       </c>
       <c r="H40" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I40" s="15">
@@ -56666,7 +56666,7 @@
         <v>n/a</v>
       </c>
       <c r="H41" s="29">
-        <f t="shared" ref="H41:H72" si="2">D41</f>
+        <f t="shared" ref="H41:H72" si="3">D41</f>
         <v>1</v>
       </c>
       <c r="I41" s="15">
@@ -56806,7 +56806,7 @@
         <v>n/a</v>
       </c>
       <c r="H42" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I42" s="15">
@@ -56946,7 +56946,7 @@
         <v>n/a</v>
       </c>
       <c r="H43" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I43" s="15">
@@ -57087,7 +57087,7 @@
         <v>n/a</v>
       </c>
       <c r="H44" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I44" s="15">
@@ -57232,7 +57232,7 @@
         <v>n/a</v>
       </c>
       <c r="H45" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I45" s="15">
@@ -57371,7 +57371,7 @@
         <v>n/a</v>
       </c>
       <c r="H46" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I46" s="15">
@@ -57510,7 +57510,7 @@
         <v>n/a</v>
       </c>
       <c r="H47" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I47" s="15">
@@ -57649,7 +57649,7 @@
         <v>n/a</v>
       </c>
       <c r="H48" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I48" s="15">
@@ -57788,7 +57788,7 @@
         <v>n/a</v>
       </c>
       <c r="H49" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I49" s="15">
@@ -57927,7 +57927,7 @@
         <v>n/a</v>
       </c>
       <c r="H50" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I50" s="15">
@@ -58068,7 +58068,7 @@
         <v>n/a</v>
       </c>
       <c r="H51" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I51" s="15">
@@ -58214,7 +58214,7 @@
         <v>s-curve</v>
       </c>
       <c r="H52" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.75216927859794647</v>
       </c>
       <c r="I52" s="15">
@@ -58353,7 +58353,7 @@
         <v>n/a</v>
       </c>
       <c r="H53" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I53" s="15">
@@ -58492,7 +58492,7 @@
         <v>n/a</v>
       </c>
       <c r="H54" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I54" s="15">
@@ -58632,7 +58632,7 @@
         <v>linear</v>
       </c>
       <c r="H55" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.24783072140205353</v>
       </c>
       <c r="I55" s="15">
@@ -58772,7 +58772,7 @@
         <v>n/a</v>
       </c>
       <c r="H56" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I56" s="15">
@@ -58912,7 +58912,7 @@
         <v>n/a</v>
       </c>
       <c r="H57" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I57" s="15">
@@ -59053,7 +59053,7 @@
         <v>n/a</v>
       </c>
       <c r="H58" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I58" s="15">
@@ -59198,7 +59198,7 @@
         <v>n/a</v>
       </c>
       <c r="H59" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I59" s="15">
@@ -59338,7 +59338,7 @@
         <v>n/a</v>
       </c>
       <c r="H60" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I60" s="15">
@@ -59478,7 +59478,7 @@
         <v>n/a</v>
       </c>
       <c r="H61" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I61" s="15">
@@ -59617,7 +59617,7 @@
         <v>n/a</v>
       </c>
       <c r="H62" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I62" s="15">
@@ -59756,7 +59756,7 @@
         <v>n/a</v>
       </c>
       <c r="H63" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I63" s="15">
@@ -59895,7 +59895,7 @@
         <v>n/a</v>
       </c>
       <c r="H64" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I64" s="15">
@@ -60036,7 +60036,7 @@
         <v>n/a</v>
       </c>
       <c r="H65" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I65" s="15">
@@ -60181,7 +60181,7 @@
         <v>n/a</v>
       </c>
       <c r="H66" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I66" s="15">
@@ -60320,7 +60320,7 @@
         <v>n/a</v>
       </c>
       <c r="H67" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I67" s="15">
@@ -60460,7 +60460,7 @@
         <v>linear</v>
       </c>
       <c r="H68" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.77564463977542331</v>
       </c>
       <c r="I68" s="15">
@@ -60600,7 +60600,7 @@
         <v>linear</v>
       </c>
       <c r="H69" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.22435536022457658</v>
       </c>
       <c r="I69" s="15">
@@ -60739,7 +60739,7 @@
         <v>n/a</v>
       </c>
       <c r="H70" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I70" s="15">
@@ -60878,7 +60878,7 @@
         <v>n/a</v>
       </c>
       <c r="H71" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I71" s="15">
@@ -61019,7 +61019,7 @@
         <v>n/a</v>
       </c>
       <c r="H72" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I72" s="15">
@@ -61164,7 +61164,7 @@
         <v>n/a</v>
       </c>
       <c r="H73" s="29">
-        <f t="shared" ref="H73:H93" si="3">D73</f>
+        <f t="shared" ref="H73:H93" si="4">D73</f>
         <v>0</v>
       </c>
       <c r="I73" s="15">
@@ -61303,7 +61303,7 @@
         <v>n/a</v>
       </c>
       <c r="H74" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I74" s="15">
@@ -61442,7 +61442,7 @@
         <v>n/a</v>
       </c>
       <c r="H75" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I75" s="15">
@@ -61581,7 +61581,7 @@
         <v>n/a</v>
       </c>
       <c r="H76" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I76" s="15">
@@ -61720,7 +61720,7 @@
         <v>n/a</v>
       </c>
       <c r="H77" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I77" s="15">
@@ -61859,7 +61859,7 @@
         <v>n/a</v>
       </c>
       <c r="H78" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I78" s="15">
@@ -62000,7 +62000,7 @@
         <v>n/a</v>
       </c>
       <c r="H79" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I79" s="15">
@@ -62146,7 +62146,7 @@
         <v>s-curve</v>
       </c>
       <c r="H80" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I80" s="15">
@@ -62286,7 +62286,7 @@
         <v>n/a</v>
       </c>
       <c r="H81" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I81" s="15">
@@ -62425,7 +62425,7 @@
         <v>n/a</v>
       </c>
       <c r="H82" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I82" s="15">
@@ -62565,7 +62565,7 @@
         <v>n/a</v>
       </c>
       <c r="H83" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I83" s="15">
@@ -62705,7 +62705,7 @@
         <v>n/a</v>
       </c>
       <c r="H84" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I84" s="15">
@@ -62845,7 +62845,7 @@
         <v>n/a</v>
       </c>
       <c r="H85" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I85" s="15">
@@ -62987,7 +62987,7 @@
         <v>n/a</v>
       </c>
       <c r="H86" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I86" s="15">
@@ -63132,7 +63132,7 @@
         <v>n/a</v>
       </c>
       <c r="H87" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I87" s="15">
@@ -63271,7 +63271,7 @@
         <v>n/a</v>
       </c>
       <c r="H88" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I88" s="15">
@@ -63410,7 +63410,7 @@
         <v>n/a</v>
       </c>
       <c r="H89" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I89" s="15">
@@ -63549,7 +63549,7 @@
         <v>n/a</v>
       </c>
       <c r="H90" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I90" s="15">
@@ -63688,7 +63688,7 @@
         <v>n/a</v>
       </c>
       <c r="H91" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I91" s="15">
@@ -63827,7 +63827,7 @@
         <v>n/a</v>
       </c>
       <c r="H92" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I92" s="15">
@@ -63968,7 +63968,7 @@
         <v>n/a</v>
       </c>
       <c r="H93" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I93" s="15">
@@ -64255,19 +64255,19 @@
       </c>
       <c r="C2">
         <f>Data!I10</f>
-        <v>3.8452728387264615E-2</v>
+        <v>3.0565768877676487E-2</v>
       </c>
       <c r="D2">
         <f>Data!J10</f>
-        <v>4.3397240750809356E-2</v>
+        <v>3.4756657361210842E-2</v>
       </c>
       <c r="E2">
         <f>Data!K10</f>
-        <v>4.999153989574362E-2</v>
+        <v>4.1587705894632315E-2</v>
       </c>
       <c r="F2">
         <f>Data!L10</f>
-        <v>5.8750051814605499E-2</v>
+        <v>5.264151967794517E-2</v>
       </c>
       <c r="G2">
         <f>Data!M10</f>
@@ -64275,103 +64275,103 @@
       </c>
       <c r="H2">
         <f>Data!N10</f>
-        <v>8.5493641158949502E-2</v>
+        <v>9.806879419650627E-2</v>
       </c>
       <c r="I2">
         <f>Data!O10</f>
-        <v>0.10520751524499683</v>
+        <v>0.14037179853299253</v>
       </c>
       <c r="J2">
         <f>Data!P10</f>
-        <v>0.13050858543369728</v>
+        <v>0.20207492269482669</v>
       </c>
       <c r="K2">
         <f>Data!Q10</f>
-        <v>0.16247562109993127</v>
+        <v>0.28651151686663684</v>
       </c>
       <c r="L2">
         <f>Data!R10</f>
-        <v>0.20207492269482669</v>
+        <v>0.39250071469828041</v>
       </c>
       <c r="M2">
         <f>Data!S10</f>
-        <v>0.24994576623848519</v>
+        <v>0.51201688620463759</v>
       </c>
       <c r="N2">
         <f>Data!T10</f>
-        <v>0.30613729591557276</v>
+        <v>0.63153305771099466</v>
       </c>
       <c r="O2">
         <f>Data!U10</f>
-        <v>0.36986125049264856</v>
+        <v>0.73752225554263828</v>
       </c>
       <c r="P2">
         <f>Data!V10</f>
-        <v>0.43936350389960366</v>
+        <v>0.82195884971444833</v>
       </c>
       <c r="Q2">
         <f>Data!W10</f>
-        <v>0.51201688620463759</v>
+        <v>0.88366197387628254</v>
       </c>
       <c r="R2">
         <f>Data!X10</f>
-        <v>0.58467026850967152</v>
+        <v>0.92596497821276891</v>
       </c>
       <c r="S2">
         <f>Data!Y10</f>
-        <v>0.65417252191662656</v>
+        <v>0.95371394946469412</v>
       </c>
       <c r="T2">
         <f>Data!Z10</f>
-        <v>0.71789647649370236</v>
+        <v>0.9713922527313299</v>
       </c>
       <c r="U2">
         <f>Data!AA10</f>
-        <v>0.77408800617078988</v>
+        <v>0.98244606651464272</v>
       </c>
       <c r="V2">
         <f>Data!AB10</f>
-        <v>0.82195884971444833</v>
+        <v>0.98927711504806426</v>
       </c>
       <c r="W2">
         <f>Data!AC10</f>
-        <v>0.86155815130934388</v>
+        <v>0.9934680035315987</v>
       </c>
       <c r="X2">
         <f>Data!AD10</f>
-        <v>0.89352518697557781</v>
+        <v>0.99602768304764211</v>
       </c>
       <c r="Y2">
         <f>Data!AE10</f>
-        <v>0.91882625716427835</v>
+        <v>0.99758680330556582</v>
       </c>
       <c r="Z2">
         <f>Data!AF10</f>
-        <v>0.93854013125032565</v>
+        <v>0.9985348968159663</v>
       </c>
       <c r="AA2">
         <f>Data!AG10</f>
-        <v>0.95371394946469412</v>
+        <v>0.99911084480265877</v>
       </c>
       <c r="AB2">
         <f>Data!AH10</f>
-        <v>0.9652837205946696</v>
+        <v>0.99946050671902897</v>
       </c>
       <c r="AC2">
         <f>Data!AI10</f>
-        <v>0.97404223251353139</v>
+        <v>0.99967270959824672</v>
       </c>
       <c r="AD2">
         <f>Data!AJ10</f>
-        <v>0.98063653165846576</v>
+        <v>0.99980146213963728</v>
       </c>
       <c r="AE2">
         <f>Data!AK10</f>
-        <v>0.98558104402201052</v>
+        <v>0.99987957106116954</v>
       </c>
       <c r="AF2">
         <f>Data!AL10</f>
-        <v>0.98927711504806426</v>
+        <v>0.99992695260968711</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update start year TTS value for passenger LDVs
</commit_message>
<xml_diff>
--- a/InputData/trans/TTS/Transportation Technology Shareweights.xlsx
+++ b/InputData/trans/TTS/Transportation Technology Shareweights.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\TTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E1B76E-8504-4262-9456-2423C1D1900C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C59117-3393-4404-A241-6A7581EF3C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1738" uniqueCount="928">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1737" uniqueCount="927">
   <si>
     <t>Source:</t>
   </si>
@@ -2827,13 +2827,10 @@
     <t>Psgr LDVs only</t>
   </si>
   <si>
-    <t>We assume electric passenger Evs can reach 100% by the year 2050</t>
-  </si>
-  <si>
-    <t>This results in a sales share of 21% in 2030, in line with EEI (figure to the right)</t>
-  </si>
-  <si>
-    <t>and other research.</t>
+    <t>We assume electric passenger Evs can reach 100% by the year 2040</t>
+  </si>
+  <si>
+    <t>This results in a sales share of 25% in 2030</t>
   </si>
 </sst>
 </file>
@@ -3199,6 +3196,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>TTS Value</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3249,6 +3271,108 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data!$H$9:$AL$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2037</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2038</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2041</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2042</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2043</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2044</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2046</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2047</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2049</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Data!$H$10:$AL$10</c:f>
@@ -3256,97 +3380,97 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0" formatCode="0.0000">
-                  <c:v>2.4033772409275102E-2</c:v>
+                  <c:v>5.225957218961489E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0565768877676487E-2</c:v>
+                  <c:v>5.860265758786775E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.4756657361210842E-2</c:v>
+                  <c:v>6.2672341898661429E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.1587705894632315E-2</c:v>
+                  <c:v>6.9305830513774952E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.264151967794517E-2</c:v>
+                  <c:v>8.0039958301982059E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.0319822944581098E-2</c:v>
+                  <c:v>9.7206989524203091E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.806879419650627E-2</c:v>
+                  <c:v>0.12415343617586547</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.14037179853299253</c:v>
+                  <c:v>0.16523300050310455</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.20207492269482669</c:v>
+                  <c:v>0.22515161616538465</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.28651151686663684</c:v>
+                  <c:v>0.30714622993474716</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.39250071469828041</c:v>
+                  <c:v>0.41007012715218821</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.51201688620463759</c:v>
+                  <c:v>0.52612978609480743</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.63153305771099466</c:v>
+                  <c:v>0.6421894450374267</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.73752225554263828</c:v>
+                  <c:v>0.74511334225486781</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.82195884971444833</c:v>
+                  <c:v>0.82710795602423015</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.88366197387628254</c:v>
+                  <c:v>0.88702657168651022</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.92596497821276891</c:v>
+                  <c:v>0.92810613601374947</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.95371394946469412</c:v>
+                  <c:v>0.95505258266541193</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.9713922527313299</c:v>
+                  <c:v>0.97221961388763278</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.98244606651464272</c:v>
+                  <c:v>0.98295374167583993</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.98927711504806426</c:v>
+                  <c:v>0.98958723029095352</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.9934680035315987</c:v>
+                  <c:v>0.99365691460174721</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.99602768304764211</c:v>
+                  <c:v>0.99614256593988948</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.99758680330556582</c:v>
+                  <c:v>0.99765659507171722</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.9985348968159663</c:v>
+                  <c:v>0.99857726888577869</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.99911084480265877</c:v>
+                  <c:v>0.9991365599512616</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.99946050671902897</c:v>
+                  <c:v>0.99947610933815767</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.99967270959824672</c:v>
+                  <c:v>0.99968217512388557</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.99980146213963728</c:v>
+                  <c:v>0.99980720402878975</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.99987957106116954</c:v>
+                  <c:v>0.99988305397176525</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.99992695260968711</c:v>
+                  <c:v>0.99992906520431912</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3377,6 +3501,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3424,6 +3549,7 @@
         <c:axId val="343203464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4079,67 +4205,18 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>142874</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>138114</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>266699</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>61163</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0F00-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6015037" y="1766889"/>
-          <a:ext cx="5343525" cy="3361574"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>555624</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>111918</xdr:rowOff>
+      <xdr:colOff>225424</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>29368</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>226220</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>537370</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>92075</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4490,7 +4567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B127"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -51783,8 +51860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -51910,11 +51987,6 @@
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="15" t="s">
         <v>926</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" s="15" t="s">
-        <v>927</v>
       </c>
     </row>
     <row r="35" spans="5:17" x14ac:dyDescent="0.35">
@@ -51974,7 +52046,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -51985,8 +52056,8 @@
   </sheetPr>
   <dimension ref="A1:AL93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G4" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -52272,8 +52343,8 @@
         <v>1</v>
       </c>
       <c r="D10" s="29">
-        <f>INDEX('AEO 38'!68:68,0,MATCH(2030,'AEO 38'!1:1,0))/INDEX('AEO 38'!73:73,MATCH(2021,'AEO 38'!1:1,0))</f>
-        <v>2.4033772409275102E-2</v>
+        <f>INDEX('AEO 38'!68:68,0,MATCH(2037,'AEO 38'!1:1,0))/INDEX('AEO 38'!73:73,MATCH(2021,'AEO 38'!1:1,0))</f>
+        <v>5.225957218961489E-2</v>
       </c>
       <c r="E10" s="15">
         <v>1</v>
@@ -52284,127 +52355,127 @@
       </c>
       <c r="H10" s="29">
         <f t="shared" ref="H10" si="1">D10</f>
-        <v>2.4033772409275102E-2</v>
+        <v>5.225957218961489E-2</v>
       </c>
       <c r="I10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:I$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,I$9))</f>
-        <v>3.0565768877676487E-2</v>
+        <v>5.860265758786775E-2</v>
       </c>
       <c r="J10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:J$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,J$9))</f>
-        <v>3.4756657361210842E-2</v>
+        <v>6.2672341898661429E-2</v>
       </c>
       <c r="K10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:K$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,K$9))</f>
-        <v>4.1587705894632315E-2</v>
+        <v>6.9305830513774952E-2</v>
       </c>
       <c r="L10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:L$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,L$9))</f>
-        <v>5.264151967794517E-2</v>
+        <v>8.0039958301982059E-2</v>
       </c>
       <c r="M10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:M$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,M$9))</f>
-        <v>7.0319822944581098E-2</v>
+        <v>9.7206989524203091E-2</v>
       </c>
       <c r="N10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:N$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,N$9))</f>
-        <v>9.806879419650627E-2</v>
+        <v>0.12415343617586547</v>
       </c>
       <c r="O10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:O$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,O$9))</f>
-        <v>0.14037179853299253</v>
+        <v>0.16523300050310455</v>
       </c>
       <c r="P10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:P$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,P$9))</f>
-        <v>0.20207492269482669</v>
+        <v>0.22515161616538465</v>
       </c>
       <c r="Q10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:Q$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,Q$9))</f>
-        <v>0.28651151686663684</v>
+        <v>0.30714622993474716</v>
       </c>
       <c r="R10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:R$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,R$9))</f>
-        <v>0.39250071469828041</v>
+        <v>0.41007012715218821</v>
       </c>
       <c r="S10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:S$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,S$9))</f>
-        <v>0.51201688620463759</v>
+        <v>0.52612978609480743</v>
       </c>
       <c r="T10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:T$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,T$9))</f>
-        <v>0.63153305771099466</v>
+        <v>0.6421894450374267</v>
       </c>
       <c r="U10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:U$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,U$9))</f>
-        <v>0.73752225554263828</v>
+        <v>0.74511334225486781</v>
       </c>
       <c r="V10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:V$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,V$9))</f>
-        <v>0.82195884971444833</v>
+        <v>0.82710795602423015</v>
       </c>
       <c r="W10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:W$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,W$9))</f>
-        <v>0.88366197387628254</v>
+        <v>0.88702657168651022</v>
       </c>
       <c r="X10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:X$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,X$9))</f>
-        <v>0.92596497821276891</v>
+        <v>0.92810613601374947</v>
       </c>
       <c r="Y10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:Y$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,Y$9))</f>
-        <v>0.95371394946469412</v>
+        <v>0.95505258266541193</v>
       </c>
       <c r="Z10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:Z$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,Z$9))</f>
-        <v>0.9713922527313299</v>
+        <v>0.97221961388763278</v>
       </c>
       <c r="AA10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:AA$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,AA$9))</f>
-        <v>0.98244606651464272</v>
+        <v>0.98295374167583993</v>
       </c>
       <c r="AB10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:AB$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,AB$9))</f>
-        <v>0.98927711504806426</v>
+        <v>0.98958723029095352</v>
       </c>
       <c r="AC10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:AC$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,AC$9))</f>
-        <v>0.9934680035315987</v>
+        <v>0.99365691460174721</v>
       </c>
       <c r="AD10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:AD$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,AD$9))</f>
-        <v>0.99602768304764211</v>
+        <v>0.99614256593988948</v>
       </c>
       <c r="AE10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:AE$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,AE$9))</f>
-        <v>0.99758680330556582</v>
+        <v>0.99765659507171722</v>
       </c>
       <c r="AF10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:AF$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,AF$9))</f>
-        <v>0.9985348968159663</v>
+        <v>0.99857726888577869</v>
       </c>
       <c r="AG10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:AG$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,AG$9))</f>
-        <v>0.99911084480265877</v>
+        <v>0.9991365599512616</v>
       </c>
       <c r="AH10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:AH$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,AH$9))</f>
-        <v>0.99946050671902897</v>
+        <v>0.99947610933815767</v>
       </c>
       <c r="AI10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:AI$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,AI$9))</f>
-        <v>0.99967270959824672</v>
+        <v>0.99968217512388557</v>
       </c>
       <c r="AJ10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:AJ$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,AJ$9))</f>
-        <v>0.99980146213963728</v>
+        <v>0.99980720402878975</v>
       </c>
       <c r="AK10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:AK$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,AK$9))</f>
-        <v>0.99987957106116954</v>
+        <v>0.99988305397176525</v>
       </c>
       <c r="AL10" s="15">
         <f>IF($F10="s-curve",$D10+($E10-$D10)*$O$2/(1+EXP($O$3*(COUNT($H$9:AL$9)+$O$4))),TREND($D10:$E10,$D$9:$E$9,AL$9))</f>
-        <v>0.99992695260968711</v>
+        <v>0.99992906520431912</v>
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.35">
@@ -64251,127 +64322,127 @@
       </c>
       <c r="B2">
         <f>Data!H10</f>
-        <v>2.4033772409275102E-2</v>
+        <v>5.225957218961489E-2</v>
       </c>
       <c r="C2">
         <f>Data!I10</f>
-        <v>3.0565768877676487E-2</v>
+        <v>5.860265758786775E-2</v>
       </c>
       <c r="D2">
         <f>Data!J10</f>
-        <v>3.4756657361210842E-2</v>
+        <v>6.2672341898661429E-2</v>
       </c>
       <c r="E2">
         <f>Data!K10</f>
-        <v>4.1587705894632315E-2</v>
+        <v>6.9305830513774952E-2</v>
       </c>
       <c r="F2">
         <f>Data!L10</f>
-        <v>5.264151967794517E-2</v>
+        <v>8.0039958301982059E-2</v>
       </c>
       <c r="G2">
         <f>Data!M10</f>
-        <v>7.0319822944581098E-2</v>
+        <v>9.7206989524203091E-2</v>
       </c>
       <c r="H2">
         <f>Data!N10</f>
-        <v>9.806879419650627E-2</v>
+        <v>0.12415343617586547</v>
       </c>
       <c r="I2">
         <f>Data!O10</f>
-        <v>0.14037179853299253</v>
+        <v>0.16523300050310455</v>
       </c>
       <c r="J2">
         <f>Data!P10</f>
-        <v>0.20207492269482669</v>
+        <v>0.22515161616538465</v>
       </c>
       <c r="K2">
         <f>Data!Q10</f>
-        <v>0.28651151686663684</v>
+        <v>0.30714622993474716</v>
       </c>
       <c r="L2">
         <f>Data!R10</f>
-        <v>0.39250071469828041</v>
+        <v>0.41007012715218821</v>
       </c>
       <c r="M2">
         <f>Data!S10</f>
-        <v>0.51201688620463759</v>
+        <v>0.52612978609480743</v>
       </c>
       <c r="N2">
         <f>Data!T10</f>
-        <v>0.63153305771099466</v>
+        <v>0.6421894450374267</v>
       </c>
       <c r="O2">
         <f>Data!U10</f>
-        <v>0.73752225554263828</v>
+        <v>0.74511334225486781</v>
       </c>
       <c r="P2">
         <f>Data!V10</f>
-        <v>0.82195884971444833</v>
+        <v>0.82710795602423015</v>
       </c>
       <c r="Q2">
         <f>Data!W10</f>
-        <v>0.88366197387628254</v>
+        <v>0.88702657168651022</v>
       </c>
       <c r="R2">
         <f>Data!X10</f>
-        <v>0.92596497821276891</v>
+        <v>0.92810613601374947</v>
       </c>
       <c r="S2">
         <f>Data!Y10</f>
-        <v>0.95371394946469412</v>
+        <v>0.95505258266541193</v>
       </c>
       <c r="T2">
         <f>Data!Z10</f>
-        <v>0.9713922527313299</v>
+        <v>0.97221961388763278</v>
       </c>
       <c r="U2">
         <f>Data!AA10</f>
-        <v>0.98244606651464272</v>
+        <v>0.98295374167583993</v>
       </c>
       <c r="V2">
         <f>Data!AB10</f>
-        <v>0.98927711504806426</v>
+        <v>0.98958723029095352</v>
       </c>
       <c r="W2">
         <f>Data!AC10</f>
-        <v>0.9934680035315987</v>
+        <v>0.99365691460174721</v>
       </c>
       <c r="X2">
         <f>Data!AD10</f>
-        <v>0.99602768304764211</v>
+        <v>0.99614256593988948</v>
       </c>
       <c r="Y2">
         <f>Data!AE10</f>
-        <v>0.99758680330556582</v>
+        <v>0.99765659507171722</v>
       </c>
       <c r="Z2">
         <f>Data!AF10</f>
-        <v>0.9985348968159663</v>
+        <v>0.99857726888577869</v>
       </c>
       <c r="AA2">
         <f>Data!AG10</f>
-        <v>0.99911084480265877</v>
+        <v>0.9991365599512616</v>
       </c>
       <c r="AB2">
         <f>Data!AH10</f>
-        <v>0.99946050671902897</v>
+        <v>0.99947610933815767</v>
       </c>
       <c r="AC2">
         <f>Data!AI10</f>
-        <v>0.99967270959824672</v>
+        <v>0.99968217512388557</v>
       </c>
       <c r="AD2">
         <f>Data!AJ10</f>
-        <v>0.99980146213963728</v>
+        <v>0.99980720402878975</v>
       </c>
       <c r="AE2">
         <f>Data!AK10</f>
-        <v>0.99987957106116954</v>
+        <v>0.99988305397176525</v>
       </c>
       <c r="AF2">
         <f>Data!AL10</f>
-        <v>0.99992695260968711</v>
+        <v>0.99992906520431912</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Increase TTS shareweight for passenger LDV PHEVs
</commit_message>
<xml_diff>
--- a/InputData/trans/TTS/Transportation Technology Shareweights.xlsx
+++ b/InputData/trans/TTS/Transportation Technology Shareweights.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\TTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D3DD02-EBCA-496B-826B-94DED77DECDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123259A3-E51E-4CD2-BDCD-D3B53C79C9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
     <sheet name="TTS-motorbikes-psgr" sheetId="17" r:id="rId20"/>
     <sheet name="TTS-motorbikes-frgt" sheetId="18" r:id="rId21"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1781" uniqueCount="971">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1797" uniqueCount="987">
   <si>
     <t>Source:</t>
   </si>
@@ -2964,6 +2964,54 @@
   </si>
   <si>
     <t>https://www.energy.gov/energysaver/articles/new-plug-electric-vehicle-sales-united-states-nearly-doubled-2020-2021</t>
+  </si>
+  <si>
+    <t>pixels for all PEVs, 2030</t>
+  </si>
+  <si>
+    <t>pixels for BEVs, 2030</t>
+  </si>
+  <si>
+    <t>Percentage of PEVs as BEVs</t>
+  </si>
+  <si>
+    <t>Deloitte US 2030 PEV value</t>
+  </si>
+  <si>
+    <t>Assumed BEV sales share</t>
+  </si>
+  <si>
+    <t>Assumed PHEV sales share</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* We calibrate to a projection from Deloitte, which estimates 27% </t>
+  </si>
+  <si>
+    <t>of US LDV sales will be electric in 2030. From the global breakdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">above, they expect about 81% of PEV sales will be BEVs, with the </t>
+  </si>
+  <si>
+    <t>rest as PHEVs. We calibrate to similar numbers in the US by adjusting</t>
+  </si>
+  <si>
+    <t>the 2030 max potential sales share in the Data tab.</t>
+  </si>
+  <si>
+    <t>Deloitte</t>
+  </si>
+  <si>
+    <t>Electric vehicles: Setting a course for 2030</t>
+  </si>
+  <si>
+    <t>https://www2.deloitte.com/us/en/insights/focus/future-of-mobility/electric-vehicle-trends-2030.html</t>
+  </si>
+  <si>
+    <t>We use a hard coded value for PHEVs in 2020 in order to match</t>
+  </si>
+  <si>
+    <t>historical data.</t>
   </si>
 </sst>
 </file>
@@ -3768,7 +3816,7 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3857,6 +3905,10 @@
     <xf numFmtId="3" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="88">
     <cellStyle name="20% - Accent1" xfId="28" builtinId="30" customBuiltin="1"/>
@@ -6100,13 +6152,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>85</xdr:row>
+      <xdr:row>100</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>111</xdr:row>
       <xdr:rowOff>47034</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6144,13 +6196,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>91</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>335702</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:colOff>69002</xdr:colOff>
+      <xdr:row>99</xdr:row>
       <xdr:rowOff>152208</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6228,6 +6280,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>216356</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{027899A3-F83F-F8A7-BCD4-73014DA6F3D1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="14344650"/>
+          <a:ext cx="3943350" cy="2242006"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6271,16 +6367,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>136525</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>612775</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>92075</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>53975</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6647,10 +6743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B125"/>
+  <dimension ref="A1:B130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6743,429 +6839,452 @@
         <v>970</v>
       </c>
     </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B20" s="47"/>
+    </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="3" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B22" s="3">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B23" s="3" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B24" s="47" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B26" s="16" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B22" s="15" t="s">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B27" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B23" s="3">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B28" s="3">
         <v>2020</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B24" s="15" t="s">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B29" s="15" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B25" s="15" t="s">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B30" s="15" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B26" s="15" t="s">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B31" s="15" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B28" s="16" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B33" s="16" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B29" s="17" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B34" s="17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B31" s="16" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B36" s="16" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B32" s="18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B33" s="7">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B34" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B35" s="18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B36" s="18"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B37" s="18" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B38" s="7">
-        <v>2015</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B39" s="18" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B40" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B41" s="18"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B42" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B43" s="7">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B44" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B45" s="18" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" s="14" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" s="14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" s="35" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" s="35" t="s">
         <v>907</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" s="35" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" s="35" t="s">
         <v>908</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" s="35" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" s="35" t="s">
         <v>909</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" s="47" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" s="47" t="s">
         <v>910</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" s="14"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" s="15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51" s="15" t="s">
-        <v>107</v>
-      </c>
-    </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" s="15" t="s">
-        <v>35</v>
-      </c>
+      <c r="A52" s="14"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="15" t="s">
-        <v>906</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" s="15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" s="15" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" s="16" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B56" s="19"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B58" s="16" t="s">
+      <c r="B61" s="19"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B63" s="16" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B59" s="20"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B60" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B61" s="15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B62" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B64" s="15" t="s">
-        <v>31</v>
-      </c>
+      <c r="B64" s="20"/>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B65" s="15" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B66" s="15" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B67" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B68" s="15" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B69" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B71" s="16" t="s">
-        <v>44</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B70" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B72" s="15" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B73" s="15" t="s">
-        <v>134</v>
+        <v>26</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B74" s="15" t="s">
-        <v>912</v>
-      </c>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B75" s="15" t="s">
-        <v>135</v>
+        <v>27</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B76" s="15" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B77" s="15" t="s">
-        <v>914</v>
+      <c r="B76" s="16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B78" s="15" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B79" s="15" t="s">
-        <v>139</v>
+        <v>912</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B80" s="15" t="s">
-        <v>42</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B81" s="15" t="s">
+        <v>913</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B82" s="15" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B83" s="15" t="s">
-        <v>45</v>
+        <v>914</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B84" s="15" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B85" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B86" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B87" s="15" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B88" s="15" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B88" s="16" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B90" s="15" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B91" s="15" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B92" s="15" t="s">
-        <v>141</v>
+        <v>45</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B93" s="15" t="s">
-        <v>142</v>
+      <c r="B93" s="16" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B95" s="15" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B96" s="15" t="s">
-        <v>75</v>
+        <v>140</v>
       </c>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B97" s="15" t="s">
-        <v>85</v>
+        <v>141</v>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B98" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B99" s="15" t="s">
-        <v>86</v>
+        <v>142</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B100" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B101" s="15" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B102" s="15" t="s">
-        <v>84</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B103" s="15" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B104" s="15" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B105" s="15" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B106" s="15" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B107" s="15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B108" s="15" t="s">
-        <v>111</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B109" s="15" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B110" s="15" t="s">
-        <v>68</v>
+        <v>112</v>
       </c>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B111" s="15" t="s">
-        <v>69</v>
+        <v>109</v>
       </c>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B112" s="15" t="s">
-        <v>70</v>
+        <v>110</v>
       </c>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B113" s="15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B114" s="15" t="s">
-        <v>72</v>
+        <v>111</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B115" s="15" t="s">
-        <v>73</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B116" s="15" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B117" s="15" t="s">
-        <v>123</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B118" s="15" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B119" s="15" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B120" s="15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B121" s="15" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B122" s="15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B123" s="15" t="s">
-        <v>53</v>
+        <v>123</v>
       </c>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B124" s="15" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B125" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="126" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B126" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="127" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B127" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="128" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B128" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B129" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="130" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B130" s="15" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A46" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A51" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -7840,127 +7959,127 @@
       </c>
       <c r="B6" s="15">
         <f>Data!H14</f>
-        <v>1.7500000000000002E-2</v>
+        <v>1.7641947805604345E-2</v>
       </c>
       <c r="C6" s="15">
         <f>Data!I14</f>
-        <v>2.0146623971724009E-2</v>
+        <v>5.1345518914747604E-2</v>
       </c>
       <c r="D6" s="15">
         <f>Data!J14</f>
-        <v>2.1054197652496692E-2</v>
+        <v>7.8869239433912761E-2</v>
       </c>
       <c r="E6" s="15">
         <f>Data!K14</f>
-        <v>2.2264592511898683E-2</v>
+        <v>0.12043936074535663</v>
       </c>
       <c r="F6" s="15">
         <f>Data!L14</f>
-        <v>2.3872232318586158E-2</v>
+        <v>0.17261688857579932</v>
       </c>
       <c r="G6" s="15">
         <f>Data!M14</f>
-        <v>2.5995883550110573E-2</v>
+        <v>0.22479441640624204</v>
       </c>
       <c r="H6" s="15">
         <f>Data!N14</f>
-        <v>2.8781063773285744E-2</v>
+        <v>0.26636453771768587</v>
       </c>
       <c r="I6" s="15">
         <f>Data!O14</f>
-        <v>3.2399578998058384E-2</v>
+        <v>0.29388825823685111</v>
       </c>
       <c r="J6" s="15">
         <f>Data!P14</f>
-        <v>3.7043633600479256E-2</v>
+        <v>0.30994988154038999</v>
       </c>
       <c r="K6" s="15">
         <f>Data!Q14</f>
-        <v>4.2911237539929523E-2</v>
+        <v>0.31864013308886613</v>
       </c>
       <c r="L6" s="15">
         <f>Data!R14</f>
-        <v>5.0179756912938397E-2</v>
+        <v>0.32315037349563713</v>
       </c>
       <c r="M6" s="15">
         <f>Data!S14</f>
-        <v>5.8966531923743418E-2</v>
+        <v>0.32544067136138988</v>
       </c>
       <c r="N6" s="15">
         <f>Data!T14</f>
-        <v>6.9280583071290994E-2</v>
+        <v>0.32659080149166408</v>
       </c>
       <c r="O6" s="15">
         <f>Data!U14</f>
-        <v>8.0977223661233097E-2</v>
+        <v>0.3271651375801809</v>
       </c>
       <c r="P6" s="15">
         <f>Data!V14</f>
-        <v>9.3734480860469802E-2</v>
+        <v>0.32745113829838129</v>
       </c>
       <c r="Q6" s="15">
         <f>Data!W14</f>
-        <v>0.1070701331454796</v>
+        <v>0.32759335844966003</v>
       </c>
       <c r="R6" s="15">
         <f>Data!X14</f>
-        <v>0.1204057854304894</v>
+        <v>0.32766403139580214</v>
       </c>
       <c r="S6" s="15">
         <f>Data!Y14</f>
-        <v>0.13316304262972609</v>
+        <v>0.32769913851400356</v>
       </c>
       <c r="T6" s="15">
         <f>Data!Z14</f>
-        <v>0.14485968321966819</v>
+        <v>0.32771657514633645</v>
       </c>
       <c r="U6" s="15">
         <f>Data!AA14</f>
-        <v>0.15517373436721577</v>
+        <v>0.3277252346501377</v>
       </c>
       <c r="V6" s="15">
         <f>Data!AB14</f>
-        <v>0.16396050937802081</v>
+        <v>0.32772953501211155</v>
       </c>
       <c r="W6" s="15">
         <f>Data!AC14</f>
-        <v>0.17122902875102969</v>
+        <v>0.32773167055297159</v>
       </c>
       <c r="X6" s="15">
         <f>Data!AD14</f>
-        <v>0.17709663269047993</v>
+        <v>0.32773273104210349</v>
       </c>
       <c r="Y6" s="15">
         <f>Data!AE14</f>
-        <v>0.18174068729290083</v>
+        <v>0.3277332576681154</v>
       </c>
       <c r="Z6" s="15">
         <f>Data!AF14</f>
-        <v>0.18535920251767346</v>
+        <v>0.32773351918351784</v>
       </c>
       <c r="AA6" s="15">
         <f>Data!AG14</f>
-        <v>0.18814438274084866</v>
+        <v>0.32773364904838725</v>
       </c>
       <c r="AB6" s="15">
         <f>Data!AH14</f>
-        <v>0.19026803397237302</v>
+        <v>0.32773371353741332</v>
       </c>
       <c r="AC6" s="15">
         <f>Data!AI14</f>
-        <v>0.19187567377906051</v>
+        <v>0.32773374556172585</v>
       </c>
       <c r="AD6" s="15">
         <f>Data!AJ14</f>
-        <v>0.1930860686384625</v>
+        <v>0.32773376146453126</v>
       </c>
       <c r="AE6" s="15">
         <f>Data!AK14</f>
-        <v>0.19399364231923522</v>
+        <v>0.32773376936163134</v>
       </c>
       <c r="AF6" s="15">
         <f>Data!AL14</f>
-        <v>0.19467206246239127</v>
+        <v>0.32773377328321535</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.35">
@@ -8898,123 +9017,123 @@
       </c>
       <c r="C6" s="15">
         <f>Data!I21</f>
-        <v>2.9051695263562845E-3</v>
+        <v>4.8419492105938079E-3</v>
       </c>
       <c r="D6" s="15">
         <f>Data!J21</f>
-        <v>3.9014030028430464E-3</v>
+        <v>6.5023383380717441E-3</v>
       </c>
       <c r="E6" s="15">
         <f>Data!K21</f>
-        <v>5.230039899493835E-3</v>
+        <v>8.7167331658230592E-3</v>
       </c>
       <c r="F6" s="15">
         <f>Data!L21</f>
-        <v>6.9947281308572898E-3</v>
+        <v>1.1657880218095483E-2</v>
       </c>
       <c r="G6" s="15">
         <f>Data!M21</f>
-        <v>9.3258363307179917E-3</v>
+        <v>1.5543060551196652E-2</v>
       </c>
       <c r="H6" s="15">
         <f>Data!N21</f>
-        <v>1.2383097504283182E-2</v>
+        <v>2.063849584047197E-2</v>
       </c>
       <c r="I6" s="15">
         <f>Data!O21</f>
-        <v>1.6355101186702026E-2</v>
+        <v>2.7258501977836708E-2</v>
       </c>
       <c r="J6" s="15">
         <f>Data!P21</f>
-        <v>2.1452827971402487E-2</v>
+        <v>3.5754713285670814E-2</v>
       </c>
       <c r="K6" s="15">
         <f>Data!Q21</f>
-        <v>2.789363117568806E-2</v>
+        <v>4.6489385292813434E-2</v>
       </c>
       <c r="L6" s="15">
         <f>Data!R21</f>
-        <v>3.5872203579549629E-2</v>
+        <v>5.9787005965916053E-2</v>
       </c>
       <c r="M6" s="15">
         <f>Data!S21</f>
-        <v>4.5517348212510605E-2</v>
+        <v>7.5862247020851009E-2</v>
       </c>
       <c r="N6" s="15">
         <f>Data!T21</f>
-        <v>5.6838966775353432E-2</v>
+        <v>9.4731611292255713E-2</v>
       </c>
       <c r="O6" s="15">
         <f>Data!U21</f>
-        <v>6.9678238302281689E-2</v>
+        <v>0.11613039717046947</v>
       </c>
       <c r="P6" s="15">
         <f>Data!V21</f>
-        <v>8.368173681626577E-2</v>
+        <v>0.13946956136044295</v>
       </c>
       <c r="Q6" s="15">
         <f>Data!W21</f>
-        <v>9.8320133145479605E-2</v>
+        <v>0.16386688857579934</v>
       </c>
       <c r="R6" s="15">
         <f>Data!X21</f>
-        <v>0.11295852947469344</v>
+        <v>0.18826421579115574</v>
       </c>
       <c r="S6" s="15">
         <f>Data!Y21</f>
-        <v>0.12696202798867751</v>
+        <v>0.21160337998112919</v>
       </c>
       <c r="T6" s="15">
         <f>Data!Z21</f>
-        <v>0.13980129951560577</v>
+        <v>0.23300216585934294</v>
       </c>
       <c r="U6" s="15">
         <f>Data!AA21</f>
-        <v>0.1511229180784486</v>
+        <v>0.25187153013074765</v>
       </c>
       <c r="V6" s="15">
         <f>Data!AB21</f>
-        <v>0.16076806271140956</v>
+        <v>0.26794677118568261</v>
       </c>
       <c r="W6" s="15">
         <f>Data!AC21</f>
-        <v>0.16874663511527116</v>
+        <v>0.2812443918587853</v>
       </c>
       <c r="X6" s="15">
         <f>Data!AD21</f>
-        <v>0.17518743831955672</v>
+        <v>0.29197906386592787</v>
       </c>
       <c r="Y6" s="15">
         <f>Data!AE21</f>
-        <v>0.18028516510425718</v>
+        <v>0.30047527517376199</v>
       </c>
       <c r="Z6" s="15">
         <f>Data!AF21</f>
-        <v>0.18425716878667603</v>
+        <v>0.30709528131112673</v>
       </c>
       <c r="AA6" s="15">
         <f>Data!AG21</f>
-        <v>0.18731442996024122</v>
+        <v>0.31219071660040204</v>
       </c>
       <c r="AB6" s="15">
         <f>Data!AH21</f>
-        <v>0.18964553816010193</v>
+        <v>0.31607589693350319</v>
       </c>
       <c r="AC6" s="15">
         <f>Data!AI21</f>
-        <v>0.19141022639146535</v>
+        <v>0.31901704398577563</v>
       </c>
       <c r="AD6" s="15">
         <f>Data!AJ21</f>
-        <v>0.19273886328811618</v>
+        <v>0.32123143881352695</v>
       </c>
       <c r="AE6" s="15">
         <f>Data!AK21</f>
-        <v>0.19373509676460293</v>
+        <v>0.32289182794100485</v>
       </c>
       <c r="AF6" s="15">
         <f>Data!AL21</f>
-        <v>0.19447979096635587</v>
+        <v>0.32413298494392645</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.35">
@@ -56144,16 +56263,17 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AF103"/>
+  <dimension ref="A1:AF118"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75:XFD76"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61:AF68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28.453125" style="15" customWidth="1"/>
-    <col min="2" max="6" width="9.1796875" style="15"/>
+    <col min="2" max="5" width="9.1796875" style="15"/>
+    <col min="6" max="6" width="13" style="15" customWidth="1"/>
     <col min="7" max="7" width="14.26953125" style="15" customWidth="1"/>
     <col min="8" max="16384" width="9.1796875" style="15"/>
   </cols>
@@ -56796,97 +56916,97 @@
         <v>953</v>
       </c>
       <c r="B62" s="15">
-        <v>328761</v>
+        <v>349182</v>
       </c>
       <c r="C62" s="15">
-        <v>537999</v>
-      </c>
-      <c r="D62" s="15">
-        <v>923271</v>
+        <v>603744</v>
+      </c>
+      <c r="D62" s="58">
+        <v>1098920</v>
       </c>
       <c r="E62" s="58">
-        <v>1396960</v>
+        <v>1600640</v>
       </c>
       <c r="F62" s="58">
-        <v>1986480</v>
+        <v>2209510</v>
       </c>
       <c r="G62" s="58">
-        <v>2681780</v>
+        <v>2809740</v>
       </c>
       <c r="H62" s="58">
-        <v>3356340</v>
+        <v>3313430</v>
       </c>
       <c r="I62" s="58">
-        <v>3975250</v>
+        <v>3838830</v>
       </c>
       <c r="J62" s="58">
-        <v>4520760</v>
+        <v>4387740</v>
       </c>
       <c r="K62" s="58">
-        <v>5024490</v>
+        <v>4901270</v>
       </c>
       <c r="L62" s="58">
-        <v>5560350</v>
+        <v>5460140</v>
       </c>
       <c r="M62" s="58">
-        <v>6002870</v>
+        <v>5896040</v>
       </c>
       <c r="N62" s="58">
-        <v>6380960</v>
+        <v>6271520</v>
       </c>
       <c r="O62" s="58">
-        <v>6747030</v>
+        <v>6625100</v>
       </c>
       <c r="P62" s="58">
-        <v>7064830</v>
+        <v>6942390</v>
       </c>
       <c r="Q62" s="58">
-        <v>7362140</v>
+        <v>7274900</v>
       </c>
       <c r="R62" s="58">
-        <v>7662150</v>
+        <v>7567320</v>
       </c>
       <c r="S62" s="58">
-        <v>7954220</v>
+        <v>7866920</v>
       </c>
       <c r="T62" s="58">
-        <v>8263950</v>
+        <v>8176700</v>
       </c>
       <c r="U62" s="58">
-        <v>8541650</v>
+        <v>8461000</v>
       </c>
       <c r="V62" s="58">
-        <v>8834150</v>
+        <v>8757100</v>
       </c>
       <c r="W62" s="58">
-        <v>9135740</v>
+        <v>9060000</v>
       </c>
       <c r="X62" s="58">
-        <v>9421100</v>
+        <v>9346980</v>
       </c>
       <c r="Y62" s="58">
-        <v>9727780</v>
+        <v>9657430</v>
       </c>
       <c r="Z62" s="58">
-        <v>10043400</v>
+        <v>9970180</v>
       </c>
       <c r="AA62" s="58">
-        <v>10341400</v>
+        <v>10265600</v>
       </c>
       <c r="AB62" s="58">
-        <v>10658000</v>
+        <v>10577800</v>
       </c>
       <c r="AC62" s="58">
-        <v>10996100</v>
+        <v>10885700</v>
       </c>
       <c r="AD62" s="58">
-        <v>11299000</v>
+        <v>11185100</v>
       </c>
       <c r="AE62" s="58">
-        <v>11614300</v>
+        <v>11495700</v>
       </c>
       <c r="AF62" s="58">
-        <v>11941900</v>
+        <v>11818600</v>
       </c>
     </row>
     <row r="63" spans="1:32" x14ac:dyDescent="0.35">
@@ -56894,97 +57014,97 @@
         <v>954</v>
       </c>
       <c r="B63" s="15">
-        <v>1848</v>
+        <v>1905</v>
       </c>
       <c r="C63" s="15">
-        <v>2034</v>
+        <v>2100</v>
       </c>
       <c r="D63" s="15">
-        <v>1845</v>
+        <v>1965</v>
       </c>
       <c r="E63" s="15">
-        <v>1947</v>
+        <v>2016</v>
       </c>
       <c r="F63" s="15">
-        <v>2127</v>
+        <v>2154</v>
       </c>
       <c r="G63" s="15">
-        <v>2121</v>
+        <v>2082</v>
       </c>
       <c r="H63" s="15">
-        <v>2103</v>
+        <v>1983</v>
       </c>
       <c r="I63" s="15">
-        <v>2103</v>
+        <v>1974</v>
       </c>
       <c r="J63" s="15">
-        <v>2127</v>
+        <v>1989</v>
       </c>
       <c r="K63" s="15">
-        <v>2235</v>
+        <v>2085</v>
       </c>
       <c r="L63" s="15">
-        <v>2376</v>
+        <v>2214</v>
       </c>
       <c r="M63" s="15">
-        <v>2499</v>
+        <v>2334</v>
       </c>
       <c r="N63" s="15">
+        <v>2490</v>
+      </c>
+      <c r="O63" s="15">
         <v>2664</v>
       </c>
-      <c r="O63" s="15">
-        <v>2841</v>
-      </c>
       <c r="P63" s="15">
-        <v>3048</v>
+        <v>2859</v>
       </c>
       <c r="Q63" s="15">
-        <v>3261</v>
+        <v>3060</v>
       </c>
       <c r="R63" s="15">
-        <v>3459</v>
+        <v>3255</v>
       </c>
       <c r="S63" s="15">
-        <v>3639</v>
+        <v>3432</v>
       </c>
       <c r="T63" s="15">
-        <v>3810</v>
+        <v>3594</v>
       </c>
       <c r="U63" s="15">
-        <v>3942</v>
+        <v>3723</v>
       </c>
       <c r="V63" s="15">
-        <v>4047</v>
+        <v>3822</v>
       </c>
       <c r="W63" s="15">
-        <v>4125</v>
+        <v>3900</v>
       </c>
       <c r="X63" s="15">
-        <v>4176</v>
+        <v>3948</v>
       </c>
       <c r="Y63" s="15">
-        <v>4212</v>
+        <v>3984</v>
       </c>
       <c r="Z63" s="15">
-        <v>4227</v>
+        <v>3999</v>
       </c>
       <c r="AA63" s="15">
-        <v>4227</v>
+        <v>3996</v>
       </c>
       <c r="AB63" s="15">
-        <v>4218</v>
+        <v>3990</v>
       </c>
       <c r="AC63" s="15">
-        <v>4194</v>
+        <v>3966</v>
       </c>
       <c r="AD63" s="15">
-        <v>4164</v>
+        <v>3939</v>
       </c>
       <c r="AE63" s="15">
-        <v>4128</v>
+        <v>3903</v>
       </c>
       <c r="AF63" s="15">
-        <v>4092</v>
+        <v>3867</v>
       </c>
     </row>
     <row r="64" spans="1:32" x14ac:dyDescent="0.35">
@@ -56992,97 +57112,97 @@
         <v>955</v>
       </c>
       <c r="B64" s="58">
-        <v>19477000</v>
+        <v>19452500</v>
       </c>
       <c r="C64" s="58">
-        <v>20253400</v>
+        <v>20032800</v>
       </c>
       <c r="D64" s="58">
-        <v>20805100</v>
+        <v>20303000</v>
       </c>
       <c r="E64" s="58">
-        <v>21068800</v>
+        <v>20341500</v>
       </c>
       <c r="F64" s="58">
-        <v>20826400</v>
+        <v>19837400</v>
       </c>
       <c r="G64" s="58">
-        <v>20441500</v>
+        <v>19349100</v>
       </c>
       <c r="H64" s="58">
-        <v>20029300</v>
+        <v>18994500</v>
       </c>
       <c r="I64" s="58">
-        <v>19607900</v>
+        <v>18606300</v>
       </c>
       <c r="J64" s="58">
-        <v>19210800</v>
+        <v>18204900</v>
       </c>
       <c r="K64" s="58">
-        <v>18841200</v>
+        <v>17839100</v>
       </c>
       <c r="L64" s="58">
-        <v>18447900</v>
+        <v>17460000</v>
       </c>
       <c r="M64" s="58">
-        <v>18140100</v>
+        <v>17198600</v>
       </c>
       <c r="N64" s="58">
-        <v>17853400</v>
+        <v>16970700</v>
       </c>
       <c r="O64" s="58">
-        <v>17584800</v>
+        <v>16776200</v>
       </c>
       <c r="P64" s="58">
-        <v>17348000</v>
+        <v>16604800</v>
       </c>
       <c r="Q64" s="58">
-        <v>17116600</v>
+        <v>16403800</v>
       </c>
       <c r="R64" s="58">
-        <v>16883500</v>
+        <v>16240000</v>
       </c>
       <c r="S64" s="58">
-        <v>16671400</v>
+        <v>16078700</v>
       </c>
       <c r="T64" s="58">
-        <v>16445700</v>
+        <v>15905000</v>
       </c>
       <c r="U64" s="58">
-        <v>16277600</v>
+        <v>15776400</v>
       </c>
       <c r="V64" s="58">
-        <v>16105100</v>
+        <v>15638900</v>
       </c>
       <c r="W64" s="58">
-        <v>15923300</v>
+        <v>15487900</v>
       </c>
       <c r="X64" s="58">
-        <v>15770800</v>
+        <v>15360700</v>
       </c>
       <c r="Y64" s="58">
-        <v>15600400</v>
+        <v>15207500</v>
       </c>
       <c r="Z64" s="58">
-        <v>15424200</v>
+        <v>15051800</v>
       </c>
       <c r="AA64" s="58">
-        <v>15280700</v>
+        <v>14925500</v>
       </c>
       <c r="AB64" s="58">
-        <v>15139600</v>
+        <v>14800800</v>
       </c>
       <c r="AC64" s="58">
-        <v>14981900</v>
+        <v>14683100</v>
       </c>
       <c r="AD64" s="58">
-        <v>14863800</v>
+        <v>14577500</v>
       </c>
       <c r="AE64" s="58">
-        <v>14747000</v>
+        <v>14473200</v>
       </c>
       <c r="AF64" s="58">
-        <v>14637400</v>
+        <v>14375400</v>
       </c>
     </row>
     <row r="65" spans="1:32" x14ac:dyDescent="0.35">
@@ -57090,97 +57210,97 @@
         <v>956</v>
       </c>
       <c r="B65" s="15">
-        <v>21453</v>
+        <v>22110</v>
       </c>
       <c r="C65" s="15">
-        <v>27300</v>
+        <v>28173</v>
       </c>
       <c r="D65" s="15">
-        <v>30579</v>
+        <v>32691</v>
       </c>
       <c r="E65" s="15">
-        <v>36993</v>
+        <v>37941</v>
       </c>
       <c r="F65" s="15">
-        <v>40968</v>
+        <v>41217</v>
       </c>
       <c r="G65" s="15">
-        <v>44637</v>
+        <v>43569</v>
       </c>
       <c r="H65" s="15">
-        <v>48036</v>
+        <v>45132</v>
       </c>
       <c r="I65" s="15">
-        <v>51357</v>
+        <v>48126</v>
       </c>
       <c r="J65" s="15">
-        <v>54516</v>
+        <v>50952</v>
       </c>
       <c r="K65" s="15">
-        <v>57900</v>
+        <v>54015</v>
       </c>
       <c r="L65" s="15">
-        <v>61539</v>
+        <v>57375</v>
       </c>
       <c r="M65" s="15">
-        <v>64995</v>
+        <v>60678</v>
       </c>
       <c r="N65" s="15">
-        <v>68463</v>
+        <v>64011</v>
       </c>
       <c r="O65" s="15">
-        <v>71736</v>
+        <v>67245</v>
       </c>
       <c r="P65" s="15">
-        <v>75210</v>
+        <v>70590</v>
       </c>
       <c r="Q65" s="15">
-        <v>78315</v>
+        <v>73515</v>
       </c>
       <c r="R65" s="15">
-        <v>81387</v>
+        <v>76596</v>
       </c>
       <c r="S65" s="15">
-        <v>84360</v>
+        <v>79521</v>
       </c>
       <c r="T65" s="15">
-        <v>87636</v>
+        <v>82653</v>
       </c>
       <c r="U65" s="15">
-        <v>90561</v>
+        <v>85512</v>
       </c>
       <c r="V65" s="15">
-        <v>93648</v>
+        <v>88494</v>
       </c>
       <c r="W65" s="15">
-        <v>96702</v>
+        <v>91416</v>
       </c>
       <c r="X65" s="15">
-        <v>99771</v>
+        <v>94353</v>
       </c>
       <c r="Y65" s="15">
-        <v>102693</v>
+        <v>97170</v>
       </c>
       <c r="Z65" s="15">
-        <v>105336</v>
+        <v>99654</v>
       </c>
       <c r="AA65" s="15">
-        <v>108225</v>
+        <v>102369</v>
       </c>
       <c r="AB65" s="15">
-        <v>111222</v>
+        <v>105171</v>
       </c>
       <c r="AC65" s="15">
-        <v>113991</v>
+        <v>107820</v>
       </c>
       <c r="AD65" s="15">
-        <v>116880</v>
+        <v>110532</v>
       </c>
       <c r="AE65" s="15">
-        <v>119871</v>
+        <v>113328</v>
       </c>
       <c r="AF65" s="15">
-        <v>122847</v>
+        <v>116103</v>
       </c>
     </row>
     <row r="66" spans="1:32" x14ac:dyDescent="0.35">
@@ -57188,97 +57308,97 @@
         <v>957</v>
       </c>
       <c r="B66" s="15">
-        <v>83631</v>
+        <v>86889</v>
       </c>
       <c r="C66" s="15">
-        <v>94413</v>
+        <v>248313</v>
       </c>
       <c r="D66" s="15">
-        <v>109887</v>
+        <v>434007</v>
       </c>
       <c r="E66" s="15">
-        <v>114378</v>
+        <v>636849</v>
       </c>
       <c r="F66" s="15">
-        <v>121590</v>
-      </c>
-      <c r="G66" s="15">
-        <v>129444</v>
-      </c>
-      <c r="H66" s="15">
-        <v>140181</v>
-      </c>
-      <c r="I66" s="15">
-        <v>152049</v>
-      </c>
-      <c r="J66" s="15">
-        <v>167559</v>
-      </c>
-      <c r="K66" s="15">
-        <v>190572</v>
-      </c>
-      <c r="L66" s="15">
-        <v>218340</v>
-      </c>
-      <c r="M66" s="15">
-        <v>253572</v>
-      </c>
-      <c r="N66" s="15">
-        <v>292587</v>
-      </c>
-      <c r="O66" s="15">
-        <v>335565</v>
-      </c>
-      <c r="P66" s="15">
-        <v>382035</v>
-      </c>
-      <c r="Q66" s="15">
-        <v>430077</v>
-      </c>
-      <c r="R66" s="15">
-        <v>476250</v>
-      </c>
-      <c r="S66" s="15">
-        <v>519198</v>
-      </c>
-      <c r="T66" s="15">
-        <v>558639</v>
-      </c>
-      <c r="U66" s="15">
-        <v>590619</v>
-      </c>
-      <c r="V66" s="15">
-        <v>617439</v>
-      </c>
-      <c r="W66" s="15">
-        <v>638484</v>
-      </c>
-      <c r="X66" s="15">
-        <v>653250</v>
-      </c>
-      <c r="Y66" s="15">
-        <v>664245</v>
-      </c>
-      <c r="Z66" s="15">
-        <v>671571</v>
-      </c>
-      <c r="AA66" s="15">
-        <v>675162</v>
-      </c>
-      <c r="AB66" s="15">
-        <v>676623</v>
-      </c>
-      <c r="AC66" s="15">
-        <v>675378</v>
-      </c>
-      <c r="AD66" s="15">
-        <v>672426</v>
-      </c>
-      <c r="AE66" s="15">
-        <v>668622</v>
-      </c>
-      <c r="AF66" s="15">
-        <v>663933</v>
+        <v>887172</v>
+      </c>
+      <c r="G66" s="58">
+        <v>1095060</v>
+      </c>
+      <c r="H66" s="58">
+        <v>1221050</v>
+      </c>
+      <c r="I66" s="58">
+        <v>1293530</v>
+      </c>
+      <c r="J66" s="58">
+        <v>1310350</v>
+      </c>
+      <c r="K66" s="58">
+        <v>1320140</v>
+      </c>
+      <c r="L66" s="58">
+        <v>1310940</v>
+      </c>
+      <c r="M66" s="58">
+        <v>1306520</v>
+      </c>
+      <c r="N66" s="58">
+        <v>1289590</v>
+      </c>
+      <c r="O66" s="58">
+        <v>1270880</v>
+      </c>
+      <c r="P66" s="58">
+        <v>1252620</v>
+      </c>
+      <c r="Q66" s="58">
+        <v>1235240</v>
+      </c>
+      <c r="R66" s="58">
+        <v>1219780</v>
+      </c>
+      <c r="S66" s="58">
+        <v>1204400</v>
+      </c>
+      <c r="T66" s="58">
+        <v>1191940</v>
+      </c>
+      <c r="U66" s="58">
+        <v>1177850</v>
+      </c>
+      <c r="V66" s="58">
+        <v>1166230</v>
+      </c>
+      <c r="W66" s="58">
+        <v>1155260</v>
+      </c>
+      <c r="X66" s="58">
+        <v>1143250</v>
+      </c>
+      <c r="Y66" s="58">
+        <v>1133420</v>
+      </c>
+      <c r="Z66" s="58">
+        <v>1123340</v>
+      </c>
+      <c r="AA66" s="58">
+        <v>1112470</v>
+      </c>
+      <c r="AB66" s="58">
+        <v>1102060</v>
+      </c>
+      <c r="AC66" s="58">
+        <v>1091130</v>
+      </c>
+      <c r="AD66" s="58">
+        <v>1079340</v>
+      </c>
+      <c r="AE66" s="58">
+        <v>1067910</v>
+      </c>
+      <c r="AF66" s="58">
+        <v>1056400</v>
       </c>
     </row>
     <row r="67" spans="1:32" x14ac:dyDescent="0.35">
@@ -57286,97 +57406,97 @@
         <v>958</v>
       </c>
       <c r="B67" s="15">
+        <v>1728</v>
+      </c>
+      <c r="C67" s="15">
         <v>1677</v>
       </c>
-      <c r="C67" s="15">
-        <v>1626</v>
-      </c>
       <c r="D67" s="15">
-        <v>1953</v>
+        <v>2079</v>
       </c>
       <c r="E67" s="15">
-        <v>2073</v>
+        <v>2148</v>
       </c>
       <c r="F67" s="15">
+        <v>2136</v>
+      </c>
+      <c r="G67" s="15">
+        <v>2076</v>
+      </c>
+      <c r="H67" s="15">
+        <v>1974</v>
+      </c>
+      <c r="I67" s="15">
+        <v>1938</v>
+      </c>
+      <c r="J67" s="15">
+        <v>1908</v>
+      </c>
+      <c r="K67" s="15">
+        <v>1932</v>
+      </c>
+      <c r="L67" s="15">
+        <v>1962</v>
+      </c>
+      <c r="M67" s="15">
+        <v>2001</v>
+      </c>
+      <c r="N67" s="15">
+        <v>2037</v>
+      </c>
+      <c r="O67" s="15">
+        <v>2070</v>
+      </c>
+      <c r="P67" s="15">
         <v>2106</v>
       </c>
-      <c r="G67" s="15">
-        <v>2115</v>
-      </c>
-      <c r="H67" s="15">
-        <v>2094</v>
-      </c>
-      <c r="I67" s="15">
-        <v>2067</v>
-      </c>
-      <c r="J67" s="15">
-        <v>2040</v>
-      </c>
-      <c r="K67" s="15">
-        <v>2073</v>
-      </c>
-      <c r="L67" s="15">
-        <v>2103</v>
-      </c>
-      <c r="M67" s="15">
-        <v>2142</v>
-      </c>
-      <c r="N67" s="15">
-        <v>2178</v>
-      </c>
-      <c r="O67" s="15">
-        <v>2211</v>
-      </c>
-      <c r="P67" s="15">
-        <v>2244</v>
-      </c>
       <c r="Q67" s="15">
+        <v>2139</v>
+      </c>
+      <c r="R67" s="15">
+        <v>2169</v>
+      </c>
+      <c r="S67" s="15">
+        <v>2196</v>
+      </c>
+      <c r="T67" s="15">
+        <v>2223</v>
+      </c>
+      <c r="U67" s="15">
+        <v>2253</v>
+      </c>
+      <c r="V67" s="15">
         <v>2277</v>
       </c>
-      <c r="R67" s="15">
-        <v>2304</v>
-      </c>
-      <c r="S67" s="15">
-        <v>2328</v>
-      </c>
-      <c r="T67" s="15">
-        <v>2358</v>
-      </c>
-      <c r="U67" s="15">
-        <v>2385</v>
-      </c>
-      <c r="V67" s="15">
-        <v>2409</v>
-      </c>
       <c r="W67" s="15">
-        <v>2436</v>
+        <v>2301</v>
       </c>
       <c r="X67" s="15">
-        <v>2466</v>
+        <v>2331</v>
       </c>
       <c r="Y67" s="15">
-        <v>2490</v>
+        <v>2355</v>
       </c>
       <c r="Z67" s="15">
+        <v>2379</v>
+      </c>
+      <c r="AA67" s="15">
+        <v>2406</v>
+      </c>
+      <c r="AB67" s="15">
+        <v>2427</v>
+      </c>
+      <c r="AC67" s="15">
+        <v>2451</v>
+      </c>
+      <c r="AD67" s="15">
+        <v>2469</v>
+      </c>
+      <c r="AE67" s="15">
+        <v>2493</v>
+      </c>
+      <c r="AF67" s="15">
         <v>2514</v>
-      </c>
-      <c r="AA67" s="15">
-        <v>2544</v>
-      </c>
-      <c r="AB67" s="15">
-        <v>2568</v>
-      </c>
-      <c r="AC67" s="15">
-        <v>2592</v>
-      </c>
-      <c r="AD67" s="15">
-        <v>2613</v>
-      </c>
-      <c r="AE67" s="15">
-        <v>2637</v>
-      </c>
-      <c r="AF67" s="15">
-        <v>2658</v>
       </c>
     </row>
     <row r="68" spans="1:32" x14ac:dyDescent="0.35">
@@ -57393,7 +57513,7 @@
         <v>21</v>
       </c>
       <c r="E68" s="15">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F68" s="15">
         <v>30</v>
@@ -57402,79 +57522,79 @@
         <v>36</v>
       </c>
       <c r="H68" s="15">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I68" s="15">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J68" s="15">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="K68" s="15">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="L68" s="15">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="M68" s="15">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="N68" s="15">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="O68" s="15">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="P68" s="15">
-        <v>285</v>
+        <v>267</v>
       </c>
       <c r="Q68" s="15">
-        <v>339</v>
+        <v>318</v>
       </c>
       <c r="R68" s="15">
-        <v>399</v>
+        <v>375</v>
       </c>
       <c r="S68" s="15">
-        <v>459</v>
+        <v>432</v>
       </c>
       <c r="T68" s="15">
-        <v>519</v>
+        <v>492</v>
       </c>
       <c r="U68" s="15">
-        <v>579</v>
+        <v>546</v>
       </c>
       <c r="V68" s="15">
-        <v>636</v>
+        <v>600</v>
       </c>
       <c r="W68" s="15">
-        <v>690</v>
+        <v>651</v>
       </c>
       <c r="X68" s="15">
-        <v>738</v>
+        <v>699</v>
       </c>
       <c r="Y68" s="15">
-        <v>786</v>
+        <v>744</v>
       </c>
       <c r="Z68" s="15">
-        <v>828</v>
+        <v>783</v>
       </c>
       <c r="AA68" s="15">
-        <v>870</v>
+        <v>822</v>
       </c>
       <c r="AB68" s="15">
-        <v>906</v>
+        <v>858</v>
       </c>
       <c r="AC68" s="15">
-        <v>942</v>
+        <v>891</v>
       </c>
       <c r="AD68" s="15">
-        <v>972</v>
+        <v>921</v>
       </c>
       <c r="AE68" s="15">
-        <v>1002</v>
+        <v>948</v>
       </c>
       <c r="AF68" s="15">
-        <v>1032</v>
+        <v>975</v>
       </c>
     </row>
     <row r="70" spans="1:32" x14ac:dyDescent="0.35">
@@ -57483,127 +57603,127 @@
       </c>
       <c r="B70" s="48">
         <f>B62/SUM(B$62:B$68)</f>
-        <v>1.650872218881811E-2</v>
+        <v>1.7534211300949881E-2</v>
       </c>
       <c r="C70" s="48">
         <f t="shared" ref="C70:AF70" si="0">C62/SUM(C$62:C$68)</f>
-        <v>2.5720919756939725E-2</v>
+        <v>2.8864040627204268E-2</v>
       </c>
       <c r="D70" s="48">
         <f t="shared" si="0"/>
-        <v>4.2211197396420444E-2</v>
+        <v>5.0241664454241851E-2</v>
       </c>
       <c r="E70" s="48">
         <f t="shared" si="0"/>
-        <v>6.1754528666172294E-2</v>
+        <v>7.0758650731765238E-2</v>
       </c>
       <c r="F70" s="48">
         <f t="shared" si="0"/>
-        <v>8.6444988992676622E-2</v>
+        <v>9.6150854372302696E-2</v>
       </c>
       <c r="G70" s="48">
         <f t="shared" si="0"/>
-        <v>0.11508978791314754</v>
+        <v>0.12058109328935021</v>
       </c>
       <c r="H70" s="48">
         <f t="shared" si="0"/>
-        <v>0.1423498985223533</v>
+        <v>0.14052991776991805</v>
       </c>
       <c r="I70" s="48">
         <f t="shared" si="0"/>
-        <v>0.16709202046859911</v>
+        <v>0.16135807728986457</v>
       </c>
       <c r="J70" s="48">
         <f t="shared" si="0"/>
-        <v>0.18869620902088391</v>
+        <v>0.18314372646523142</v>
       </c>
       <c r="K70" s="48">
         <f t="shared" si="0"/>
-        <v>0.20832460043328452</v>
+        <v>0.2032151164147846</v>
       </c>
       <c r="L70" s="48">
         <f t="shared" si="0"/>
-        <v>0.22888945668562335</v>
+        <v>0.22476422487454586</v>
       </c>
       <c r="M70" s="48">
         <f t="shared" si="0"/>
-        <v>0.24535227615452435</v>
+        <v>0.24098600537220211</v>
       </c>
       <c r="N70" s="48">
         <f t="shared" si="0"/>
-        <v>0.2593839363224501</v>
+        <v>0.25493439672527313</v>
       </c>
       <c r="O70" s="48">
         <f t="shared" si="0"/>
-        <v>0.27266878019393226</v>
+        <v>0.26774162599682239</v>
       </c>
       <c r="P70" s="48">
         <f t="shared" si="0"/>
-        <v>0.28400582223935278</v>
+        <v>0.27908396458027679</v>
       </c>
       <c r="Q70" s="48">
         <f t="shared" si="0"/>
-        <v>0.29456797298796633</v>
+        <v>0.29107782779895086</v>
       </c>
       <c r="R70" s="48">
         <f t="shared" si="0"/>
-        <v>0.30515006522046739</v>
+        <v>0.30137284720381674</v>
       </c>
       <c r="S70" s="48">
         <f t="shared" si="0"/>
-        <v>0.3151983205949816</v>
+        <v>0.31173895957540304</v>
       </c>
       <c r="T70" s="48">
         <f t="shared" si="0"/>
-        <v>0.32583197661187263</v>
+        <v>0.32239200063148094</v>
       </c>
       <c r="U70" s="48">
         <f t="shared" si="0"/>
-        <v>0.33487032906925285</v>
+        <v>0.33170916981988363</v>
       </c>
       <c r="V70" s="48">
         <f t="shared" si="0"/>
-        <v>0.34431158320656369</v>
+        <v>0.34130863415238544</v>
       </c>
       <c r="W70" s="48">
         <f t="shared" si="0"/>
-        <v>0.35407817932283486</v>
+        <v>0.35114335532126362</v>
       </c>
       <c r="X70" s="48">
         <f t="shared" si="0"/>
-        <v>0.36301598074097552</v>
+        <v>0.36016052705388557</v>
       </c>
       <c r="Y70" s="48">
         <f t="shared" si="0"/>
-        <v>0.37267466704282326</v>
+        <v>0.36997957636638767</v>
       </c>
       <c r="Z70" s="48">
         <f t="shared" si="0"/>
-        <v>0.3825754580323476</v>
+        <v>0.37978549173238674</v>
       </c>
       <c r="AA70" s="48">
         <f t="shared" si="0"/>
-        <v>0.3915250022640257</v>
+        <v>0.38865470220283727</v>
       </c>
       <c r="AB70" s="48">
         <f t="shared" si="0"/>
-        <v>0.40078009600747744</v>
+        <v>0.39776474399041617</v>
       </c>
       <c r="AC70" s="48">
         <f t="shared" si="0"/>
-        <v>0.41068385298473431</v>
+        <v>0.40656121081044905</v>
       </c>
       <c r="AD70" s="48">
         <f t="shared" si="0"/>
-        <v>0.41910462797370385</v>
+        <v>0.41488065880011504</v>
       </c>
       <c r="AE70" s="48">
         <f t="shared" si="0"/>
-        <v>0.42766360453590085</v>
+        <v>0.42329771221057977</v>
       </c>
       <c r="AF70" s="48">
         <f t="shared" si="0"/>
-        <v>0.43625192528551504</v>
+        <v>0.43174767576613876</v>
       </c>
     </row>
     <row r="71" spans="1:32" x14ac:dyDescent="0.35">
@@ -57612,127 +57732,127 @@
       </c>
       <c r="B71" s="48">
         <f>B66/SUM(B$62:B$68)</f>
-        <v>4.1995277583808527E-3</v>
+        <v>4.3631403844649327E-3</v>
       </c>
       <c r="C71" s="48">
         <f t="shared" ref="C71:AF71" si="1">C66/SUM(C$62:C$68)</f>
-        <v>4.5137429567935075E-3</v>
+        <v>1.1871449687720248E-2</v>
       </c>
       <c r="D71" s="48">
         <f t="shared" si="1"/>
-        <v>5.0239440514220132E-3</v>
+        <v>1.9842421709307449E-2</v>
       </c>
       <c r="E71" s="48">
         <f t="shared" si="1"/>
-        <v>5.0562360266431785E-3</v>
+        <v>2.815284883538707E-2</v>
       </c>
       <c r="F71" s="48">
         <f t="shared" si="1"/>
-        <v>5.2911915607605168E-3</v>
+        <v>3.86069064069339E-2</v>
       </c>
       <c r="G71" s="48">
         <f t="shared" si="1"/>
-        <v>5.5551471435499825E-3</v>
+        <v>4.699492907437551E-2</v>
       </c>
       <c r="H71" s="48">
         <f t="shared" si="1"/>
-        <v>5.9453902538962114E-3</v>
+        <v>5.1787439629917768E-2</v>
       </c>
       <c r="I71" s="48">
         <f t="shared" si="1"/>
-        <v>6.3910885152455889E-3</v>
+        <v>5.4371127066517276E-2</v>
       </c>
       <c r="J71" s="48">
         <f t="shared" si="1"/>
-        <v>6.9939010448089008E-3</v>
+        <v>5.4693847396089096E-2</v>
       </c>
       <c r="K71" s="48">
         <f t="shared" si="1"/>
-        <v>7.9014657714060327E-3</v>
+        <v>5.473528366807251E-2</v>
       </c>
       <c r="L71" s="48">
         <f t="shared" si="1"/>
-        <v>8.9878737800208625E-3</v>
+        <v>5.3964259699758099E-2</v>
       </c>
       <c r="M71" s="48">
         <f t="shared" si="1"/>
-        <v>1.036412039058901E-2</v>
+        <v>5.3400763179844352E-2</v>
       </c>
       <c r="N71" s="48">
         <f t="shared" si="1"/>
-        <v>1.1893565823446113E-2</v>
+        <v>5.2421238977623442E-2</v>
       </c>
       <c r="O71" s="48">
         <f t="shared" si="1"/>
-        <v>1.3561240905372715E-2</v>
+        <v>5.1360353450791936E-2</v>
       </c>
       <c r="P71" s="48">
         <f t="shared" si="1"/>
-        <v>1.5357788410932908E-2</v>
+        <v>5.0355303535604641E-2</v>
       </c>
       <c r="Q71" s="48">
         <f t="shared" si="1"/>
-        <v>1.7207892014923055E-2</v>
+        <v>4.9423493932614339E-2</v>
       </c>
       <c r="R71" s="48">
         <f t="shared" si="1"/>
-        <v>1.8966963392944226E-2</v>
+        <v>4.857843616528329E-2</v>
       </c>
       <c r="S71" s="48">
         <f t="shared" si="1"/>
-        <v>2.0574027076982186E-2</v>
+        <v>4.7726226135846733E-2</v>
       </c>
       <c r="T71" s="48">
         <f t="shared" si="1"/>
-        <v>2.2026083117937537E-2</v>
+        <v>4.699596673874392E-2</v>
       </c>
       <c r="U71" s="48">
         <f t="shared" si="1"/>
-        <v>2.315486807403172E-2</v>
+        <v>4.6177005752552881E-2</v>
       </c>
       <c r="V71" s="48">
         <f t="shared" si="1"/>
-        <v>2.4064726048740114E-2</v>
+        <v>4.5453902365798778E-2</v>
       </c>
       <c r="W71" s="48">
         <f t="shared" si="1"/>
-        <v>2.4746025198479918E-2</v>
+        <v>4.477504113338223E-2</v>
       </c>
       <c r="X71" s="48">
         <f t="shared" si="1"/>
-        <v>2.5171178463135119E-2</v>
+        <v>4.4052038471715432E-2</v>
       </c>
       <c r="Y71" s="48">
         <f t="shared" si="1"/>
-        <v>2.5447459154078332E-2</v>
+        <v>4.3421723113208285E-2</v>
       </c>
       <c r="Z71" s="48">
         <f t="shared" si="1"/>
-        <v>2.5581634001059575E-2</v>
+        <v>4.2790424474047538E-2</v>
       </c>
       <c r="AA71" s="48">
         <f t="shared" si="1"/>
-        <v>2.5561607091746194E-2</v>
+        <v>4.2118015172965088E-2</v>
       </c>
       <c r="AB71" s="48">
         <f t="shared" si="1"/>
-        <v>2.5443519506555393E-2</v>
+        <v>4.1441567600264517E-2</v>
       </c>
       <c r="AC71" s="48">
         <f t="shared" si="1"/>
-        <v>2.5224110299208253E-2</v>
+        <v>4.0751732451896089E-2</v>
       </c>
       <c r="AD71" s="48">
         <f t="shared" si="1"/>
-        <v>2.4941751355858553E-2</v>
+        <v>4.0035161980609572E-2</v>
       </c>
       <c r="AE71" s="48">
         <f t="shared" si="1"/>
-        <v>2.4620105782699183E-2</v>
+        <v>3.9322865057960822E-2</v>
       </c>
       <c r="AF71" s="48">
         <f t="shared" si="1"/>
-        <v>2.4254268542743439E-2</v>
+        <v>3.8591562848336439E-2</v>
       </c>
     </row>
     <row r="72" spans="1:32" x14ac:dyDescent="0.35">
@@ -57741,127 +57861,127 @@
       </c>
       <c r="B72" s="59">
         <f>SUM(B70:B71)</f>
-        <v>2.0708249947198963E-2</v>
+        <v>2.1897351685414814E-2</v>
       </c>
       <c r="C72" s="59">
         <f t="shared" ref="C72:AF72" si="2">SUM(C70:C71)</f>
-        <v>3.0234662713733231E-2</v>
+        <v>4.0735490314924516E-2</v>
       </c>
       <c r="D72" s="59">
         <f t="shared" si="2"/>
-        <v>4.7235141447842459E-2</v>
+        <v>7.0084086163549303E-2</v>
       </c>
       <c r="E72" s="59">
         <f t="shared" si="2"/>
-        <v>6.6810764692815466E-2</v>
+        <v>9.8911499567152311E-2</v>
       </c>
       <c r="F72" s="59">
         <f t="shared" si="2"/>
-        <v>9.1736180553437144E-2</v>
+        <v>0.1347577607792366</v>
       </c>
       <c r="G72" s="59">
         <f t="shared" si="2"/>
-        <v>0.12064493505669753</v>
+        <v>0.16757602236372571</v>
       </c>
       <c r="H72" s="59">
         <f t="shared" si="2"/>
-        <v>0.14829528877624951</v>
+        <v>0.19231735739983583</v>
       </c>
       <c r="I72" s="59">
         <f t="shared" si="2"/>
-        <v>0.1734831089838447</v>
+        <v>0.21572920435638185</v>
       </c>
       <c r="J72" s="59">
         <f t="shared" si="2"/>
-        <v>0.19569011006569281</v>
+        <v>0.23783757386132051</v>
       </c>
       <c r="K72" s="59">
         <f t="shared" si="2"/>
-        <v>0.21622606620469054</v>
+        <v>0.25795040008285708</v>
       </c>
       <c r="L72" s="59">
         <f t="shared" si="2"/>
-        <v>0.23787733046564422</v>
+        <v>0.27872848457430399</v>
       </c>
       <c r="M72" s="59">
         <f t="shared" si="2"/>
-        <v>0.25571639654511336</v>
+        <v>0.29438676855204648</v>
       </c>
       <c r="N72" s="59">
         <f t="shared" si="2"/>
-        <v>0.27127750214589624</v>
+        <v>0.30735563570289659</v>
       </c>
       <c r="O72" s="59">
         <f t="shared" si="2"/>
-        <v>0.28623002109930495</v>
+        <v>0.31910197944761431</v>
       </c>
       <c r="P72" s="59">
         <f t="shared" si="2"/>
-        <v>0.29936361065028566</v>
+        <v>0.32943926811588142</v>
       </c>
       <c r="Q72" s="59">
         <f t="shared" si="2"/>
-        <v>0.3117758650028894</v>
+        <v>0.34050132173156522</v>
       </c>
       <c r="R72" s="59">
         <f t="shared" si="2"/>
-        <v>0.32411702861341163</v>
+        <v>0.34995128336910003</v>
       </c>
       <c r="S72" s="59">
         <f t="shared" si="2"/>
-        <v>0.33577234767196379</v>
+        <v>0.35946518571124975</v>
       </c>
       <c r="T72" s="59">
         <f t="shared" si="2"/>
-        <v>0.34785805972981015</v>
+        <v>0.36938796737022483</v>
       </c>
       <c r="U72" s="59">
         <f t="shared" si="2"/>
-        <v>0.35802519714328457</v>
+        <v>0.37788617557243653</v>
       </c>
       <c r="V72" s="59">
         <f t="shared" si="2"/>
-        <v>0.36837630925530379</v>
+        <v>0.38676253651818421</v>
       </c>
       <c r="W72" s="59">
         <f t="shared" si="2"/>
-        <v>0.37882420452131477</v>
+        <v>0.39591839645464583</v>
       </c>
       <c r="X72" s="59">
         <f t="shared" si="2"/>
-        <v>0.38818715920411062</v>
+        <v>0.40421256552560103</v>
       </c>
       <c r="Y72" s="59">
         <f t="shared" si="2"/>
-        <v>0.39812212619690157</v>
+        <v>0.41340129947959597</v>
       </c>
       <c r="Z72" s="59">
         <f t="shared" si="2"/>
-        <v>0.40815709203340717</v>
+        <v>0.42257591620643425</v>
       </c>
       <c r="AA72" s="59">
         <f t="shared" si="2"/>
-        <v>0.41708660935577191</v>
+        <v>0.43077271737580236</v>
       </c>
       <c r="AB72" s="59">
         <f t="shared" si="2"/>
-        <v>0.42622361551403282</v>
+        <v>0.43920631159068069</v>
       </c>
       <c r="AC72" s="59">
         <f t="shared" si="2"/>
-        <v>0.43590796328394255</v>
+        <v>0.44731294326234516</v>
       </c>
       <c r="AD72" s="59">
         <f t="shared" si="2"/>
-        <v>0.44404637932956242</v>
+        <v>0.45491582078072462</v>
       </c>
       <c r="AE72" s="59">
         <f t="shared" si="2"/>
-        <v>0.45228371031860004</v>
+        <v>0.46262057726854061</v>
       </c>
       <c r="AF72" s="59">
         <f t="shared" si="2"/>
-        <v>0.46050619382825847</v>
+        <v>0.47033923861447519</v>
       </c>
     </row>
     <row r="73" spans="1:32" x14ac:dyDescent="0.35">
@@ -57933,107 +58053,191 @@
       <c r="AE74" s="59"/>
       <c r="AF74" s="59"/>
     </row>
-    <row r="76" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A76" s="47" t="s">
+    <row r="76" spans="1:32" ht="29" x14ac:dyDescent="0.35">
+      <c r="F76" s="60" t="s">
+        <v>971</v>
+      </c>
+      <c r="G76" s="15">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="77" spans="1:32" ht="29" x14ac:dyDescent="0.35">
+      <c r="F77" s="60" t="s">
+        <v>972</v>
+      </c>
+      <c r="G77" s="15">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="78" spans="1:32" ht="29" x14ac:dyDescent="0.35">
+      <c r="F78" s="60" t="s">
+        <v>973</v>
+      </c>
+      <c r="G78" s="48">
+        <f>G77/G76</f>
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="80" spans="1:32" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="F80" s="60" t="s">
+        <v>974</v>
+      </c>
+      <c r="G80" s="48">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="F81" s="60" t="s">
+        <v>975</v>
+      </c>
+      <c r="G81" s="48">
+        <f>G80*G78</f>
+        <v>0.21937500000000001</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A82" s="15" t="s">
+        <v>977</v>
+      </c>
+      <c r="F82" s="60" t="s">
+        <v>976</v>
+      </c>
+      <c r="G82" s="48">
+        <f>G80-G81</f>
+        <v>5.0625000000000003E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A83" s="15" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A84" s="15" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A85" s="15" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A86" s="15" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A87" s="15" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A88" s="15" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A91" s="47" t="s">
         <v>916</v>
       </c>
     </row>
-    <row r="78" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="E78" s="43"/>
-      <c r="F78" s="43"/>
-      <c r="G78" s="43"/>
-      <c r="H78" s="43"/>
-      <c r="I78" s="43"/>
-      <c r="J78" s="43"/>
-      <c r="K78" s="43" t="s">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="E93" s="43"/>
+      <c r="F93" s="43"/>
+      <c r="G93" s="43"/>
+      <c r="H93" s="43"/>
+      <c r="I93" s="43"/>
+      <c r="J93" s="43"/>
+      <c r="K93" s="43" t="s">
         <v>933</v>
       </c>
-      <c r="L78" s="43"/>
-      <c r="M78" s="43"/>
-      <c r="N78" s="43"/>
-      <c r="O78" s="43"/>
-    </row>
-    <row r="79" spans="1:32" s="41" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="E79" s="42"/>
-      <c r="F79" s="42"/>
-      <c r="G79" s="42"/>
-      <c r="H79" s="42"/>
-      <c r="I79" s="42"/>
-      <c r="J79" s="42"/>
-      <c r="K79" s="42"/>
-      <c r="L79" s="42"/>
-      <c r="M79" s="42"/>
-      <c r="N79" s="42"/>
-      <c r="O79" s="42"/>
-    </row>
-    <row r="80" spans="1:32" s="41" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="E80" s="42"/>
-      <c r="F80" s="42"/>
-      <c r="G80" s="42"/>
-      <c r="H80" s="42"/>
-      <c r="I80" s="42"/>
-      <c r="J80" s="42"/>
-      <c r="K80" s="42"/>
-      <c r="L80" s="42"/>
-      <c r="M80" s="42"/>
-      <c r="N80" s="42"/>
-      <c r="O80" s="42"/>
-    </row>
-    <row r="81" spans="5:17" s="41" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="E81" s="42"/>
-      <c r="F81" s="42"/>
-      <c r="G81" s="42"/>
-      <c r="H81" s="42"/>
-      <c r="I81" s="42"/>
-      <c r="J81" s="42"/>
-      <c r="K81" s="42"/>
-      <c r="L81" s="42"/>
-      <c r="M81" s="42"/>
-      <c r="N81" s="42"/>
-      <c r="O81" s="42"/>
-      <c r="P81" s="42"/>
-      <c r="Q81" s="42"/>
-    </row>
-    <row r="88" spans="5:17" x14ac:dyDescent="0.35">
-      <c r="K88" s="15" t="s">
+      <c r="L93" s="43"/>
+      <c r="M93" s="43"/>
+      <c r="N93" s="43"/>
+      <c r="O93" s="43"/>
+    </row>
+    <row r="94" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E94" s="42"/>
+      <c r="F94" s="42"/>
+      <c r="G94" s="42"/>
+      <c r="H94" s="42"/>
+      <c r="I94" s="42"/>
+      <c r="J94" s="42"/>
+      <c r="K94" s="42"/>
+      <c r="L94" s="42"/>
+      <c r="M94" s="42"/>
+      <c r="N94" s="42"/>
+      <c r="O94" s="42"/>
+    </row>
+    <row r="95" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E95" s="42"/>
+      <c r="F95" s="42"/>
+      <c r="G95" s="42"/>
+      <c r="H95" s="42"/>
+      <c r="I95" s="42"/>
+      <c r="J95" s="42"/>
+      <c r="K95" s="42"/>
+      <c r="L95" s="42"/>
+      <c r="M95" s="42"/>
+      <c r="N95" s="42"/>
+      <c r="O95" s="42"/>
+    </row>
+    <row r="96" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E96" s="42"/>
+      <c r="F96" s="42"/>
+      <c r="G96" s="42"/>
+      <c r="H96" s="42"/>
+      <c r="I96" s="42"/>
+      <c r="J96" s="42"/>
+      <c r="K96" s="42"/>
+      <c r="L96" s="42"/>
+      <c r="M96" s="42"/>
+      <c r="N96" s="42"/>
+      <c r="O96" s="42"/>
+      <c r="P96" s="42"/>
+      <c r="Q96" s="42"/>
+    </row>
+    <row r="103" spans="11:11" x14ac:dyDescent="0.35">
+      <c r="K103" s="15" t="s">
         <v>934</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A99" s="15" t="s">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114" s="15" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A101" s="15" t="s">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A116" s="15" t="s">
         <v>935</v>
       </c>
-      <c r="B101" s="15">
+      <c r="B116" s="15">
         <f>SUM('AEO 49'!E210,'AEO 49'!E221,'AEO 44'!G36)</f>
         <v>1.326343</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A102" s="15" t="s">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A117" s="15" t="s">
         <v>936</v>
       </c>
-      <c r="B102" s="15">
+      <c r="B117" s="15">
         <f>SUM('AEO 49'!E214,'AEO 49'!E225,'AEO 44'!K36)</f>
         <v>1079.7512820000002</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A103" s="15" t="s">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A118" s="15" t="s">
         <v>931</v>
       </c>
-      <c r="B103" s="48">
-        <f>B101/B102</f>
+      <c r="B118" s="48">
+        <f>B116/B117</f>
         <v>1.228378259059108E-3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A76" r:id="rId1" xr:uid="{21E58E80-C89D-48AA-B679-F2359EAD50AA}"/>
+    <hyperlink ref="A91" r:id="rId1" xr:uid="{21E58E80-C89D-48AA-B679-F2359EAD50AA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -58051,8 +58255,8 @@
   </sheetPr>
   <dimension ref="A1:AL93"/>
   <sheetViews>
-    <sheetView topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10:AL10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -58340,7 +58544,7 @@
       <c r="D10" s="29">
         <v>0.17499999999999999</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="17">
         <v>1</v>
       </c>
       <c r="F10" s="9" t="str">
@@ -58900,137 +59104,137 @@
       <c r="D14" s="29">
         <v>1.7500000000000002E-2</v>
       </c>
-      <c r="E14" s="29">
-        <f>SUM(SUM(INDEX('AEO 39'!25:26,0,MATCH(E$9,'AEO 39'!$1:$1,0))),SUM(INDEX('AEO 39'!47:48,0,MATCH(E$9,'AEO 39'!$1:$1,0))))/INDEX('AEO 39'!$59:$59,MATCH(E$9,'AEO 39'!$1:$1,0))*Assumptions!A11*3</f>
-        <v>0.19664026629095921</v>
+      <c r="E14" s="61">
+        <f>SUM(SUM(INDEX('AEO 39'!25:26,0,MATCH(E$9,'AEO 39'!$1:$1,0))),SUM(INDEX('AEO 39'!47:48,0,MATCH(E$9,'AEO 39'!$1:$1,0))))/INDEX('AEO 39'!$59:$59,MATCH(E$9,'AEO 39'!$1:$1,0))*Assumptions!A11*5</f>
+        <v>0.32773377715159868</v>
       </c>
       <c r="F14" s="9" t="str">
         <f>IF(D14=E14,"n/a",IF(OR(C14="battery electric vehicle",C14="natural gas vehicle",C14="plugin hybrid vehicle",C14="hydrogen vehicle"),"s-curve","linear"))</f>
         <v>s-curve</v>
       </c>
-      <c r="H14" s="29">
-        <f t="shared" si="1"/>
-        <v>1.7500000000000002E-2</v>
+      <c r="H14" s="22">
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:H$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,H$9))/2</f>
+        <v>1.7641947805604345E-2</v>
       </c>
       <c r="I14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:I$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,I$9))</f>
-        <v>2.0146623971724009E-2</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:I$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,I$9))</f>
+        <v>5.1345518914747604E-2</v>
       </c>
       <c r="J14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:J$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,J$9))</f>
-        <v>2.1054197652496692E-2</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:J$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,J$9))</f>
+        <v>7.8869239433912761E-2</v>
       </c>
       <c r="K14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:K$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,K$9))</f>
-        <v>2.2264592511898683E-2</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:K$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,K$9))</f>
+        <v>0.12043936074535663</v>
       </c>
       <c r="L14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:L$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,L$9))</f>
-        <v>2.3872232318586158E-2</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:L$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,L$9))</f>
+        <v>0.17261688857579932</v>
       </c>
       <c r="M14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:M$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,M$9))</f>
-        <v>2.5995883550110573E-2</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:M$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,M$9))</f>
+        <v>0.22479441640624204</v>
       </c>
       <c r="N14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:N$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,N$9))</f>
-        <v>2.8781063773285744E-2</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:N$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,N$9))</f>
+        <v>0.26636453771768587</v>
       </c>
       <c r="O14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:O$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,O$9))</f>
-        <v>3.2399578998058384E-2</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:O$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,O$9))</f>
+        <v>0.29388825823685111</v>
       </c>
       <c r="P14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:P$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,P$9))</f>
-        <v>3.7043633600479256E-2</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:P$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,P$9))</f>
+        <v>0.30994988154038999</v>
       </c>
       <c r="Q14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:Q$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,Q$9))</f>
-        <v>4.2911237539929523E-2</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:Q$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,Q$9))</f>
+        <v>0.31864013308886613</v>
       </c>
       <c r="R14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:R$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,R$9))</f>
-        <v>5.0179756912938397E-2</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:R$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,R$9))</f>
+        <v>0.32315037349563713</v>
       </c>
       <c r="S14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:S$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,S$9))</f>
-        <v>5.8966531923743418E-2</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:S$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,S$9))</f>
+        <v>0.32544067136138988</v>
       </c>
       <c r="T14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:T$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,T$9))</f>
-        <v>6.9280583071290994E-2</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:T$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,T$9))</f>
+        <v>0.32659080149166408</v>
       </c>
       <c r="U14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:U$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,U$9))</f>
-        <v>8.0977223661233097E-2</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:U$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,U$9))</f>
+        <v>0.3271651375801809</v>
       </c>
       <c r="V14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:V$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,V$9))</f>
-        <v>9.3734480860469802E-2</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:V$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,V$9))</f>
+        <v>0.32745113829838129</v>
       </c>
       <c r="W14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:W$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,W$9))</f>
-        <v>0.1070701331454796</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:W$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,W$9))</f>
+        <v>0.32759335844966003</v>
       </c>
       <c r="X14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:X$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,X$9))</f>
-        <v>0.1204057854304894</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:X$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,X$9))</f>
+        <v>0.32766403139580214</v>
       </c>
       <c r="Y14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:Y$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,Y$9))</f>
-        <v>0.13316304262972609</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:Y$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,Y$9))</f>
+        <v>0.32769913851400356</v>
       </c>
       <c r="Z14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:Z$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,Z$9))</f>
-        <v>0.14485968321966819</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:Z$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,Z$9))</f>
+        <v>0.32771657514633645</v>
       </c>
       <c r="AA14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:AA$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,AA$9))</f>
-        <v>0.15517373436721577</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:AA$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,AA$9))</f>
+        <v>0.3277252346501377</v>
       </c>
       <c r="AB14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:AB$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,AB$9))</f>
-        <v>0.16396050937802081</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:AB$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,AB$9))</f>
+        <v>0.32772953501211155</v>
       </c>
       <c r="AC14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:AC$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,AC$9))</f>
-        <v>0.17122902875102969</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:AC$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,AC$9))</f>
+        <v>0.32773167055297159</v>
       </c>
       <c r="AD14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:AD$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,AD$9))</f>
-        <v>0.17709663269047993</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:AD$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,AD$9))</f>
+        <v>0.32773273104210349</v>
       </c>
       <c r="AE14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:AE$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,AE$9))</f>
-        <v>0.18174068729290083</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:AE$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,AE$9))</f>
+        <v>0.3277332576681154</v>
       </c>
       <c r="AF14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:AF$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,AF$9))</f>
-        <v>0.18535920251767346</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:AF$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,AF$9))</f>
+        <v>0.32773351918351784</v>
       </c>
       <c r="AG14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:AG$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,AG$9))</f>
-        <v>0.18814438274084866</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:AG$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,AG$9))</f>
+        <v>0.32773364904838725</v>
       </c>
       <c r="AH14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:AH$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,AH$9))</f>
-        <v>0.19026803397237302</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:AH$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,AH$9))</f>
+        <v>0.32773371353741332</v>
       </c>
       <c r="AI14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:AI$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,AI$9))</f>
-        <v>0.19187567377906051</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:AI$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,AI$9))</f>
+        <v>0.32773374556172585</v>
       </c>
       <c r="AJ14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:AJ$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,AJ$9))</f>
-        <v>0.1930860686384625</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:AJ$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,AJ$9))</f>
+        <v>0.32773376146453126</v>
       </c>
       <c r="AK14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:AK$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,AK$9))</f>
-        <v>0.19399364231923522</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:AK$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,AK$9))</f>
+        <v>0.32773376936163134</v>
       </c>
       <c r="AL14" s="15">
-        <f>IF($F14="s-curve",$D14+($E14-$D14)*$I$2/(1+EXP($I$3*(COUNT($H$9:AL$9)+$I$4))),TREND($D14:$E14,$D$9:$E$9,AL$9))</f>
-        <v>0.19467206246239127</v>
+        <f>IF($F14="s-curve",$D14+($E14-$D14)*$O$2/(1+EXP($O$3*(COUNT($H$9:AL$9)+$O$4))),TREND($D14:$E14,$D$9:$E$9,AL$9))</f>
+        <v>0.32773377328321535</v>
       </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.35">
@@ -59891,7 +60095,7 @@
       </c>
       <c r="E21" s="29">
         <f>E14</f>
-        <v>0.19664026629095921</v>
+        <v>0.32773377715159868</v>
       </c>
       <c r="F21" s="9" t="str">
         <f>IF(D21=E21,"n/a",IF(OR(C21="battery electric vehicle",C21="natural gas vehicle",C21="plugin hybrid vehicle"),"s-curve","linear"))</f>
@@ -59903,123 +60107,123 @@
       </c>
       <c r="I21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:I$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,I$9))</f>
-        <v>2.9051695263562845E-3</v>
+        <v>4.8419492105938079E-3</v>
       </c>
       <c r="J21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:J$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,J$9))</f>
-        <v>3.9014030028430464E-3</v>
+        <v>6.5023383380717441E-3</v>
       </c>
       <c r="K21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:K$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,K$9))</f>
-        <v>5.230039899493835E-3</v>
+        <v>8.7167331658230592E-3</v>
       </c>
       <c r="L21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:L$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,L$9))</f>
-        <v>6.9947281308572898E-3</v>
+        <v>1.1657880218095483E-2</v>
       </c>
       <c r="M21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:M$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,M$9))</f>
-        <v>9.3258363307179917E-3</v>
+        <v>1.5543060551196652E-2</v>
       </c>
       <c r="N21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:N$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,N$9))</f>
-        <v>1.2383097504283182E-2</v>
+        <v>2.063849584047197E-2</v>
       </c>
       <c r="O21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:O$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,O$9))</f>
-        <v>1.6355101186702026E-2</v>
+        <v>2.7258501977836708E-2</v>
       </c>
       <c r="P21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:P$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,P$9))</f>
-        <v>2.1452827971402487E-2</v>
+        <v>3.5754713285670814E-2</v>
       </c>
       <c r="Q21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:Q$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,Q$9))</f>
-        <v>2.789363117568806E-2</v>
+        <v>4.6489385292813434E-2</v>
       </c>
       <c r="R21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:R$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,R$9))</f>
-        <v>3.5872203579549629E-2</v>
+        <v>5.9787005965916053E-2</v>
       </c>
       <c r="S21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:S$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,S$9))</f>
-        <v>4.5517348212510605E-2</v>
+        <v>7.5862247020851009E-2</v>
       </c>
       <c r="T21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:T$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,T$9))</f>
-        <v>5.6838966775353432E-2</v>
+        <v>9.4731611292255713E-2</v>
       </c>
       <c r="U21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:U$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,U$9))</f>
-        <v>6.9678238302281689E-2</v>
+        <v>0.11613039717046947</v>
       </c>
       <c r="V21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:V$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,V$9))</f>
-        <v>8.368173681626577E-2</v>
+        <v>0.13946956136044295</v>
       </c>
       <c r="W21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:W$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,W$9))</f>
-        <v>9.8320133145479605E-2</v>
+        <v>0.16386688857579934</v>
       </c>
       <c r="X21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:X$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,X$9))</f>
-        <v>0.11295852947469344</v>
+        <v>0.18826421579115574</v>
       </c>
       <c r="Y21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:Y$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,Y$9))</f>
-        <v>0.12696202798867751</v>
+        <v>0.21160337998112919</v>
       </c>
       <c r="Z21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:Z$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,Z$9))</f>
-        <v>0.13980129951560577</v>
+        <v>0.23300216585934294</v>
       </c>
       <c r="AA21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:AA$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,AA$9))</f>
-        <v>0.1511229180784486</v>
+        <v>0.25187153013074765</v>
       </c>
       <c r="AB21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:AB$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,AB$9))</f>
-        <v>0.16076806271140956</v>
+        <v>0.26794677118568261</v>
       </c>
       <c r="AC21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:AC$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,AC$9))</f>
-        <v>0.16874663511527116</v>
+        <v>0.2812443918587853</v>
       </c>
       <c r="AD21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:AD$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,AD$9))</f>
-        <v>0.17518743831955672</v>
+        <v>0.29197906386592787</v>
       </c>
       <c r="AE21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:AE$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,AE$9))</f>
-        <v>0.18028516510425718</v>
+        <v>0.30047527517376199</v>
       </c>
       <c r="AF21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:AF$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,AF$9))</f>
-        <v>0.18425716878667603</v>
+        <v>0.30709528131112673</v>
       </c>
       <c r="AG21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:AG$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,AG$9))</f>
-        <v>0.18731442996024122</v>
+        <v>0.31219071660040204</v>
       </c>
       <c r="AH21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:AH$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,AH$9))</f>
-        <v>0.18964553816010193</v>
+        <v>0.31607589693350319</v>
       </c>
       <c r="AI21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:AI$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,AI$9))</f>
-        <v>0.19141022639146535</v>
+        <v>0.31901704398577563</v>
       </c>
       <c r="AJ21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:AJ$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,AJ$9))</f>
-        <v>0.19273886328811618</v>
+        <v>0.32123143881352695</v>
       </c>
       <c r="AK21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:AK$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,AK$9))</f>
-        <v>0.19373509676460293</v>
+        <v>0.32289182794100485</v>
       </c>
       <c r="AL21" s="15">
         <f>IF($F21="s-curve",$D21+($E21-$D21)*$I$2/(1+EXP($I$3*(COUNT($H$9:AL$9)+$I$4))),TREND($D21:$E21,$D$9:$E$9,AL$9))</f>
-        <v>0.19447979096635587</v>
+        <v>0.32413298494392645</v>
       </c>
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Additional ZEV calibration edits in TTS file
</commit_message>
<xml_diff>
--- a/InputData/trans/TTS/Transportation Technology Shareweights.xlsx
+++ b/InputData/trans/TTS/Transportation Technology Shareweights.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\TTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464FD464-6630-4FC2-9D91-A6FF915FAC0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3E9D49-3C08-403B-955B-13A3673F78ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -4668,466 +4668,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>TTS Value</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Data!$I$9:$AL$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
-                <c:pt idx="0">
-                  <c:v>2021</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2022</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2023</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2024</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2025</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2026</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2027</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2028</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2029</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2030</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2031</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2032</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2033</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2034</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2035</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2036</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2037</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2038</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2039</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2040</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2041</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2042</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2043</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2044</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2045</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2046</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2047</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2049</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2050</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Data!$I$10:$AL$10</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="30"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>1.7999999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.8000000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>5.8459569384324707E-2</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
-                  <c:v>6.9874456154344386E-2</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>9.3149431265043575E-2</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>0.13877269058395222</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>0.22166909866365125</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>0.35342187838502587</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="General">
-                  <c:v>0.52400000000000002</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="General">
-                  <c:v>0.69457812161497412</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="General">
-                  <c:v>0.82633090133634868</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="General">
-                  <c:v>0.90922730941604779</c:v>
-                </c:pt>
-                <c:pt idx="12" formatCode="General">
-                  <c:v>0.95485056873495655</c:v>
-                </c:pt>
-                <c:pt idx="13" formatCode="General">
-                  <c:v>0.97812554384565553</c:v>
-                </c:pt>
-                <c:pt idx="14" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="15" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="16" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="17" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="18" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="19" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="20" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="21" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="22" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="23" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="24" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="25" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="26" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="27" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="28" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="29" formatCode="General">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7845-4F26-8099-2F927049CEFA}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="343204120"/>
-        <c:axId val="343203464"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="343204120"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="343203464"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="343203464"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="1"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="343204120"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5180,99 +4720,99 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Data!$I$10:$AL$10</c:f>
+              <c:f>Data!$I$17:$AL$17</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>1.7999999999999999E-2</c:v>
+                <c:pt idx="0" formatCode="0.0000">
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.8000000000000001E-2</c:v>
+                  <c:v>0.21838189592802051</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>5.8459569384324707E-2</c:v>
+                <c:pt idx="2">
+                  <c:v>0.23794069854205344</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="General">
-                  <c:v>6.9874456154344386E-2</c:v>
+                <c:pt idx="3">
+                  <c:v>0.27627957191928759</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>9.3149431265043575E-2</c:v>
+                <c:pt idx="4">
+                  <c:v>0.3459404190450851</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>0.13877269058395222</c:v>
+                <c:pt idx="5">
+                  <c:v>0.45665704065968565</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>0.22166909866365125</c:v>
+                <c:pt idx="6">
+                  <c:v>0.60000000000000009</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>0.35342187838502587</c:v>
+                <c:pt idx="7">
+                  <c:v>0.74334295934031447</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="General">
-                  <c:v>0.52400000000000002</c:v>
+                <c:pt idx="8">
+                  <c:v>0.85405958095491497</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="General">
-                  <c:v>0.69457812161497412</c:v>
+                <c:pt idx="9">
+                  <c:v>0.92372042808071253</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="General">
-                  <c:v>0.82633090133634868</c:v>
+                <c:pt idx="10">
+                  <c:v>0.9620593014579466</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
-                  <c:v>0.90922730941604779</c:v>
+                <c:pt idx="11">
+                  <c:v>0.98161810407197958</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="General">
-                  <c:v>0.95485056873495655</c:v>
+                <c:pt idx="12">
+                  <c:v>0.99121044589552554</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="General">
-                  <c:v>0.97812554384565553</c:v>
+                <c:pt idx="13">
+                  <c:v>0.99582389944515337</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="General">
-                  <c:v>1</c:v>
+                <c:pt idx="14">
+                  <c:v>0.99802190147469227</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="General">
-                  <c:v>1</c:v>
+                <c:pt idx="15">
+                  <c:v>0.99906439178795559</c:v>
                 </c:pt>
-                <c:pt idx="16" formatCode="General">
-                  <c:v>1</c:v>
+                <c:pt idx="16">
+                  <c:v>0.99955777709046112</c:v>
                 </c:pt>
-                <c:pt idx="17" formatCode="General">
-                  <c:v>1</c:v>
+                <c:pt idx="17">
+                  <c:v>0.9997910477447236</c:v>
                 </c:pt>
-                <c:pt idx="18" formatCode="General">
-                  <c:v>1</c:v>
+                <c:pt idx="18">
+                  <c:v>0.99990128433921099</c:v>
                 </c:pt>
-                <c:pt idx="19" formatCode="General">
-                  <c:v>1</c:v>
+                <c:pt idx="19">
+                  <c:v>0.99995336698747117</c:v>
                 </c:pt>
-                <c:pt idx="20" formatCode="General">
-                  <c:v>1</c:v>
+                <c:pt idx="20">
+                  <c:v>0.99997797144710843</c:v>
                 </c:pt>
-                <c:pt idx="21" formatCode="General">
-                  <c:v>1</c:v>
+                <c:pt idx="21">
+                  <c:v>0.99998959429722678</c:v>
                 </c:pt>
-                <c:pt idx="22" formatCode="General">
-                  <c:v>1</c:v>
+                <c:pt idx="22">
+                  <c:v>0.99999508466031828</c:v>
                 </c:pt>
-                <c:pt idx="23" formatCode="General">
-                  <c:v>1</c:v>
+                <c:pt idx="23">
+                  <c:v>0.99999767815041185</c:v>
                 </c:pt>
-                <c:pt idx="24" formatCode="General">
-                  <c:v>1</c:v>
+                <c:pt idx="24">
+                  <c:v>0.99999890323423446</c:v>
                 </c:pt>
-                <c:pt idx="25" formatCode="General">
-                  <c:v>1</c:v>
+                <c:pt idx="25">
+                  <c:v>0.99999948192416133</c:v>
                 </c:pt>
-                <c:pt idx="26" formatCode="General">
-                  <c:v>1</c:v>
+                <c:pt idx="26">
+                  <c:v>0.99999975527821849</c:v>
                 </c:pt>
-                <c:pt idx="27" formatCode="General">
-                  <c:v>1</c:v>
+                <c:pt idx="27">
+                  <c:v>0.99999988440159693</c:v>
                 </c:pt>
-                <c:pt idx="28" formatCode="General">
-                  <c:v>1</c:v>
+                <c:pt idx="28">
+                  <c:v>0.99999994539517689</c:v>
                 </c:pt>
-                <c:pt idx="29" formatCode="General">
-                  <c:v>1</c:v>
+                <c:pt idx="29">
+                  <c:v>0.99999997420650688</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5280,7 +4820,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-EB5A-4159-9417-DF28BAD9DBA5}"/>
+              <c16:uniqueId val="{00000000-3B56-4178-8258-F69654CF177C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5293,11 +4833,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1489141072"/>
-        <c:axId val="908462080"/>
+        <c:axId val="720846560"/>
+        <c:axId val="1290876240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1489141072"/>
+        <c:axId val="720846560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5339,7 +4879,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="908462080"/>
+        <c:crossAx val="1290876240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5347,7 +4887,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="908462080"/>
+        <c:axId val="1290876240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5367,7 +4907,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5398,7 +4938,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1489141072"/>
+        <c:crossAx val="720846560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5495,46 +5035,6 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -6606,522 +6106,6 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -7167,23 +6151,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>361949</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>169068</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>141287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>57945</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>53975</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>463550</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>144462</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49228D84-E7C9-CF7F-FA1E-0DFE7495F1B0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7196,42 +6180,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76711D4E-A789-C8D9-97AA-2C6E9406FC81}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7529,7 +6477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
@@ -9238,123 +8186,123 @@
       </c>
       <c r="B2">
         <f>Data!I17</f>
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="C2">
         <f>Data!J17</f>
-        <v>7.1828501414524334E-2</v>
+        <v>0.21838189592802051</v>
       </c>
       <c r="D2">
         <f>Data!K17</f>
-        <v>9.505457951868844E-2</v>
+        <v>0.23794069854205344</v>
       </c>
       <c r="E2">
         <f>Data!L17</f>
-        <v>0.14058199165415403</v>
+        <v>0.27627957191928759</v>
       </c>
       <c r="F2">
         <f>Data!M17</f>
-        <v>0.22330424761603851</v>
+        <v>0.3459404190450851</v>
       </c>
       <c r="G2">
         <f>Data!N17</f>
-        <v>0.35478023578337664</v>
+        <v>0.45665704065968565</v>
       </c>
       <c r="H2">
         <f>Data!O17</f>
-        <v>0.52500000000000002</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="I2">
         <f>Data!P17</f>
-        <v>0.69521976421662335</v>
+        <v>0.74334295934031447</v>
       </c>
       <c r="J2">
         <f>Data!Q17</f>
-        <v>0.82669575238396142</v>
+        <v>0.85405958095491497</v>
       </c>
       <c r="K2">
         <f>Data!R17</f>
-        <v>0.90941800834584607</v>
+        <v>0.92372042808071253</v>
       </c>
       <c r="L2">
         <f>Data!S17</f>
-        <v>0.9549454204813117</v>
+        <v>0.9620593014579466</v>
       </c>
       <c r="M2">
         <f>Data!T17</f>
-        <v>0.97817149858547559</v>
+        <v>0.98161810407197958</v>
       </c>
       <c r="N2">
         <f>Data!U17</f>
-        <v>0.98956240450093647</v>
+        <v>0.99121044589552554</v>
       </c>
       <c r="O2">
         <f>Data!V17</f>
-        <v>0.9950408805911195</v>
+        <v>0.99582389944515337</v>
       </c>
       <c r="P2">
         <f>Data!W17</f>
-        <v>0.9976510080011971</v>
+        <v>0.99802190147469227</v>
       </c>
       <c r="Q2">
         <f>Data!X17</f>
-        <v>0.99888896524819726</v>
+        <v>0.99906439178795559</v>
       </c>
       <c r="R2">
         <f>Data!Y17</f>
-        <v>0.99947486029492261</v>
+        <v>0.99955777709046112</v>
       </c>
       <c r="S2">
         <f>Data!Z17</f>
-        <v>0.9997518691968591</v>
+        <v>0.9997910477447236</v>
       </c>
       <c r="T2">
         <f>Data!AA17</f>
-        <v>0.99988277515281299</v>
+        <v>0.99990128433921099</v>
       </c>
       <c r="U2">
         <f>Data!AB17</f>
-        <v>0.9999446232976219</v>
+        <v>0.99995336698747117</v>
       </c>
       <c r="V2">
         <f>Data!AC17</f>
-        <v>0.99997384109344112</v>
+        <v>0.99997797144710843</v>
       </c>
       <c r="W2">
         <f>Data!AD17</f>
-        <v>0.99998764322795686</v>
+        <v>0.99998959429722678</v>
       </c>
       <c r="X2">
         <f>Data!AE17</f>
-        <v>0.99999416303412791</v>
+        <v>0.99999508466031828</v>
       </c>
       <c r="Y2">
         <f>Data!AF17</f>
-        <v>0.99999724280361402</v>
+        <v>0.99999767815041185</v>
       </c>
       <c r="Z2">
         <f>Data!AG17</f>
-        <v>0.99999869759065341</v>
+        <v>0.99999890323423446</v>
       </c>
       <c r="AA2">
         <f>Data!AH17</f>
-        <v>0.99999938478494166</v>
+        <v>0.99999948192416133</v>
       </c>
       <c r="AB2">
         <f>Data!AI17</f>
-        <v>0.9999997093928843</v>
+        <v>0.99999975527821849</v>
       </c>
       <c r="AC2">
         <f>Data!AJ17</f>
-        <v>0.99999986272689645</v>
+        <v>0.99999988440159693</v>
       </c>
       <c r="AD2">
         <f>Data!AK17</f>
-        <v>0.99999993515677243</v>
+        <v>0.99999994539517689</v>
       </c>
       <c r="AE2">
         <f>Data!AL17</f>
-        <v>0.99999996937022695</v>
+        <v>0.99999997420650688</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.35">
@@ -10267,115 +9215,115 @@
       </c>
       <c r="D2">
         <f>Data!K24</f>
-        <v>0.60036442047776029</v>
+        <v>0.60439477705223721</v>
       </c>
       <c r="E2">
         <f>Data!L24</f>
-        <v>0.6006004729026948</v>
+        <v>0.60919094796401019</v>
       </c>
       <c r="F2">
         <f>Data!M24</f>
-        <v>0.60098904926265384</v>
+        <v>0.61897034927102668</v>
       </c>
       <c r="G2">
         <f>Data!N24</f>
-        <v>0.60162805508635842</v>
+        <v>0.63813978595964382</v>
       </c>
       <c r="H2">
         <f>Data!O24</f>
-        <v>0.60267714036971387</v>
+        <v>0.6729702095225425</v>
       </c>
       <c r="I2">
         <f>Data!P24</f>
-        <v>0.60439477705223721</v>
+        <v>0.72832852032984285</v>
       </c>
       <c r="J2">
         <f>Data!Q24</f>
-        <v>0.60719448398483655</v>
+        <v>0.8</v>
       </c>
       <c r="K2">
         <f>Data!R24</f>
-        <v>0.6117248923005425</v>
+        <v>0.87167147967015723</v>
       </c>
       <c r="L2">
         <f>Data!S24</f>
-        <v>0.61897034927102668</v>
+        <v>0.92702979047745737</v>
       </c>
       <c r="M2">
         <f>Data!T24</f>
-        <v>0.63034327200849738</v>
+        <v>0.96186021404035627</v>
       </c>
       <c r="N2">
         <f>Data!U24</f>
-        <v>0.64768116880884696</v>
+        <v>0.9810296507289733</v>
       </c>
       <c r="O2">
         <f>Data!V24</f>
-        <v>0.6729702095225425</v>
+        <v>0.99080905203598979</v>
       </c>
       <c r="P2">
         <f>Data!W24</f>
-        <v>0.707576568547998</v>
+        <v>0.99560522294776277</v>
       </c>
       <c r="Q2">
         <f>Data!X24</f>
-        <v>0.75101626751925821</v>
+        <v>0.99791194972257657</v>
       </c>
       <c r="R2">
         <f>Data!Y24</f>
-        <v>0.8</v>
+        <v>0.99901095073734614</v>
       </c>
       <c r="S2">
         <f>Data!Z24</f>
-        <v>0.84898373248074188</v>
+        <v>0.99953219589397779</v>
       </c>
       <c r="T2">
         <f>Data!AA24</f>
-        <v>0.89242343145200187</v>
+        <v>0.99977888854523056</v>
       </c>
       <c r="U2">
         <f>Data!AB24</f>
-        <v>0.92702979047745737</v>
+        <v>0.99989552387236169</v>
       </c>
       <c r="V2">
         <f>Data!AC24</f>
-        <v>0.95231883119115301</v>
+        <v>0.9999506421696055</v>
       </c>
       <c r="W2">
         <f>Data!AD24</f>
-        <v>0.9696567279915026</v>
+        <v>0.99997668349373559</v>
       </c>
       <c r="X2">
         <f>Data!AE24</f>
-        <v>0.9810296507289733</v>
+        <v>0.99998898572355421</v>
       </c>
       <c r="Y2">
         <f>Data!AF24</f>
-        <v>0.98827510769945737</v>
+        <v>0.99999479714861339</v>
       </c>
       <c r="Z2">
         <f>Data!AG24</f>
-        <v>0.99280551601516343</v>
+        <v>0.99999754233015903</v>
       </c>
       <c r="AA2">
         <f>Data!AH24</f>
-        <v>0.99560522294776277</v>
+        <v>0.99999883907520593</v>
       </c>
       <c r="AB2">
         <f>Data!AI24</f>
-        <v>0.99732285963028611</v>
+        <v>0.99999945161711723</v>
       </c>
       <c r="AC2">
         <f>Data!AJ24</f>
-        <v>0.99837194491364156</v>
+        <v>0.99999974096208066</v>
       </c>
       <c r="AD2">
         <f>Data!AK24</f>
-        <v>0.99901095073734614</v>
+        <v>0.99999987763910925</v>
       </c>
       <c r="AE2">
         <f>Data!AL24</f>
-        <v>0.99939952709730528</v>
+        <v>0.99999994220079846</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.35">
@@ -11655,123 +10603,123 @@
       </c>
       <c r="B5">
         <f>Data!I34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="C5">
         <f>Data!J34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="D5">
         <f>Data!K34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E5">
         <f>Data!L34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="F5">
         <f>Data!M34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="G5">
         <f>Data!N34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="H5">
         <f>Data!O34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="I5">
         <f>Data!P34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="J5">
         <f>Data!Q34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="K5">
         <f>Data!R34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="L5">
         <f>Data!S34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="M5">
         <f>Data!T34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="N5">
         <f>Data!U34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="O5">
         <f>Data!V34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="P5">
         <f>Data!W34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="Q5">
         <f>Data!X34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="R5">
         <f>Data!Y34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="S5">
         <f>Data!Z34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="T5">
         <f>Data!AA34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="U5">
         <f>Data!AB34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="V5">
         <f>Data!AC34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="W5">
         <f>Data!AD34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="X5">
         <f>Data!AE34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="Y5">
         <f>Data!AF34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="Z5">
         <f>Data!AG34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AA5">
         <f>Data!AH34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AB5">
         <f>Data!AI34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AC5">
         <f>Data!AJ34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AD5">
         <f>Data!AK34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AE5">
         <f>Data!AL34</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.35">
@@ -12030,123 +10978,123 @@
       </c>
       <c r="B8">
         <f>Data!I37</f>
-        <v>0.2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="C8">
         <f>Data!J37</f>
-        <v>0.20147740316932733</v>
+        <v>7.6108052376995472E-2</v>
       </c>
       <c r="D8">
         <f>Data!K37</f>
-        <v>0.20198403057340777</v>
+        <v>7.6488022930055813E-2</v>
       </c>
       <c r="E8">
         <f>Data!L37</f>
-        <v>0.2026596993576866</v>
+        <v>7.6994774518264933E-2</v>
       </c>
       <c r="F8">
         <f>Data!M37</f>
-        <v>0.20355711892726364</v>
+        <v>7.7667839195447716E-2</v>
       </c>
       <c r="G8">
         <f>Data!N37</f>
-        <v>0.20474258731775669</v>
+        <v>7.8556940488317503E-2</v>
       </c>
       <c r="H8">
         <f>Data!O37</f>
-        <v>0.20629733560569966</v>
+        <v>7.9723001704274737E-2</v>
       </c>
       <c r="I8">
         <f>Data!P37</f>
-        <v>0.20831726964939223</v>
+        <v>8.1237952237044178E-2</v>
       </c>
       <c r="J8">
         <f>Data!Q37</f>
-        <v>0.21090968211956129</v>
+        <v>8.3182261589670958E-2</v>
       </c>
       <c r="K8">
         <f>Data!R37</f>
-        <v>0.21418510649004879</v>
+        <v>8.5638829867536584E-2</v>
       </c>
       <c r="L8">
         <f>Data!S37</f>
-        <v>0.21824255238063564</v>
+        <v>8.8681914285476726E-2</v>
       </c>
       <c r="M8">
         <f>Data!T37</f>
-        <v>0.22314752165009824</v>
+        <v>9.2360641237573676E-2</v>
       </c>
       <c r="N8">
         <f>Data!U37</f>
-        <v>0.22890504973749962</v>
+        <v>9.6678787303124708E-2</v>
       </c>
       <c r="O8">
         <f>Data!V37</f>
-        <v>0.23543436937742046</v>
+        <v>0.10157577703306533</v>
       </c>
       <c r="P8">
         <f>Data!W37</f>
-        <v>0.24255574831883409</v>
+        <v>0.10691681123912558</v>
       </c>
       <c r="Q8">
         <f>Data!X37</f>
-        <v>0.25</v>
+        <v>0.11249999999999999</v>
       </c>
       <c r="R8">
         <f>Data!Y37</f>
-        <v>0.25744425168116591</v>
+        <v>0.11808318876087442</v>
       </c>
       <c r="S8">
         <f>Data!Z37</f>
-        <v>0.26456563062257954</v>
+        <v>0.12342422296693464</v>
       </c>
       <c r="T8">
         <f>Data!AA37</f>
-        <v>0.27109495026250041</v>
+        <v>0.1283212126968753</v>
       </c>
       <c r="U8">
         <f>Data!AB37</f>
-        <v>0.27685247834990179</v>
+        <v>0.13263935876242633</v>
       </c>
       <c r="V8">
         <f>Data!AC37</f>
-        <v>0.28175744761936439</v>
+        <v>0.13631808571452325</v>
       </c>
       <c r="W8">
         <f>Data!AD37</f>
-        <v>0.28581489350995121</v>
+        <v>0.13936117013246341</v>
       </c>
       <c r="X8">
         <f>Data!AE37</f>
-        <v>0.28909031788043871</v>
+        <v>0.14181773841032902</v>
       </c>
       <c r="Y8">
         <f>Data!AF37</f>
-        <v>0.29168273035060777</v>
+        <v>0.14376204776295581</v>
       </c>
       <c r="Z8">
         <f>Data!AG37</f>
-        <v>0.29370266439430037</v>
+        <v>0.14527699829572527</v>
       </c>
       <c r="AA8">
         <f>Data!AH37</f>
-        <v>0.29525741268224331</v>
+        <v>0.14644305951168249</v>
       </c>
       <c r="AB8">
         <f>Data!AI37</f>
-        <v>0.29644288107273636</v>
+        <v>0.1473321608045523</v>
       </c>
       <c r="AC8">
         <f>Data!AJ37</f>
-        <v>0.29734030064231343</v>
+        <v>0.14800522548173506</v>
       </c>
       <c r="AD8">
         <f>Data!AK37</f>
-        <v>0.29801596942659225</v>
+        <v>0.14851197706994418</v>
       </c>
       <c r="AE8">
         <f>Data!AL37</f>
-        <v>0.29852259683067267</v>
+        <v>0.14889194762300451</v>
       </c>
     </row>
   </sheetData>
@@ -56660,8 +55608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AE136"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61:AE68"/>
+    <sheetView topLeftCell="A90" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:XFD138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -63460,8 +62408,8 @@
   </sheetPr>
   <dimension ref="A1:AL93"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24:AL24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -64715,7 +63663,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="22">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F17">
         <f>F10</f>
@@ -64727,123 +63675,123 @@
       </c>
       <c r="I17" s="22">
         <f t="shared" si="1"/>
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="J17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:J$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,J$9))</f>
-        <v>7.1828501414524334E-2</v>
+        <v>0.21838189592802051</v>
       </c>
       <c r="K17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:K$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,K$9))</f>
-        <v>9.505457951868844E-2</v>
+        <v>0.23794069854205344</v>
       </c>
       <c r="L17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:L$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,L$9))</f>
-        <v>0.14058199165415403</v>
+        <v>0.27627957191928759</v>
       </c>
       <c r="M17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:M$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,M$9))</f>
-        <v>0.22330424761603851</v>
+        <v>0.3459404190450851</v>
       </c>
       <c r="N17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:N$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,N$9))</f>
-        <v>0.35478023578337664</v>
+        <v>0.45665704065968565</v>
       </c>
       <c r="O17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:O$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,O$9))</f>
-        <v>0.52500000000000002</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="P17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:P$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,P$9))</f>
-        <v>0.69521976421662335</v>
+        <v>0.74334295934031447</v>
       </c>
       <c r="Q17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:Q$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,Q$9))</f>
-        <v>0.82669575238396142</v>
+        <v>0.85405958095491497</v>
       </c>
       <c r="R17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:R$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,R$9))</f>
-        <v>0.90941800834584607</v>
+        <v>0.92372042808071253</v>
       </c>
       <c r="S17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:S$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,S$9))</f>
-        <v>0.9549454204813117</v>
+        <v>0.9620593014579466</v>
       </c>
       <c r="T17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:T$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,T$9))</f>
-        <v>0.97817149858547559</v>
+        <v>0.98161810407197958</v>
       </c>
       <c r="U17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:U$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,U$9))</f>
-        <v>0.98956240450093647</v>
+        <v>0.99121044589552554</v>
       </c>
       <c r="V17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:V$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,V$9))</f>
-        <v>0.9950408805911195</v>
+        <v>0.99582389944515337</v>
       </c>
       <c r="W17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:W$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,W$9))</f>
-        <v>0.9976510080011971</v>
+        <v>0.99802190147469227</v>
       </c>
       <c r="X17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:X$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,X$9))</f>
-        <v>0.99888896524819726</v>
+        <v>0.99906439178795559</v>
       </c>
       <c r="Y17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:Y$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,Y$9))</f>
-        <v>0.99947486029492261</v>
+        <v>0.99955777709046112</v>
       </c>
       <c r="Z17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:Z$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,Z$9))</f>
-        <v>0.9997518691968591</v>
+        <v>0.9997910477447236</v>
       </c>
       <c r="AA17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:AA$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,AA$9))</f>
-        <v>0.99988277515281299</v>
+        <v>0.99990128433921099</v>
       </c>
       <c r="AB17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:AB$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,AB$9))</f>
-        <v>0.9999446232976219</v>
+        <v>0.99995336698747117</v>
       </c>
       <c r="AC17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:AC$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,AC$9))</f>
-        <v>0.99997384109344112</v>
+        <v>0.99997797144710843</v>
       </c>
       <c r="AD17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:AD$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,AD$9))</f>
-        <v>0.99998764322795686</v>
+        <v>0.99998959429722678</v>
       </c>
       <c r="AE17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:AE$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,AE$9))</f>
-        <v>0.99999416303412791</v>
+        <v>0.99999508466031828</v>
       </c>
       <c r="AF17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:AF$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,AF$9))</f>
-        <v>0.99999724280361402</v>
+        <v>0.99999767815041185</v>
       </c>
       <c r="AG17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:AG$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,AG$9))</f>
-        <v>0.99999869759065341</v>
+        <v>0.99999890323423446</v>
       </c>
       <c r="AH17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:AH$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,AH$9))</f>
-        <v>0.99999938478494166</v>
+        <v>0.99999948192416133</v>
       </c>
       <c r="AI17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:AI$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,AI$9))</f>
-        <v>0.9999997093928843</v>
+        <v>0.99999975527821849</v>
       </c>
       <c r="AJ17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:AJ$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,AJ$9))</f>
-        <v>0.99999986272689645</v>
+        <v>0.99999988440159693</v>
       </c>
       <c r="AK17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:AK$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,AK$9))</f>
-        <v>0.99999993515677243</v>
+        <v>0.99999994539517689</v>
       </c>
       <c r="AL17">
         <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:AL$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,AL$9))</f>
-        <v>0.99999996937022695</v>
+        <v>0.99999997420650688</v>
       </c>
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.35">
@@ -65698,116 +64646,116 @@
         <v>0.6</v>
       </c>
       <c r="K24">
-        <f>IF($G24="s-curve",$E24+($F24-$E24)*$R$2/(1+EXP($R$3*(COUNT($K$9:K$9)+$R$4))),TREND($E24:$F24,$E$9:$F$9,K$9))</f>
-        <v>0.60036442047776029</v>
+        <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($K$9:K$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,K$9))</f>
+        <v>0.60439477705223721</v>
       </c>
       <c r="L24">
-        <f>IF($G24="s-curve",$E24+($F24-$E24)*$R$2/(1+EXP($R$3*(COUNT($K$9:L$9)+$R$4))),TREND($E24:$F24,$E$9:$F$9,L$9))</f>
-        <v>0.6006004729026948</v>
+        <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($K$9:L$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,L$9))</f>
+        <v>0.60919094796401019</v>
       </c>
       <c r="M24">
-        <f>IF($G24="s-curve",$E24+($F24-$E24)*$R$2/(1+EXP($R$3*(COUNT($K$9:M$9)+$R$4))),TREND($E24:$F24,$E$9:$F$9,M$9))</f>
-        <v>0.60098904926265384</v>
+        <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($K$9:M$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,M$9))</f>
+        <v>0.61897034927102668</v>
       </c>
       <c r="N24">
-        <f>IF($G24="s-curve",$E24+($F24-$E24)*$R$2/(1+EXP($R$3*(COUNT($K$9:N$9)+$R$4))),TREND($E24:$F24,$E$9:$F$9,N$9))</f>
-        <v>0.60162805508635842</v>
+        <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($K$9:N$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,N$9))</f>
+        <v>0.63813978595964382</v>
       </c>
       <c r="O24">
-        <f>IF($G24="s-curve",$E24+($F24-$E24)*$R$2/(1+EXP($R$3*(COUNT($K$9:O$9)+$R$4))),TREND($E24:$F24,$E$9:$F$9,O$9))</f>
-        <v>0.60267714036971387</v>
+        <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($K$9:O$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,O$9))</f>
+        <v>0.6729702095225425</v>
       </c>
       <c r="P24">
-        <f>IF($G24="s-curve",$E24+($F24-$E24)*$R$2/(1+EXP($R$3*(COUNT($K$9:P$9)+$R$4))),TREND($E24:$F24,$E$9:$F$9,P$9))</f>
-        <v>0.60439477705223721</v>
+        <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($K$9:P$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,P$9))</f>
+        <v>0.72832852032984285</v>
       </c>
       <c r="Q24">
-        <f>IF($G24="s-curve",$E24+($F24-$E24)*$R$2/(1+EXP($R$3*(COUNT($K$9:Q$9)+$R$4))),TREND($E24:$F24,$E$9:$F$9,Q$9))</f>
-        <v>0.60719448398483655</v>
+        <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($K$9:Q$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,Q$9))</f>
+        <v>0.8</v>
       </c>
       <c r="R24">
-        <f>IF($G24="s-curve",$E24+($F24-$E24)*$R$2/(1+EXP($R$3*(COUNT($K$9:R$9)+$R$4))),TREND($E24:$F24,$E$9:$F$9,R$9))</f>
-        <v>0.6117248923005425</v>
+        <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($K$9:R$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,R$9))</f>
+        <v>0.87167147967015723</v>
       </c>
       <c r="S24">
-        <f>IF($G24="s-curve",$E24+($F24-$E24)*$R$2/(1+EXP($R$3*(COUNT($K$9:S$9)+$R$4))),TREND($E24:$F24,$E$9:$F$9,S$9))</f>
-        <v>0.61897034927102668</v>
+        <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($K$9:S$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,S$9))</f>
+        <v>0.92702979047745737</v>
       </c>
       <c r="T24">
-        <f>IF($G24="s-curve",$E24+($F24-$E24)*$R$2/(1+EXP($R$3*(COUNT($K$9:T$9)+$R$4))),TREND($E24:$F24,$E$9:$F$9,T$9))</f>
-        <v>0.63034327200849738</v>
+        <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($K$9:T$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,T$9))</f>
+        <v>0.96186021404035627</v>
       </c>
       <c r="U24">
-        <f>IF($G24="s-curve",$E24+($F24-$E24)*$R$2/(1+EXP($R$3*(COUNT($K$9:U$9)+$R$4))),TREND($E24:$F24,$E$9:$F$9,U$9))</f>
-        <v>0.64768116880884696</v>
+        <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($K$9:U$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,U$9))</f>
+        <v>0.9810296507289733</v>
       </c>
       <c r="V24">
-        <f>IF($G24="s-curve",$E24+($F24-$E24)*$R$2/(1+EXP($R$3*(COUNT($K$9:V$9)+$R$4))),TREND($E24:$F24,$E$9:$F$9,V$9))</f>
-        <v>0.6729702095225425</v>
+        <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($K$9:V$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,V$9))</f>
+        <v>0.99080905203598979</v>
       </c>
       <c r="W24">
-        <f>IF($G24="s-curve",$E24+($F24-$E24)*$R$2/(1+EXP($R$3*(COUNT($K$9:W$9)+$R$4))),TREND($E24:$F24,$E$9:$F$9,W$9))</f>
-        <v>0.707576568547998</v>
+        <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($K$9:W$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,W$9))</f>
+        <v>0.99560522294776277</v>
       </c>
       <c r="X24">
-        <f>IF($G24="s-curve",$E24+($F24-$E24)*$R$2/(1+EXP($R$3*(COUNT($K$9:X$9)+$R$4))),TREND($E24:$F24,$E$9:$F$9,X$9))</f>
-        <v>0.75101626751925821</v>
+        <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($K$9:X$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,X$9))</f>
+        <v>0.99791194972257657</v>
       </c>
       <c r="Y24">
-        <f>IF($G24="s-curve",$E24+($F24-$E24)*$R$2/(1+EXP($R$3*(COUNT($K$9:Y$9)+$R$4))),TREND($E24:$F24,$E$9:$F$9,Y$9))</f>
-        <v>0.8</v>
+        <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($K$9:Y$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,Y$9))</f>
+        <v>0.99901095073734614</v>
       </c>
       <c r="Z24">
-        <f>IF($G24="s-curve",$E24+($F24-$E24)*$R$2/(1+EXP($R$3*(COUNT($K$9:Z$9)+$R$4))),TREND($E24:$F24,$E$9:$F$9,Z$9))</f>
-        <v>0.84898373248074188</v>
+        <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($K$9:Z$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,Z$9))</f>
+        <v>0.99953219589397779</v>
       </c>
       <c r="AA24">
-        <f>IF($G24="s-curve",$E24+($F24-$E24)*$R$2/(1+EXP($R$3*(COUNT($K$9:AA$9)+$R$4))),TREND($E24:$F24,$E$9:$F$9,AA$9))</f>
-        <v>0.89242343145200187</v>
+        <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($K$9:AA$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,AA$9))</f>
+        <v>0.99977888854523056</v>
       </c>
       <c r="AB24">
-        <f>IF($G24="s-curve",$E24+($F24-$E24)*$R$2/(1+EXP($R$3*(COUNT($K$9:AB$9)+$R$4))),TREND($E24:$F24,$E$9:$F$9,AB$9))</f>
-        <v>0.92702979047745737</v>
+        <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($K$9:AB$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,AB$9))</f>
+        <v>0.99989552387236169</v>
       </c>
       <c r="AC24">
-        <f>IF($G24="s-curve",$E24+($F24-$E24)*$R$2/(1+EXP($R$3*(COUNT($K$9:AC$9)+$R$4))),TREND($E24:$F24,$E$9:$F$9,AC$9))</f>
-        <v>0.95231883119115301</v>
+        <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($K$9:AC$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,AC$9))</f>
+        <v>0.9999506421696055</v>
       </c>
       <c r="AD24">
-        <f>IF($G24="s-curve",$E24+($F24-$E24)*$R$2/(1+EXP($R$3*(COUNT($K$9:AD$9)+$R$4))),TREND($E24:$F24,$E$9:$F$9,AD$9))</f>
-        <v>0.9696567279915026</v>
+        <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($K$9:AD$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,AD$9))</f>
+        <v>0.99997668349373559</v>
       </c>
       <c r="AE24">
-        <f>IF($G24="s-curve",$E24+($F24-$E24)*$R$2/(1+EXP($R$3*(COUNT($K$9:AE$9)+$R$4))),TREND($E24:$F24,$E$9:$F$9,AE$9))</f>
-        <v>0.9810296507289733</v>
+        <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($K$9:AE$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,AE$9))</f>
+        <v>0.99998898572355421</v>
       </c>
       <c r="AF24">
-        <f>IF($G24="s-curve",$E24+($F24-$E24)*$R$2/(1+EXP($R$3*(COUNT($K$9:AF$9)+$R$4))),TREND($E24:$F24,$E$9:$F$9,AF$9))</f>
-        <v>0.98827510769945737</v>
+        <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($K$9:AF$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,AF$9))</f>
+        <v>0.99999479714861339</v>
       </c>
       <c r="AG24">
-        <f>IF($G24="s-curve",$E24+($F24-$E24)*$R$2/(1+EXP($R$3*(COUNT($K$9:AG$9)+$R$4))),TREND($E24:$F24,$E$9:$F$9,AG$9))</f>
-        <v>0.99280551601516343</v>
+        <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($K$9:AG$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,AG$9))</f>
+        <v>0.99999754233015903</v>
       </c>
       <c r="AH24">
-        <f>IF($G24="s-curve",$E24+($F24-$E24)*$R$2/(1+EXP($R$3*(COUNT($K$9:AH$9)+$R$4))),TREND($E24:$F24,$E$9:$F$9,AH$9))</f>
-        <v>0.99560522294776277</v>
+        <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($K$9:AH$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,AH$9))</f>
+        <v>0.99999883907520593</v>
       </c>
       <c r="AI24">
-        <f>IF($G24="s-curve",$E24+($F24-$E24)*$R$2/(1+EXP($R$3*(COUNT($K$9:AI$9)+$R$4))),TREND($E24:$F24,$E$9:$F$9,AI$9))</f>
-        <v>0.99732285963028611</v>
+        <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($K$9:AI$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,AI$9))</f>
+        <v>0.99999945161711723</v>
       </c>
       <c r="AJ24">
-        <f>IF($G24="s-curve",$E24+($F24-$E24)*$R$2/(1+EXP($R$3*(COUNT($K$9:AJ$9)+$R$4))),TREND($E24:$F24,$E$9:$F$9,AJ$9))</f>
-        <v>0.99837194491364156</v>
+        <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($K$9:AJ$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,AJ$9))</f>
+        <v>0.99999974096208066</v>
       </c>
       <c r="AK24">
-        <f>IF($G24="s-curve",$E24+($F24-$E24)*$R$2/(1+EXP($R$3*(COUNT($K$9:AK$9)+$R$4))),TREND($E24:$F24,$E$9:$F$9,AK$9))</f>
-        <v>0.99901095073734614</v>
+        <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($K$9:AK$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,AK$9))</f>
+        <v>0.99999987763910925</v>
       </c>
       <c r="AL24">
-        <f>IF($G24="s-curve",$E24+($F24-$E24)*$R$2/(1+EXP($R$3*(COUNT($K$9:AL$9)+$R$4))),TREND($E24:$F24,$E$9:$F$9,AL$9))</f>
-        <v>0.99939952709730528</v>
+        <f>IF($G24="s-curve",$E24+($F24-$E24)*$O$2/(1+EXP($O$3*(COUNT($K$9:AL$9)+$O$4))),TREND($E24:$F24,$E$9:$F$9,AL$9))</f>
+        <v>0.99999994220079846</v>
       </c>
     </row>
     <row r="25" spans="1:38" x14ac:dyDescent="0.35">
@@ -67050,10 +65998,10 @@
         <v>4</v>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="F34">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="G34" s="7" t="str">
         <f>IF(E34=F34,"n/a",IF(OR(C34="battery electric vehicle",C34="natural gas vehicle",C34="plugin hybrid vehicle"),"s-curve","linear"))</f>
@@ -67061,123 +66009,123 @@
       </c>
       <c r="I34" s="22">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="J34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:J$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,J$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="K34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:K$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,K$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="L34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:L$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,L$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="M34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:M$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,M$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="N34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:N$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,N$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="O34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:O$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,O$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="P34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:P$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,P$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="Q34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:Q$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,Q$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="R34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:R$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,R$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="S34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:S$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,S$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="T34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:T$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,T$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="U34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:U$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,U$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="V34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:V$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,V$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="W34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:W$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,W$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="X34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:X$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,X$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="Y34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:Y$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,Y$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="Z34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:Z$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,Z$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AA34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:AA$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,AA$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AB34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:AB$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,AB$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AC34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:AC$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,AC$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AD34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:AD$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,AD$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AE34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:AE$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,AE$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AF34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:AF$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,AF$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AG34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:AG$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,AG$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AH34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:AH$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,AH$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AI34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:AI$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,AI$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AJ34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:AJ$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,AJ$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AK34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:AK$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,AK$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="AL34">
         <f>IF($G34="s-curve",$E34+($F34-$E34)*$I$2/(1+EXP($I$3*(COUNT($I$9:AL$9)+$I$4))),TREND($E34:$F34,$E$9:$F$9,AL$9))</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="35" spans="1:38" x14ac:dyDescent="0.35">
@@ -67460,10 +66408,10 @@
       </c>
       <c r="D37" s="23"/>
       <c r="E37" s="26">
-        <v>0.2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="F37" s="26">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="G37" s="8" t="str">
         <f>IF(E37=F37,"n/a",IF(OR(C37="battery electric vehicle",C37="natural gas vehicle",C37="plugin hybrid vehicle",C37="hydrogen vehicle"),"s-curve","linear"))</f>
@@ -67471,123 +66419,123 @@
       </c>
       <c r="I37" s="22">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="J37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:J$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,J$9))</f>
-        <v>0.20147740316932733</v>
+        <v>7.6108052376995472E-2</v>
       </c>
       <c r="K37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:K$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,K$9))</f>
-        <v>0.20198403057340777</v>
+        <v>7.6488022930055813E-2</v>
       </c>
       <c r="L37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:L$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,L$9))</f>
-        <v>0.2026596993576866</v>
+        <v>7.6994774518264933E-2</v>
       </c>
       <c r="M37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:M$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,M$9))</f>
-        <v>0.20355711892726364</v>
+        <v>7.7667839195447716E-2</v>
       </c>
       <c r="N37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:N$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,N$9))</f>
-        <v>0.20474258731775669</v>
+        <v>7.8556940488317503E-2</v>
       </c>
       <c r="O37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:O$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,O$9))</f>
-        <v>0.20629733560569966</v>
+        <v>7.9723001704274737E-2</v>
       </c>
       <c r="P37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:P$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,P$9))</f>
-        <v>0.20831726964939223</v>
+        <v>8.1237952237044178E-2</v>
       </c>
       <c r="Q37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:Q$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,Q$9))</f>
-        <v>0.21090968211956129</v>
+        <v>8.3182261589670958E-2</v>
       </c>
       <c r="R37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:R$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,R$9))</f>
-        <v>0.21418510649004879</v>
+        <v>8.5638829867536584E-2</v>
       </c>
       <c r="S37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:S$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,S$9))</f>
-        <v>0.21824255238063564</v>
+        <v>8.8681914285476726E-2</v>
       </c>
       <c r="T37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:T$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,T$9))</f>
-        <v>0.22314752165009824</v>
+        <v>9.2360641237573676E-2</v>
       </c>
       <c r="U37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:U$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,U$9))</f>
-        <v>0.22890504973749962</v>
+        <v>9.6678787303124708E-2</v>
       </c>
       <c r="V37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:V$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,V$9))</f>
-        <v>0.23543436937742046</v>
+        <v>0.10157577703306533</v>
       </c>
       <c r="W37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:W$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,W$9))</f>
-        <v>0.24255574831883409</v>
+        <v>0.10691681123912558</v>
       </c>
       <c r="X37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:X$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,X$9))</f>
-        <v>0.25</v>
+        <v>0.11249999999999999</v>
       </c>
       <c r="Y37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:Y$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,Y$9))</f>
-        <v>0.25744425168116591</v>
+        <v>0.11808318876087442</v>
       </c>
       <c r="Z37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:Z$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,Z$9))</f>
-        <v>0.26456563062257954</v>
+        <v>0.12342422296693464</v>
       </c>
       <c r="AA37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:AA$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,AA$9))</f>
-        <v>0.27109495026250041</v>
+        <v>0.1283212126968753</v>
       </c>
       <c r="AB37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:AB$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,AB$9))</f>
-        <v>0.27685247834990179</v>
+        <v>0.13263935876242633</v>
       </c>
       <c r="AC37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:AC$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,AC$9))</f>
-        <v>0.28175744761936439</v>
+        <v>0.13631808571452325</v>
       </c>
       <c r="AD37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:AD$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,AD$9))</f>
-        <v>0.28581489350995121</v>
+        <v>0.13936117013246341</v>
       </c>
       <c r="AE37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:AE$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,AE$9))</f>
-        <v>0.28909031788043871</v>
+        <v>0.14181773841032902</v>
       </c>
       <c r="AF37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:AF$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,AF$9))</f>
-        <v>0.29168273035060777</v>
+        <v>0.14376204776295581</v>
       </c>
       <c r="AG37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:AG$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,AG$9))</f>
-        <v>0.29370266439430037</v>
+        <v>0.14527699829572527</v>
       </c>
       <c r="AH37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:AH$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,AH$9))</f>
-        <v>0.29525741268224331</v>
+        <v>0.14644305951168249</v>
       </c>
       <c r="AI37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:AI$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,AI$9))</f>
-        <v>0.29644288107273636</v>
+        <v>0.1473321608045523</v>
       </c>
       <c r="AJ37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:AJ$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,AJ$9))</f>
-        <v>0.29734030064231343</v>
+        <v>0.14800522548173506</v>
       </c>
       <c r="AK37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:AK$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,AK$9))</f>
-        <v>0.29801596942659225</v>
+        <v>0.14851197706994418</v>
       </c>
       <c r="AL37">
         <f>IF($G37="s-curve",$E37+($F37-$E37)*$I$2/(1+EXP($I$3*(COUNT($I$9:AL$9)+$I$4))),TREND($E37:$F37,$E$9:$F$9,AL$9))</f>
-        <v>0.29852259683067267</v>
+        <v>0.14889194762300451</v>
       </c>
     </row>
     <row r="38" spans="1:38" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Realign historical sales shares
</commit_message>
<xml_diff>
--- a/InputData/trans/TTS/Transportation Technology Shareweights.xlsx
+++ b/InputData/trans/TTS/Transportation Technology Shareweights.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\TTS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\trans\TTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBE303B-A634-4BFD-8D3E-1A435B9313D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ADFAEA9-4DE2-4E51-8EC4-8481039509F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -5066,94 +5066,94 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>1.7999999999999999E-2</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.8000000000000001E-2</c:v>
+                  <c:v>6.8000000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>9.9000000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>0.11695001406416487</c:v>
+                  <c:v>0.13550148435693454</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>0.13877269058395222</c:v>
+                  <c:v>0.15686570128597005</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="General">
-                  <c:v>0.16657479699442046</c:v>
+                  <c:v>0.18408372983067212</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
-                  <c:v>0.20137571999690912</c:v>
+                  <c:v>0.21815354100537743</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
-                  <c:v>0.2439885939545019</c:v>
+                  <c:v>0.25987118651848296</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="General">
-                  <c:v>0.2947822959785894</c:v>
+                  <c:v>0.30959779396223247</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
-                  <c:v>0.35342187838502587</c:v>
+                  <c:v>0.36700545236853371</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="General">
-                  <c:v>0.41867144928034067</c:v>
+                  <c:v>0.43088423395932512</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="General">
-                  <c:v>0.4883667872327504</c:v>
+                  <c:v>0.49911538413962542</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="General">
-                  <c:v>0.55963321276724964</c:v>
+                  <c:v>0.56888461586037464</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="General">
-                  <c:v>0.62932855071965943</c:v>
+                  <c:v>0.63711576604067499</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="General">
-                  <c:v>0.69457812161497412</c:v>
+                  <c:v>0.70099454763146607</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="General">
-                  <c:v>0.75321770402141064</c:v>
+                  <c:v>0.75840220603776753</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="General">
-                  <c:v>0.80401140604549803</c:v>
+                  <c:v>0.80812881348151699</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="General">
-                  <c:v>0.84662428000309087</c:v>
+                  <c:v>0.84984645899462241</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="General">
-                  <c:v>0.88142520300557958</c:v>
+                  <c:v>0.88391627016932772</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="General">
-                  <c:v>0.90922730941604779</c:v>
+                  <c:v>0.91113429871403007</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="General">
-                  <c:v>0.9310499859358351</c:v>
+                  <c:v>0.93249851564306541</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="General">
-                  <c:v>0.94794338601042438</c:v>
+                  <c:v>0.94903701235474314</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="General">
-                  <c:v>0.96088110315315733</c:v>
+                  <c:v>0.96170292871716656</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="General">
-                  <c:v>0.97070804589199511</c:v>
+                  <c:v>0.9713234230791381</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="General">
-                  <c:v>0.97812554384565553</c:v>
+                  <c:v>0.97858509124385606</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="General">
-                  <c:v>0.98369792028342729</c:v>
+                  <c:v>0.98404040094974166</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="General">
-                  <c:v>0.98786928331016577</c:v>
+                  <c:v>0.9881241302994479</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="General">
-                  <c:v>0.9909835665099872</c:v>
+                  <c:v>0.99117298738162618</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="General">
-                  <c:v>0.99330402502844461</c:v>
+                  <c:v>0.99344469677154446</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="General">
-                  <c:v>0.99503044033973242</c:v>
+                  <c:v>0.99513484285360354</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8098,11 +8098,11 @@
       </c>
       <c r="B2">
         <f>Data!I10</f>
-        <v>1.7999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="C2">
         <f>Data!J10</f>
-        <v>4.8000000000000001E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="D2">
         <f>Data!K10</f>
@@ -8110,111 +8110,111 @@
       </c>
       <c r="E2">
         <f>Data!L10</f>
-        <v>0.11695001406416487</v>
+        <v>0.13550148435693454</v>
       </c>
       <c r="F2">
         <f>Data!M10</f>
-        <v>0.13877269058395222</v>
+        <v>0.15686570128597005</v>
       </c>
       <c r="G2">
         <f>Data!N10</f>
-        <v>0.16657479699442046</v>
+        <v>0.18408372983067212</v>
       </c>
       <c r="H2">
         <f>Data!O10</f>
-        <v>0.20137571999690912</v>
+        <v>0.21815354100537743</v>
       </c>
       <c r="I2">
         <f>Data!P10</f>
-        <v>0.2439885939545019</v>
+        <v>0.25987118651848296</v>
       </c>
       <c r="J2">
         <f>Data!Q10</f>
-        <v>0.2947822959785894</v>
+        <v>0.30959779396223247</v>
       </c>
       <c r="K2">
         <f>Data!R10</f>
-        <v>0.35342187838502587</v>
+        <v>0.36700545236853371</v>
       </c>
       <c r="L2">
         <f>Data!S10</f>
-        <v>0.41867144928034067</v>
+        <v>0.43088423395932512</v>
       </c>
       <c r="M2">
         <f>Data!T10</f>
-        <v>0.4883667872327504</v>
+        <v>0.49911538413962542</v>
       </c>
       <c r="N2">
         <f>Data!U10</f>
-        <v>0.55963321276724964</v>
+        <v>0.56888461586037464</v>
       </c>
       <c r="O2">
         <f>Data!V10</f>
-        <v>0.62932855071965943</v>
+        <v>0.63711576604067499</v>
       </c>
       <c r="P2">
         <f>Data!W10</f>
-        <v>0.69457812161497412</v>
+        <v>0.70099454763146607</v>
       </c>
       <c r="Q2">
         <f>Data!X10</f>
-        <v>0.75321770402141064</v>
+        <v>0.75840220603776753</v>
       </c>
       <c r="R2">
         <f>Data!Y10</f>
-        <v>0.80401140604549803</v>
+        <v>0.80812881348151699</v>
       </c>
       <c r="S2">
         <f>Data!Z10</f>
-        <v>0.84662428000309087</v>
+        <v>0.84984645899462241</v>
       </c>
       <c r="T2">
         <f>Data!AA10</f>
-        <v>0.88142520300557958</v>
+        <v>0.88391627016932772</v>
       </c>
       <c r="U2">
         <f>Data!AB10</f>
-        <v>0.90922730941604779</v>
+        <v>0.91113429871403007</v>
       </c>
       <c r="V2">
         <f>Data!AC10</f>
-        <v>0.9310499859358351</v>
+        <v>0.93249851564306541</v>
       </c>
       <c r="W2">
         <f>Data!AD10</f>
-        <v>0.94794338601042438</v>
+        <v>0.94903701235474314</v>
       </c>
       <c r="X2">
         <f>Data!AE10</f>
-        <v>0.96088110315315733</v>
+        <v>0.96170292871716656</v>
       </c>
       <c r="Y2">
         <f>Data!AF10</f>
-        <v>0.97070804589199511</v>
+        <v>0.9713234230791381</v>
       </c>
       <c r="Z2">
         <f>Data!AG10</f>
-        <v>0.97812554384565553</v>
+        <v>0.97858509124385606</v>
       </c>
       <c r="AA2">
         <f>Data!AH10</f>
-        <v>0.98369792028342729</v>
+        <v>0.98404040094974166</v>
       </c>
       <c r="AB2">
         <f>Data!AI10</f>
-        <v>0.98786928331016577</v>
+        <v>0.9881241302994479</v>
       </c>
       <c r="AC2">
         <f>Data!AJ10</f>
-        <v>0.9909835665099872</v>
+        <v>0.99117298738162618</v>
       </c>
       <c r="AD2">
         <f>Data!AK10</f>
-        <v>0.99330402502844461</v>
+        <v>0.99344469677154446</v>
       </c>
       <c r="AE2">
         <f>Data!AL10</f>
-        <v>0.99503044033973242</v>
+        <v>0.99513484285360354</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -8598,7 +8598,7 @@
       </c>
       <c r="B6">
         <f>Data!I14</f>
-        <v>4.1999999999999997E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="C6">
         <f>Data!J14</f>
@@ -8606,115 +8606,115 @@
       </c>
       <c r="D6">
         <f>Data!K14</f>
-        <v>1.2004677525762598E-2</v>
+        <v>1.8679140068700261E-2</v>
       </c>
       <c r="E6">
         <f>Data!L14</f>
-        <v>1.3231241043871491E-2</v>
+        <v>2.1949976116990642E-2</v>
       </c>
       <c r="F6">
         <f>Data!M14</f>
-        <v>1.4766575882216582E-2</v>
+        <v>2.6044202352577546E-2</v>
       </c>
       <c r="G6">
         <f>Data!N14</f>
-        <v>1.664655561563979E-2</v>
+        <v>3.1057481641706103E-2</v>
       </c>
       <c r="H6">
         <f>Data!O14</f>
-        <v>1.8887454234349531E-2</v>
+        <v>3.7033211291598749E-2</v>
       </c>
       <c r="I6">
         <f>Data!P14</f>
-        <v>2.1474494634633495E-2</v>
+        <v>4.3931985692355985E-2</v>
       </c>
       <c r="J6">
         <f>Data!Q14</f>
-        <v>2.435315217413268E-2</v>
+        <v>5.1608405797687135E-2</v>
       </c>
       <c r="K6">
         <f>Data!R14</f>
-        <v>2.742794649556252E-2</v>
+        <v>5.9807857321500048E-2</v>
       </c>
       <c r="L6">
         <f>Data!S14</f>
-        <v>3.0572053504437483E-2</v>
+        <v>6.8192142678499934E-2</v>
       </c>
       <c r="M6">
         <f>Data!T14</f>
-        <v>3.3646847825867326E-2</v>
+        <v>7.6391594202312868E-2</v>
       </c>
       <c r="N6">
         <f>Data!U14</f>
-        <v>3.6525505365366501E-2</v>
+        <v>8.406801430764399E-2</v>
       </c>
       <c r="O6">
         <f>Data!V14</f>
-        <v>3.9112545765650472E-2</v>
+        <v>9.0966788708401247E-2</v>
       </c>
       <c r="P6">
         <f>Data!W14</f>
-        <v>4.1353444384360213E-2</v>
+        <v>9.6942518358293872E-2</v>
       </c>
       <c r="Q6">
         <f>Data!X14</f>
-        <v>4.3233424117783421E-2</v>
+        <v>0.10195579764742244</v>
       </c>
       <c r="R6">
         <f>Data!Y14</f>
-        <v>4.4768758956128508E-2</v>
+        <v>0.10605002388300935</v>
       </c>
       <c r="S6">
         <f>Data!Z14</f>
-        <v>4.5995322474237404E-2</v>
+        <v>0.10932085993129972</v>
       </c>
       <c r="T6">
         <f>Data!AA14</f>
-        <v>4.6958087614816256E-2</v>
+        <v>0.11188823363951</v>
       </c>
       <c r="U6">
         <f>Data!AB14</f>
-        <v>4.7703384676930492E-2</v>
+        <v>0.11387569247181462</v>
       </c>
       <c r="V6">
         <f>Data!AC14</f>
-        <v>4.8274166315580479E-2</v>
+        <v>0.11539777684154792</v>
       </c>
       <c r="W6">
         <f>Data!AD14</f>
-        <v>4.8707707906999784E-2</v>
+        <v>0.1165538877519994</v>
       </c>
       <c r="X6">
         <f>Data!AE14</f>
-        <v>4.9034950463778926E-2</v>
+        <v>0.11742653457007712</v>
       </c>
       <c r="Y6">
         <f>Data!AF14</f>
-        <v>4.9280790600739442E-2</v>
+        <v>0.11808210826863849</v>
       </c>
       <c r="Z6">
         <f>Data!AG14</f>
-        <v>4.9464821322507319E-2</v>
+        <v>0.11857285686001948</v>
       </c>
       <c r="AA6">
         <f>Data!AH14</f>
-        <v>4.9602216169558261E-2</v>
+        <v>0.11893924311882201</v>
       </c>
       <c r="AB6">
         <f>Data!AI14</f>
-        <v>4.9704589339490207E-2</v>
+        <v>0.11921223823864052</v>
       </c>
       <c r="AC6">
         <f>Data!AJ14</f>
-        <v>4.9780754720870554E-2</v>
+        <v>0.11941534592232145</v>
       </c>
       <c r="AD6">
         <f>Data!AK14</f>
-        <v>4.9837359055491817E-2</v>
+        <v>0.11956629081464482</v>
       </c>
       <c r="AE6">
         <f>Data!AL14</f>
-        <v>4.9879391575460584E-2</v>
+        <v>0.11967837753456154</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
@@ -9623,119 +9623,119 @@
       </c>
       <c r="C6">
         <f>Data!J21</f>
-        <v>1.0161028688271871E-3</v>
+        <v>2.0502850873563008E-3</v>
       </c>
       <c r="D6">
         <f>Data!K21</f>
-        <v>1.26799010529499E-3</v>
+        <v>2.6568115066804157E-3</v>
       </c>
       <c r="E6">
         <f>Data!L21</f>
-        <v>1.6039220771322887E-3</v>
+        <v>3.4657116275128991E-3</v>
       </c>
       <c r="F6">
         <f>Data!M21</f>
-        <v>2.0501050777206073E-3</v>
+        <v>4.5400883268051397E-3</v>
       </c>
       <c r="G6">
         <f>Data!N21</f>
-        <v>2.6395014554061241E-3</v>
+        <v>5.9593125778357988E-3</v>
       </c>
       <c r="H6">
         <f>Data!O21</f>
-        <v>3.4124980333622964E-3</v>
+        <v>7.820632957352051E-3</v>
       </c>
       <c r="I6">
         <f>Data!P21</f>
-        <v>4.416777707171987E-3</v>
+        <v>1.0238866461746552E-2</v>
       </c>
       <c r="J6">
         <f>Data!Q21</f>
-        <v>5.705684717799993E-3</v>
+        <v>1.3342462201492896E-2</v>
       </c>
       <c r="K6">
         <f>Data!R21</f>
-        <v>7.3341745829285324E-3</v>
+        <v>1.7263749125962676E-2</v>
       </c>
       <c r="L6">
         <f>Data!S21</f>
-        <v>9.3514733398968458E-3</v>
+        <v>2.2121260006341788E-2</v>
       </c>
       <c r="M6">
         <f>Data!T21</f>
-        <v>1.1790147490354473E-2</v>
+        <v>2.7993412645423234E-2</v>
       </c>
       <c r="N6">
         <f>Data!U21</f>
-        <v>1.4652700575996493E-2</v>
+        <v>3.4886235392246209E-2</v>
       </c>
       <c r="O6">
         <f>Data!V21</f>
-        <v>1.7898976373295176E-2</v>
+        <v>4.270303493748949E-2</v>
       </c>
       <c r="P6">
         <f>Data!W21</f>
-        <v>2.1439614812797877E-2</v>
+        <v>5.1228638635981739E-2</v>
       </c>
       <c r="Q6">
         <f>Data!X21</f>
-        <v>2.5140780538215154E-2</v>
+        <v>6.0140780538215151E-2</v>
       </c>
       <c r="R6">
         <f>Data!Y21</f>
-        <v>2.8841946263632432E-2</v>
+        <v>6.9052922440448555E-2</v>
       </c>
       <c r="S6">
         <f>Data!Z21</f>
-        <v>3.2382584703135125E-2</v>
+        <v>7.7578526138940798E-2</v>
       </c>
       <c r="T6">
         <f>Data!AA21</f>
-        <v>3.5628860500433818E-2</v>
+        <v>8.5395325684184079E-2</v>
       </c>
       <c r="U6">
         <f>Data!AB21</f>
-        <v>3.8491413586075836E-2</v>
+        <v>9.2288148431007064E-2</v>
       </c>
       <c r="V6">
         <f>Data!AC21</f>
-        <v>4.0930087736533463E-2</v>
+        <v>9.816030107008851E-2</v>
       </c>
       <c r="W6">
         <f>Data!AD21</f>
-        <v>4.2947386493501785E-2</v>
+        <v>0.10301781195046764</v>
       </c>
       <c r="X6">
         <f>Data!AE21</f>
-        <v>4.457587635863032E-2</v>
+        <v>0.10693909887493741</v>
       </c>
       <c r="Y6">
         <f>Data!AF21</f>
-        <v>4.5864783369258325E-2</v>
+        <v>0.11004269461468376</v>
       </c>
       <c r="Z6">
         <f>Data!AG21</f>
-        <v>4.6869063043068017E-2</v>
+        <v>0.11246092811907826</v>
       </c>
       <c r="AA6">
         <f>Data!AH21</f>
-        <v>4.7642059621024191E-2</v>
+        <v>0.11432224849859451</v>
       </c>
       <c r="AB6">
         <f>Data!AI21</f>
-        <v>4.8231455998709705E-2</v>
+        <v>0.11574147274962517</v>
       </c>
       <c r="AC6">
         <f>Data!AJ21</f>
-        <v>4.8677638999298022E-2</v>
+        <v>0.1168158494489174</v>
       </c>
       <c r="AD6">
         <f>Data!AK21</f>
-        <v>4.9013570971135324E-2</v>
+        <v>0.1176247495697499</v>
       </c>
       <c r="AE6">
         <f>Data!AL21</f>
-        <v>4.9265458207603127E-2</v>
+        <v>0.118231275989074</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
@@ -63339,8 +63339,8 @@
   </sheetPr>
   <dimension ref="A1:AL93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63648,10 +63648,10 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>1.7999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="E10" s="22">
-        <v>4.8000000000000001E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -63662,11 +63662,11 @@
       </c>
       <c r="I10">
         <f>D10</f>
-        <v>1.7999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="J10" s="22">
         <f>E10</f>
-        <v>4.8000000000000001E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="K10" s="22">
         <f>O6</f>
@@ -63674,111 +63674,111 @@
       </c>
       <c r="L10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($K$9:L$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,L$9))</f>
-        <v>0.11695001406416487</v>
+        <v>0.13550148435693454</v>
       </c>
       <c r="M10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($K$9:M$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,M$9))</f>
-        <v>0.13877269058395222</v>
+        <v>0.15686570128597005</v>
       </c>
       <c r="N10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($K$9:N$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,N$9))</f>
-        <v>0.16657479699442046</v>
+        <v>0.18408372983067212</v>
       </c>
       <c r="O10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($K$9:O$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,O$9))</f>
-        <v>0.20137571999690912</v>
+        <v>0.21815354100537743</v>
       </c>
       <c r="P10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($K$9:P$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,P$9))</f>
-        <v>0.2439885939545019</v>
+        <v>0.25987118651848296</v>
       </c>
       <c r="Q10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($K$9:Q$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,Q$9))</f>
-        <v>0.2947822959785894</v>
+        <v>0.30959779396223247</v>
       </c>
       <c r="R10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($K$9:R$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,R$9))</f>
-        <v>0.35342187838502587</v>
+        <v>0.36700545236853371</v>
       </c>
       <c r="S10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($K$9:S$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,S$9))</f>
-        <v>0.41867144928034067</v>
+        <v>0.43088423395932512</v>
       </c>
       <c r="T10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($K$9:T$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,T$9))</f>
-        <v>0.4883667872327504</v>
+        <v>0.49911538413962542</v>
       </c>
       <c r="U10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($K$9:U$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,U$9))</f>
-        <v>0.55963321276724964</v>
+        <v>0.56888461586037464</v>
       </c>
       <c r="V10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($K$9:V$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,V$9))</f>
-        <v>0.62932855071965943</v>
+        <v>0.63711576604067499</v>
       </c>
       <c r="W10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($K$9:W$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,W$9))</f>
-        <v>0.69457812161497412</v>
+        <v>0.70099454763146607</v>
       </c>
       <c r="X10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($K$9:X$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,X$9))</f>
-        <v>0.75321770402141064</v>
+        <v>0.75840220603776753</v>
       </c>
       <c r="Y10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($K$9:Y$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,Y$9))</f>
-        <v>0.80401140604549803</v>
+        <v>0.80812881348151699</v>
       </c>
       <c r="Z10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($K$9:Z$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,Z$9))</f>
-        <v>0.84662428000309087</v>
+        <v>0.84984645899462241</v>
       </c>
       <c r="AA10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($K$9:AA$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,AA$9))</f>
-        <v>0.88142520300557958</v>
+        <v>0.88391627016932772</v>
       </c>
       <c r="AB10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($K$9:AB$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,AB$9))</f>
-        <v>0.90922730941604779</v>
+        <v>0.91113429871403007</v>
       </c>
       <c r="AC10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($K$9:AC$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,AC$9))</f>
-        <v>0.9310499859358351</v>
+        <v>0.93249851564306541</v>
       </c>
       <c r="AD10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($K$9:AD$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,AD$9))</f>
-        <v>0.94794338601042438</v>
+        <v>0.94903701235474314</v>
       </c>
       <c r="AE10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($K$9:AE$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,AE$9))</f>
-        <v>0.96088110315315733</v>
+        <v>0.96170292871716656</v>
       </c>
       <c r="AF10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($K$9:AF$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,AF$9))</f>
-        <v>0.97070804589199511</v>
+        <v>0.9713234230791381</v>
       </c>
       <c r="AG10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($K$9:AG$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,AG$9))</f>
-        <v>0.97812554384565553</v>
+        <v>0.97858509124385606</v>
       </c>
       <c r="AH10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($K$9:AH$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,AH$9))</f>
-        <v>0.98369792028342729</v>
+        <v>0.98404040094974166</v>
       </c>
       <c r="AI10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($K$9:AI$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,AI$9))</f>
-        <v>0.98786928331016577</v>
+        <v>0.9881241302994479</v>
       </c>
       <c r="AJ10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($K$9:AJ$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,AJ$9))</f>
-        <v>0.9909835665099872</v>
+        <v>0.99117298738162618</v>
       </c>
       <c r="AK10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($K$9:AK$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,AK$9))</f>
-        <v>0.99330402502844461</v>
+        <v>0.99344469677154446</v>
       </c>
       <c r="AL10">
         <f>IF($G10="s-curve",$E10+($F10-$E10)*$O$2/(1+EXP($O$3*(COUNT($K$9:AL$9)+$O$4))),TREND($E10:$F10,$E$9:$F$9,AL$9))</f>
-        <v>0.99503044033973242</v>
+        <v>0.99513484285360354</v>
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
@@ -64195,13 +64195,13 @@
         <v>5</v>
       </c>
       <c r="D14">
-        <v>4.1999999999999997E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="E14" s="22">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="F14" s="41">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
       <c r="G14" s="7" t="str">
         <f>IF(E14=F14,"n/a",IF(OR(C14="battery electric vehicle",C14="natural gas vehicle",C14="plugin hybrid vehicle",C14="hydrogen vehicle"),"s-curve","linear"))</f>
@@ -64209,7 +64209,7 @@
       </c>
       <c r="I14">
         <f>D14</f>
-        <v>4.1999999999999997E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="J14">
         <f>E14</f>
@@ -64217,115 +64217,115 @@
       </c>
       <c r="K14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:K$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,K$9))</f>
-        <v>1.2004677525762598E-2</v>
+        <v>1.8679140068700261E-2</v>
       </c>
       <c r="L14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:L$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,L$9))</f>
-        <v>1.3231241043871491E-2</v>
+        <v>2.1949976116990642E-2</v>
       </c>
       <c r="M14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:M$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,M$9))</f>
-        <v>1.4766575882216582E-2</v>
+        <v>2.6044202352577546E-2</v>
       </c>
       <c r="N14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:N$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,N$9))</f>
-        <v>1.664655561563979E-2</v>
+        <v>3.1057481641706103E-2</v>
       </c>
       <c r="O14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:O$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,O$9))</f>
-        <v>1.8887454234349531E-2</v>
+        <v>3.7033211291598749E-2</v>
       </c>
       <c r="P14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:P$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,P$9))</f>
-        <v>2.1474494634633495E-2</v>
+        <v>4.3931985692355985E-2</v>
       </c>
       <c r="Q14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:Q$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,Q$9))</f>
-        <v>2.435315217413268E-2</v>
+        <v>5.1608405797687135E-2</v>
       </c>
       <c r="R14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:R$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,R$9))</f>
-        <v>2.742794649556252E-2</v>
+        <v>5.9807857321500048E-2</v>
       </c>
       <c r="S14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:S$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,S$9))</f>
-        <v>3.0572053504437483E-2</v>
+        <v>6.8192142678499934E-2</v>
       </c>
       <c r="T14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:T$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,T$9))</f>
-        <v>3.3646847825867326E-2</v>
+        <v>7.6391594202312868E-2</v>
       </c>
       <c r="U14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:U$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,U$9))</f>
-        <v>3.6525505365366501E-2</v>
+        <v>8.406801430764399E-2</v>
       </c>
       <c r="V14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:V$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,V$9))</f>
-        <v>3.9112545765650472E-2</v>
+        <v>9.0966788708401247E-2</v>
       </c>
       <c r="W14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:W$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,W$9))</f>
-        <v>4.1353444384360213E-2</v>
+        <v>9.6942518358293872E-2</v>
       </c>
       <c r="X14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:X$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,X$9))</f>
-        <v>4.3233424117783421E-2</v>
+        <v>0.10195579764742244</v>
       </c>
       <c r="Y14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:Y$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,Y$9))</f>
-        <v>4.4768758956128508E-2</v>
+        <v>0.10605002388300935</v>
       </c>
       <c r="Z14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:Z$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,Z$9))</f>
-        <v>4.5995322474237404E-2</v>
+        <v>0.10932085993129972</v>
       </c>
       <c r="AA14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AA$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AA$9))</f>
-        <v>4.6958087614816256E-2</v>
+        <v>0.11188823363951</v>
       </c>
       <c r="AB14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AB$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AB$9))</f>
-        <v>4.7703384676930492E-2</v>
+        <v>0.11387569247181462</v>
       </c>
       <c r="AC14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AC$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AC$9))</f>
-        <v>4.8274166315580479E-2</v>
+        <v>0.11539777684154792</v>
       </c>
       <c r="AD14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AD$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AD$9))</f>
-        <v>4.8707707906999784E-2</v>
+        <v>0.1165538877519994</v>
       </c>
       <c r="AE14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AE$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AE$9))</f>
-        <v>4.9034950463778926E-2</v>
+        <v>0.11742653457007712</v>
       </c>
       <c r="AF14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AF$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AF$9))</f>
-        <v>4.9280790600739442E-2</v>
+        <v>0.11808210826863849</v>
       </c>
       <c r="AG14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AG$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AG$9))</f>
-        <v>4.9464821322507319E-2</v>
+        <v>0.11857285686001948</v>
       </c>
       <c r="AH14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AH$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AH$9))</f>
-        <v>4.9602216169558261E-2</v>
+        <v>0.11893924311882201</v>
       </c>
       <c r="AI14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AI$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AI$9))</f>
-        <v>4.9704589339490207E-2</v>
+        <v>0.11921223823864052</v>
       </c>
       <c r="AJ14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AJ$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AJ$9))</f>
-        <v>4.9780754720870554E-2</v>
+        <v>0.11941534592232145</v>
       </c>
       <c r="AK14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AK$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AK$9))</f>
-        <v>4.9837359055491817E-2</v>
+        <v>0.11956629081464482</v>
       </c>
       <c r="AL14">
         <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AL$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AL$9))</f>
-        <v>4.9879391575460584E-2</v>
+        <v>0.11967837753456154</v>
       </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
@@ -65163,7 +65163,7 @@
       </c>
       <c r="F21" s="22">
         <f>F14</f>
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
       <c r="G21" s="7" t="str">
         <f>IF(E21=F21,"n/a",IF(OR(C21="battery electric vehicle",C21="natural gas vehicle",C21="plugin hybrid vehicle"),"s-curve","linear"))</f>
@@ -65175,119 +65175,119 @@
       </c>
       <c r="J21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:J$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,J$9))</f>
-        <v>1.0161028688271871E-3</v>
+        <v>2.0502850873563008E-3</v>
       </c>
       <c r="K21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:K$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,K$9))</f>
-        <v>1.26799010529499E-3</v>
+        <v>2.6568115066804157E-3</v>
       </c>
       <c r="L21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:L$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,L$9))</f>
-        <v>1.6039220771322887E-3</v>
+        <v>3.4657116275128991E-3</v>
       </c>
       <c r="M21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:M$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,M$9))</f>
-        <v>2.0501050777206073E-3</v>
+        <v>4.5400883268051397E-3</v>
       </c>
       <c r="N21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:N$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,N$9))</f>
-        <v>2.6395014554061241E-3</v>
+        <v>5.9593125778357988E-3</v>
       </c>
       <c r="O21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:O$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,O$9))</f>
-        <v>3.4124980333622964E-3</v>
+        <v>7.820632957352051E-3</v>
       </c>
       <c r="P21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:P$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,P$9))</f>
-        <v>4.416777707171987E-3</v>
+        <v>1.0238866461746552E-2</v>
       </c>
       <c r="Q21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:Q$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,Q$9))</f>
-        <v>5.705684717799993E-3</v>
+        <v>1.3342462201492896E-2</v>
       </c>
       <c r="R21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:R$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,R$9))</f>
-        <v>7.3341745829285324E-3</v>
+        <v>1.7263749125962676E-2</v>
       </c>
       <c r="S21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:S$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,S$9))</f>
-        <v>9.3514733398968458E-3</v>
+        <v>2.2121260006341788E-2</v>
       </c>
       <c r="T21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:T$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,T$9))</f>
-        <v>1.1790147490354473E-2</v>
+        <v>2.7993412645423234E-2</v>
       </c>
       <c r="U21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:U$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,U$9))</f>
-        <v>1.4652700575996493E-2</v>
+        <v>3.4886235392246209E-2</v>
       </c>
       <c r="V21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:V$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,V$9))</f>
-        <v>1.7898976373295176E-2</v>
+        <v>4.270303493748949E-2</v>
       </c>
       <c r="W21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:W$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,W$9))</f>
-        <v>2.1439614812797877E-2</v>
+        <v>5.1228638635981739E-2</v>
       </c>
       <c r="X21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:X$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,X$9))</f>
-        <v>2.5140780538215154E-2</v>
+        <v>6.0140780538215151E-2</v>
       </c>
       <c r="Y21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:Y$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,Y$9))</f>
-        <v>2.8841946263632432E-2</v>
+        <v>6.9052922440448555E-2</v>
       </c>
       <c r="Z21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:Z$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,Z$9))</f>
-        <v>3.2382584703135125E-2</v>
+        <v>7.7578526138940798E-2</v>
       </c>
       <c r="AA21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AA$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AA$9))</f>
-        <v>3.5628860500433818E-2</v>
+        <v>8.5395325684184079E-2</v>
       </c>
       <c r="AB21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AB$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AB$9))</f>
-        <v>3.8491413586075836E-2</v>
+        <v>9.2288148431007064E-2</v>
       </c>
       <c r="AC21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AC$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AC$9))</f>
-        <v>4.0930087736533463E-2</v>
+        <v>9.816030107008851E-2</v>
       </c>
       <c r="AD21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AD$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AD$9))</f>
-        <v>4.2947386493501785E-2</v>
+        <v>0.10301781195046764</v>
       </c>
       <c r="AE21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AE$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AE$9))</f>
-        <v>4.457587635863032E-2</v>
+        <v>0.10693909887493741</v>
       </c>
       <c r="AF21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AF$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AF$9))</f>
-        <v>4.5864783369258325E-2</v>
+        <v>0.11004269461468376</v>
       </c>
       <c r="AG21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AG$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AG$9))</f>
-        <v>4.6869063043068017E-2</v>
+        <v>0.11246092811907826</v>
       </c>
       <c r="AH21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AH$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AH$9))</f>
-        <v>4.7642059621024191E-2</v>
+        <v>0.11432224849859451</v>
       </c>
       <c r="AI21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AI$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AI$9))</f>
-        <v>4.8231455998709705E-2</v>
+        <v>0.11574147274962517</v>
       </c>
       <c r="AJ21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AJ$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AJ$9))</f>
-        <v>4.8677638999298022E-2</v>
+        <v>0.1168158494489174</v>
       </c>
       <c r="AK21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AK$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AK$9))</f>
-        <v>4.9013570971135324E-2</v>
+        <v>0.1176247495697499</v>
       </c>
       <c r="AL21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AL$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AL$9))</f>
-        <v>4.9265458207603127E-2</v>
+        <v>0.118231275989074</v>
       </c>
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add EPA rules for LDVs
</commit_message>
<xml_diff>
--- a/InputData/trans/TTS/Transportation Technology Shareweights.xlsx
+++ b/InputData/trans/TTS/Transportation Technology Shareweights.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\trans\TTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ADFAEA9-4DE2-4E51-8EC4-8481039509F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEC53A5-C5F7-4C86-A85B-F3095DE5179A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1826" uniqueCount="1000">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="1004">
   <si>
     <t>Source:</t>
   </si>
@@ -3051,6 +3051,18 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Sigmoidal Curve Values for PHEV passenger LDV Technologies</t>
+  </si>
+  <si>
+    <t>2027-2032, LDV PHEVs</t>
+  </si>
+  <si>
+    <t>2023, LDV BEVs</t>
+  </si>
+  <si>
+    <t>2033, LDV PHEVs</t>
   </si>
 </sst>
 </file>
@@ -3849,7 +3861,7 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3925,6 +3937,10 @@
     <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="10" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="88">
     <cellStyle name="20% - Accent1" xfId="28" builtinId="30" customBuiltin="1"/>
@@ -5061,10 +5077,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Data!$I$10:$AL$10</c:f>
+              <c:f>Data!$I$10:$AM$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0.02</c:v>
                 </c:pt>
@@ -5161,7 +5177,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2CD7-4B7A-BC10-BFBD94963D9F}"/>
+              <c16:uniqueId val="{00000000-64A9-40DF-B5F6-DC2BB01C190E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5174,11 +5190,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="584510703"/>
-        <c:axId val="589151247"/>
+        <c:axId val="145905919"/>
+        <c:axId val="145909759"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="584510703"/>
+        <c:axId val="145905919"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5220,7 +5236,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="589151247"/>
+        <c:crossAx val="145909759"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5228,7 +5244,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="589151247"/>
+        <c:axId val="145909759"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5279,7 +5295,348 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="584510703"/>
+        <c:crossAx val="145905919"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$I$14:$AL$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>2.5000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8679140068700261E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0151128112044503E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6021242730178792E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.4401430729338323E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.1499999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.5E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.4999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.8999999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.11799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.17702858227261439</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.19652431808271453</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.21198289652972047</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.22359856927066168</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.2319787572698212</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.23784887188795553</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.24187624796588125</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.24460014783483416</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.24642468433022793</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.2476388869188586</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.24844342975100567</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.24897499940691589</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.24932554691499179</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.24955642877591674</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.24970836961542547</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.24980830595850836</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.24987401381406515</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.24991720639498693</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D32E-4CC5-851D-14400ED7F077}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="144440415"/>
+        <c:axId val="144438495"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="144440415"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="144438495"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="144438495"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="144440415"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5416,6 +5773,46 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -7003,6 +7400,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -7084,23 +7997,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>136525</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37611677-E89A-3C1B-D779-903087F49626}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AA4F8C5-6199-A6FD-10AB-7EDD21735E13}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7113,6 +8026,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25FEF526-BD1E-EFFF-D20B-034FBCB5C98A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8610,111 +9559,111 @@
       </c>
       <c r="E6">
         <f>Data!L14</f>
-        <v>2.1949976116990642E-2</v>
+        <v>2.0151128112044503E-2</v>
       </c>
       <c r="F6">
         <f>Data!M14</f>
-        <v>2.6044202352577546E-2</v>
+        <v>2.6021242730178792E-2</v>
       </c>
       <c r="G6">
         <f>Data!N14</f>
-        <v>3.1057481641706103E-2</v>
+        <v>3.4401430729338323E-2</v>
       </c>
       <c r="H6">
         <f>Data!O14</f>
-        <v>3.7033211291598749E-2</v>
+        <v>5.1499999999999997E-2</v>
       </c>
       <c r="I6">
         <f>Data!P14</f>
-        <v>4.3931985692355985E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="J6">
         <f>Data!Q14</f>
-        <v>5.1608405797687135E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="K6">
         <f>Data!R14</f>
-        <v>5.9807857321500048E-2</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="L6">
         <f>Data!S14</f>
-        <v>6.8192142678499934E-2</v>
+        <v>0.11799999999999999</v>
       </c>
       <c r="M6">
         <f>Data!T14</f>
-        <v>7.6391594202312868E-2</v>
+        <v>0.15</v>
       </c>
       <c r="N6">
         <f>Data!U14</f>
-        <v>8.406801430764399E-2</v>
+        <v>0.17702858227261439</v>
       </c>
       <c r="O6">
         <f>Data!V14</f>
-        <v>9.0966788708401247E-2</v>
+        <v>0.19652431808271453</v>
       </c>
       <c r="P6">
         <f>Data!W14</f>
-        <v>9.6942518358293872E-2</v>
+        <v>0.21198289652972047</v>
       </c>
       <c r="Q6">
         <f>Data!X14</f>
-        <v>0.10195579764742244</v>
+        <v>0.22359856927066168</v>
       </c>
       <c r="R6">
         <f>Data!Y14</f>
-        <v>0.10605002388300935</v>
+        <v>0.2319787572698212</v>
       </c>
       <c r="S6">
         <f>Data!Z14</f>
-        <v>0.10932085993129972</v>
+        <v>0.23784887188795553</v>
       </c>
       <c r="T6">
         <f>Data!AA14</f>
-        <v>0.11188823363951</v>
+        <v>0.24187624796588125</v>
       </c>
       <c r="U6">
         <f>Data!AB14</f>
-        <v>0.11387569247181462</v>
+        <v>0.24460014783483416</v>
       </c>
       <c r="V6">
         <f>Data!AC14</f>
-        <v>0.11539777684154792</v>
+        <v>0.24642468433022793</v>
       </c>
       <c r="W6">
         <f>Data!AD14</f>
-        <v>0.1165538877519994</v>
+        <v>0.2476388869188586</v>
       </c>
       <c r="X6">
         <f>Data!AE14</f>
-        <v>0.11742653457007712</v>
+        <v>0.24844342975100567</v>
       </c>
       <c r="Y6">
         <f>Data!AF14</f>
-        <v>0.11808210826863849</v>
+        <v>0.24897499940691589</v>
       </c>
       <c r="Z6">
         <f>Data!AG14</f>
-        <v>0.11857285686001948</v>
+        <v>0.24932554691499179</v>
       </c>
       <c r="AA6">
         <f>Data!AH14</f>
-        <v>0.11893924311882201</v>
+        <v>0.24955642877591674</v>
       </c>
       <c r="AB6">
         <f>Data!AI14</f>
-        <v>0.11921223823864052</v>
+        <v>0.24970836961542547</v>
       </c>
       <c r="AC6">
         <f>Data!AJ14</f>
-        <v>0.11941534592232145</v>
+        <v>0.24980830595850836</v>
       </c>
       <c r="AD6">
         <f>Data!AK14</f>
-        <v>0.11956629081464482</v>
+        <v>0.24987401381406515</v>
       </c>
       <c r="AE6">
         <f>Data!AL14</f>
-        <v>0.11967837753456154</v>
+        <v>0.24991720639498693</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
@@ -9623,119 +10572,119 @@
       </c>
       <c r="C6">
         <f>Data!J21</f>
-        <v>2.0502850873563008E-3</v>
+        <v>3.9709092074817981E-3</v>
       </c>
       <c r="D6">
         <f>Data!K21</f>
-        <v>2.6568115066804157E-3</v>
+        <v>5.2360512521104916E-3</v>
       </c>
       <c r="E6">
         <f>Data!L21</f>
-        <v>3.4657116275128991E-3</v>
+        <v>6.9233207925054616E-3</v>
       </c>
       <c r="F6">
         <f>Data!M21</f>
-        <v>4.5400883268051397E-3</v>
+        <v>9.1643429322478421E-3</v>
       </c>
       <c r="G6">
         <f>Data!N21</f>
-        <v>5.9593125778357988E-3</v>
+        <v>1.2124676090919479E-2</v>
       </c>
       <c r="H6">
         <f>Data!O21</f>
-        <v>7.820632957352051E-3</v>
+        <v>1.6007169244761595E-2</v>
       </c>
       <c r="I6">
         <f>Data!P21</f>
-        <v>1.0238866461746552E-2</v>
+        <v>2.1051317005956457E-2</v>
       </c>
       <c r="J6">
         <f>Data!Q21</f>
-        <v>1.3342462201492896E-2</v>
+        <v>2.7525048956922572E-2</v>
       </c>
       <c r="K6">
         <f>Data!R21</f>
-        <v>1.7263749125962676E-2</v>
+        <v>3.5704387563026088E-2</v>
       </c>
       <c r="L6">
         <f>Data!S21</f>
-        <v>2.2121260006341788E-2</v>
+        <v>4.5836578101168111E-2</v>
       </c>
       <c r="M6">
         <f>Data!T21</f>
-        <v>2.7993412645423234E-2</v>
+        <v>5.8085190790550939E-2</v>
       </c>
       <c r="N6">
         <f>Data!U21</f>
-        <v>3.4886235392246209E-2</v>
+        <v>7.2462800050995702E-2</v>
       </c>
       <c r="O6">
         <f>Data!V21</f>
-        <v>4.270303493748949E-2</v>
+        <v>8.8767715128136082E-2</v>
       </c>
       <c r="P6">
         <f>Data!W21</f>
-        <v>5.1228638635981739E-2</v>
+        <v>0.10655111145046607</v>
       </c>
       <c r="Q6">
         <f>Data!X21</f>
-        <v>6.0140780538215151E-2</v>
+        <v>0.12514078053821515</v>
       </c>
       <c r="R6">
         <f>Data!Y21</f>
-        <v>6.9052922440448555E-2</v>
+        <v>0.14373044962596424</v>
       </c>
       <c r="S6">
         <f>Data!Z21</f>
-        <v>7.7578526138940798E-2</v>
+        <v>0.16151384594829421</v>
       </c>
       <c r="T6">
         <f>Data!AA21</f>
-        <v>8.5395325684184079E-2</v>
+        <v>0.17781876102543459</v>
       </c>
       <c r="U6">
         <f>Data!AB21</f>
-        <v>9.2288148431007064E-2</v>
+        <v>0.19219637028587935</v>
       </c>
       <c r="V6">
         <f>Data!AC21</f>
-        <v>9.816030107008851E-2</v>
+        <v>0.20444498297526217</v>
       </c>
       <c r="W6">
         <f>Data!AD21</f>
-        <v>0.10301781195046764</v>
+        <v>0.21457717351340425</v>
       </c>
       <c r="X6">
         <f>Data!AE21</f>
-        <v>0.10693909887493741</v>
+        <v>0.22275651211950773</v>
       </c>
       <c r="Y6">
         <f>Data!AF21</f>
-        <v>0.11004269461468376</v>
+        <v>0.22923024407047385</v>
       </c>
       <c r="Z6">
         <f>Data!AG21</f>
-        <v>0.11246092811907826</v>
+        <v>0.23427439183166873</v>
       </c>
       <c r="AA6">
         <f>Data!AH21</f>
-        <v>0.11432224849859451</v>
+        <v>0.23815688498551085</v>
       </c>
       <c r="AB6">
         <f>Data!AI21</f>
-        <v>0.11574147274962517</v>
+        <v>0.24111721814418247</v>
       </c>
       <c r="AC6">
         <f>Data!AJ21</f>
-        <v>0.1168158494489174</v>
+        <v>0.24335824028392483</v>
       </c>
       <c r="AD6">
         <f>Data!AK21</f>
-        <v>0.1176247495697499</v>
+        <v>0.24504550982431983</v>
       </c>
       <c r="AE6">
         <f>Data!AL21</f>
-        <v>0.118231275989074</v>
+        <v>0.24631065186894852</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
@@ -63339,8 +64288,8 @@
   </sheetPr>
   <dimension ref="A1:AL93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63353,6 +64302,7 @@
     <col min="6" max="6" width="18" style="7" customWidth="1"/>
     <col min="7" max="7" width="13.140625" customWidth="1"/>
     <col min="8" max="9" width="9.140625" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.25">
@@ -63375,6 +64325,10 @@
         <v>998</v>
       </c>
       <c r="R1" s="17"/>
+      <c r="T1" s="16" t="s">
+        <v>1000</v>
+      </c>
+      <c r="U1" s="17"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -63398,6 +64352,12 @@
       <c r="R2" s="19">
         <v>1</v>
       </c>
+      <c r="T2" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="U2" s="19">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -63421,6 +64381,12 @@
       <c r="R3" s="19">
         <v>-0.5</v>
       </c>
+      <c r="T3" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="U3" s="19">
+        <v>-0.42</v>
+      </c>
     </row>
     <row r="4" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -63443,6 +64409,12 @@
       </c>
       <c r="R4" s="20">
         <v>-15</v>
+      </c>
+      <c r="T4" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="U4" s="20">
+        <v>-11</v>
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
@@ -63464,14 +64436,14 @@
       <c r="G6" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="N6" s="12">
-        <v>2023</v>
+      <c r="N6" s="49" t="s">
+        <v>1002</v>
       </c>
       <c r="O6" s="22">
         <v>9.9000000000000005E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12" t="s">
@@ -63485,6 +64457,12 @@
         <v>2050</v>
       </c>
       <c r="G7" s="2"/>
+      <c r="N7" s="49" t="s">
+        <v>1003</v>
+      </c>
+      <c r="O7">
+        <v>1.8679140068700261E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:38" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
@@ -63496,6 +64474,27 @@
       <c r="G8" s="27" t="s">
         <v>136</v>
       </c>
+      <c r="N8" s="49" t="s">
+        <v>1001</v>
+      </c>
+      <c r="O8">
+        <v>0.05</v>
+      </c>
+      <c r="P8">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="Q8">
+        <v>7.8E-2</v>
+      </c>
+      <c r="R8">
+        <v>0.09</v>
+      </c>
+      <c r="S8">
+        <v>0.12</v>
+      </c>
+      <c r="T8">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
@@ -63660,15 +64659,15 @@
         <f>IF(E10=F10,"n/a",IF(OR(C10="battery electric vehicle",C10="natural gas vehicle",C10="plugin hybrid vehicle"),"s-curve","linear"))</f>
         <v>s-curve</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="15">
         <f>D10</f>
         <v>0.02</v>
       </c>
-      <c r="J10" s="22">
+      <c r="J10" s="50">
         <f>E10</f>
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="K10" s="22">
+      <c r="K10" s="50">
         <f>O6</f>
         <v>9.9000000000000005E-2</v>
       </c>
@@ -64201,131 +65200,126 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="F14" s="41">
-        <v>0.12</v>
+        <v>0.25</v>
       </c>
       <c r="G14" s="7" t="str">
         <f>IF(E14=F14,"n/a",IF(OR(C14="battery electric vehicle",C14="natural gas vehicle",C14="plugin hybrid vehicle",C14="hydrogen vehicle"),"s-curve","linear"))</f>
         <v>s-curve</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="15">
         <f>D14</f>
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="15">
         <f>E14</f>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="K14">
-        <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:K$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,K$9))</f>
+      <c r="K14" s="15">
+        <f>O7</f>
         <v>1.8679140068700261E-2</v>
       </c>
       <c r="L14">
-        <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:L$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,L$9))</f>
-        <v>2.1949976116990642E-2</v>
+        <f>IF($G14="s-curve",$E14+($F14-$E14)*$U$2/(1+EXP($U$3*(COUNT($I$9:L$9)+$U$4))),TREND($E14:$F14,$E$9:$F$9,L$9))</f>
+        <v>2.0151128112044503E-2</v>
       </c>
       <c r="M14">
-        <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:M$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,M$9))</f>
-        <v>2.6044202352577546E-2</v>
+        <f>IF($G14="s-curve",$E14+($F14-$E14)*$U$2/(1+EXP($U$3*(COUNT($I$9:M$9)+$U$4))),TREND($E14:$F14,$E$9:$F$9,M$9))</f>
+        <v>2.6021242730178792E-2</v>
       </c>
       <c r="N14">
-        <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:N$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,N$9))</f>
-        <v>3.1057481641706103E-2</v>
-      </c>
-      <c r="O14">
-        <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:O$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,O$9))</f>
-        <v>3.7033211291598749E-2</v>
-      </c>
-      <c r="P14">
-        <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:P$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,P$9))</f>
-        <v>4.3931985692355985E-2</v>
-      </c>
-      <c r="Q14">
-        <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:Q$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,Q$9))</f>
-        <v>5.1608405797687135E-2</v>
-      </c>
-      <c r="R14">
-        <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:R$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,R$9))</f>
-        <v>5.9807857321500048E-2</v>
-      </c>
-      <c r="S14">
-        <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:S$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,S$9))</f>
-        <v>6.8192142678499934E-2</v>
-      </c>
-      <c r="T14">
-        <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:T$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,T$9))</f>
-        <v>7.6391594202312868E-2</v>
+        <f>IF($G14="s-curve",$E14+($F14-$E14)*$U$2/(1+EXP($U$3*(COUNT($I$9:N$9)+$U$4))),TREND($E14:$F14,$E$9:$F$9,N$9))</f>
+        <v>3.4401430729338323E-2</v>
+      </c>
+      <c r="O14" s="15">
+        <v>5.1499999999999997E-2</v>
+      </c>
+      <c r="P14" s="15">
+        <v>5.5E-2</v>
+      </c>
+      <c r="Q14" s="15">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="R14" s="15">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="S14" s="15">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="T14" s="15">
+        <f t="shared" ref="T14" si="2">T8</f>
+        <v>0.15</v>
       </c>
       <c r="U14">
-        <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:U$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,U$9))</f>
-        <v>8.406801430764399E-2</v>
+        <f>IF($G14="s-curve",$E14+($F14-$E14)*$U$2/(1+EXP($U$3*(COUNT($I$9:U$9)+$U$4))),TREND($E14:$F14,$E$9:$F$9,U$9))</f>
+        <v>0.17702858227261439</v>
       </c>
       <c r="V14">
-        <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:V$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,V$9))</f>
-        <v>9.0966788708401247E-2</v>
+        <f>IF($G14="s-curve",$E14+($F14-$E14)*$U$2/(1+EXP($U$3*(COUNT($I$9:V$9)+$U$4))),TREND($E14:$F14,$E$9:$F$9,V$9))</f>
+        <v>0.19652431808271453</v>
       </c>
       <c r="W14">
-        <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:W$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,W$9))</f>
-        <v>9.6942518358293872E-2</v>
+        <f>IF($G14="s-curve",$E14+($F14-$E14)*$U$2/(1+EXP($U$3*(COUNT($I$9:W$9)+$U$4))),TREND($E14:$F14,$E$9:$F$9,W$9))</f>
+        <v>0.21198289652972047</v>
       </c>
       <c r="X14">
-        <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:X$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,X$9))</f>
-        <v>0.10195579764742244</v>
+        <f>IF($G14="s-curve",$E14+($F14-$E14)*$U$2/(1+EXP($U$3*(COUNT($I$9:X$9)+$U$4))),TREND($E14:$F14,$E$9:$F$9,X$9))</f>
+        <v>0.22359856927066168</v>
       </c>
       <c r="Y14">
-        <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:Y$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,Y$9))</f>
-        <v>0.10605002388300935</v>
+        <f>IF($G14="s-curve",$E14+($F14-$E14)*$U$2/(1+EXP($U$3*(COUNT($I$9:Y$9)+$U$4))),TREND($E14:$F14,$E$9:$F$9,Y$9))</f>
+        <v>0.2319787572698212</v>
       </c>
       <c r="Z14">
-        <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:Z$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,Z$9))</f>
-        <v>0.10932085993129972</v>
+        <f>IF($G14="s-curve",$E14+($F14-$E14)*$U$2/(1+EXP($U$3*(COUNT($I$9:Z$9)+$U$4))),TREND($E14:$F14,$E$9:$F$9,Z$9))</f>
+        <v>0.23784887188795553</v>
       </c>
       <c r="AA14">
-        <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AA$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AA$9))</f>
-        <v>0.11188823363951</v>
+        <f>IF($G14="s-curve",$E14+($F14-$E14)*$U$2/(1+EXP($U$3*(COUNT($I$9:AA$9)+$U$4))),TREND($E14:$F14,$E$9:$F$9,AA$9))</f>
+        <v>0.24187624796588125</v>
       </c>
       <c r="AB14">
-        <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AB$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AB$9))</f>
-        <v>0.11387569247181462</v>
+        <f>IF($G14="s-curve",$E14+($F14-$E14)*$U$2/(1+EXP($U$3*(COUNT($I$9:AB$9)+$U$4))),TREND($E14:$F14,$E$9:$F$9,AB$9))</f>
+        <v>0.24460014783483416</v>
       </c>
       <c r="AC14">
-        <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AC$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AC$9))</f>
-        <v>0.11539777684154792</v>
+        <f>IF($G14="s-curve",$E14+($F14-$E14)*$U$2/(1+EXP($U$3*(COUNT($I$9:AC$9)+$U$4))),TREND($E14:$F14,$E$9:$F$9,AC$9))</f>
+        <v>0.24642468433022793</v>
       </c>
       <c r="AD14">
-        <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AD$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AD$9))</f>
-        <v>0.1165538877519994</v>
+        <f>IF($G14="s-curve",$E14+($F14-$E14)*$U$2/(1+EXP($U$3*(COUNT($I$9:AD$9)+$U$4))),TREND($E14:$F14,$E$9:$F$9,AD$9))</f>
+        <v>0.2476388869188586</v>
       </c>
       <c r="AE14">
-        <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AE$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AE$9))</f>
-        <v>0.11742653457007712</v>
+        <f>IF($G14="s-curve",$E14+($F14-$E14)*$U$2/(1+EXP($U$3*(COUNT($I$9:AE$9)+$U$4))),TREND($E14:$F14,$E$9:$F$9,AE$9))</f>
+        <v>0.24844342975100567</v>
       </c>
       <c r="AF14">
-        <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AF$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AF$9))</f>
-        <v>0.11808210826863849</v>
+        <f>IF($G14="s-curve",$E14+($F14-$E14)*$U$2/(1+EXP($U$3*(COUNT($I$9:AF$9)+$U$4))),TREND($E14:$F14,$E$9:$F$9,AF$9))</f>
+        <v>0.24897499940691589</v>
       </c>
       <c r="AG14">
-        <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AG$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AG$9))</f>
-        <v>0.11857285686001948</v>
+        <f>IF($G14="s-curve",$E14+($F14-$E14)*$U$2/(1+EXP($U$3*(COUNT($I$9:AG$9)+$U$4))),TREND($E14:$F14,$E$9:$F$9,AG$9))</f>
+        <v>0.24932554691499179</v>
       </c>
       <c r="AH14">
-        <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AH$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AH$9))</f>
-        <v>0.11893924311882201</v>
+        <f>IF($G14="s-curve",$E14+($F14-$E14)*$U$2/(1+EXP($U$3*(COUNT($I$9:AH$9)+$U$4))),TREND($E14:$F14,$E$9:$F$9,AH$9))</f>
+        <v>0.24955642877591674</v>
       </c>
       <c r="AI14">
-        <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AI$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AI$9))</f>
-        <v>0.11921223823864052</v>
+        <f>IF($G14="s-curve",$E14+($F14-$E14)*$U$2/(1+EXP($U$3*(COUNT($I$9:AI$9)+$U$4))),TREND($E14:$F14,$E$9:$F$9,AI$9))</f>
+        <v>0.24970836961542547</v>
       </c>
       <c r="AJ14">
-        <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AJ$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AJ$9))</f>
-        <v>0.11941534592232145</v>
+        <f>IF($G14="s-curve",$E14+($F14-$E14)*$U$2/(1+EXP($U$3*(COUNT($I$9:AJ$9)+$U$4))),TREND($E14:$F14,$E$9:$F$9,AJ$9))</f>
+        <v>0.24980830595850836</v>
       </c>
       <c r="AK14">
-        <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AK$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AK$9))</f>
-        <v>0.11956629081464482</v>
+        <f>IF($G14="s-curve",$E14+($F14-$E14)*$U$2/(1+EXP($U$3*(COUNT($I$9:AK$9)+$U$4))),TREND($E14:$F14,$E$9:$F$9,AK$9))</f>
+        <v>0.24987401381406515</v>
       </c>
       <c r="AL14">
-        <f>IF($G14="s-curve",$E14+($F14-$E14)*$O$2/(1+EXP($O$3*(COUNT($I$9:AL$9)+$O$4))),TREND($E14:$F14,$E$9:$F$9,AL$9))</f>
-        <v>0.11967837753456154</v>
+        <f>IF($G14="s-curve",$E14+($F14-$E14)*$U$2/(1+EXP($U$3*(COUNT($I$9:AL$9)+$U$4))),TREND($E14:$F14,$E$9:$F$9,AL$9))</f>
+        <v>0.24991720639498693</v>
       </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
@@ -65163,7 +66157,7 @@
       </c>
       <c r="F21" s="22">
         <f>F14</f>
-        <v>0.12</v>
+        <v>0.25</v>
       </c>
       <c r="G21" s="7" t="str">
         <f>IF(E21=F21,"n/a",IF(OR(C21="battery electric vehicle",C21="natural gas vehicle",C21="plugin hybrid vehicle"),"s-curve","linear"))</f>
@@ -65175,119 +66169,119 @@
       </c>
       <c r="J21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:J$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,J$9))</f>
-        <v>2.0502850873563008E-3</v>
+        <v>3.9709092074817981E-3</v>
       </c>
       <c r="K21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:K$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,K$9))</f>
-        <v>2.6568115066804157E-3</v>
+        <v>5.2360512521104916E-3</v>
       </c>
       <c r="L21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:L$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,L$9))</f>
-        <v>3.4657116275128991E-3</v>
+        <v>6.9233207925054616E-3</v>
       </c>
       <c r="M21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:M$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,M$9))</f>
-        <v>4.5400883268051397E-3</v>
+        <v>9.1643429322478421E-3</v>
       </c>
       <c r="N21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:N$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,N$9))</f>
-        <v>5.9593125778357988E-3</v>
+        <v>1.2124676090919479E-2</v>
       </c>
       <c r="O21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:O$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,O$9))</f>
-        <v>7.820632957352051E-3</v>
+        <v>1.6007169244761595E-2</v>
       </c>
       <c r="P21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:P$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,P$9))</f>
-        <v>1.0238866461746552E-2</v>
+        <v>2.1051317005956457E-2</v>
       </c>
       <c r="Q21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:Q$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,Q$9))</f>
-        <v>1.3342462201492896E-2</v>
+        <v>2.7525048956922572E-2</v>
       </c>
       <c r="R21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:R$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,R$9))</f>
-        <v>1.7263749125962676E-2</v>
+        <v>3.5704387563026088E-2</v>
       </c>
       <c r="S21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:S$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,S$9))</f>
-        <v>2.2121260006341788E-2</v>
+        <v>4.5836578101168111E-2</v>
       </c>
       <c r="T21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:T$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,T$9))</f>
-        <v>2.7993412645423234E-2</v>
+        <v>5.8085190790550939E-2</v>
       </c>
       <c r="U21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:U$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,U$9))</f>
-        <v>3.4886235392246209E-2</v>
+        <v>7.2462800050995702E-2</v>
       </c>
       <c r="V21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:V$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,V$9))</f>
-        <v>4.270303493748949E-2</v>
+        <v>8.8767715128136082E-2</v>
       </c>
       <c r="W21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:W$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,W$9))</f>
-        <v>5.1228638635981739E-2</v>
+        <v>0.10655111145046607</v>
       </c>
       <c r="X21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:X$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,X$9))</f>
-        <v>6.0140780538215151E-2</v>
+        <v>0.12514078053821515</v>
       </c>
       <c r="Y21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:Y$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,Y$9))</f>
-        <v>6.9052922440448555E-2</v>
+        <v>0.14373044962596424</v>
       </c>
       <c r="Z21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:Z$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,Z$9))</f>
-        <v>7.7578526138940798E-2</v>
+        <v>0.16151384594829421</v>
       </c>
       <c r="AA21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AA$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AA$9))</f>
-        <v>8.5395325684184079E-2</v>
+        <v>0.17781876102543459</v>
       </c>
       <c r="AB21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AB$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AB$9))</f>
-        <v>9.2288148431007064E-2</v>
+        <v>0.19219637028587935</v>
       </c>
       <c r="AC21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AC$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AC$9))</f>
-        <v>9.816030107008851E-2</v>
+        <v>0.20444498297526217</v>
       </c>
       <c r="AD21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AD$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AD$9))</f>
-        <v>0.10301781195046764</v>
+        <v>0.21457717351340425</v>
       </c>
       <c r="AE21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AE$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AE$9))</f>
-        <v>0.10693909887493741</v>
+        <v>0.22275651211950773</v>
       </c>
       <c r="AF21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AF$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AF$9))</f>
-        <v>0.11004269461468376</v>
+        <v>0.22923024407047385</v>
       </c>
       <c r="AG21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AG$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AG$9))</f>
-        <v>0.11246092811907826</v>
+        <v>0.23427439183166873</v>
       </c>
       <c r="AH21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AH$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AH$9))</f>
-        <v>0.11432224849859451</v>
+        <v>0.23815688498551085</v>
       </c>
       <c r="AI21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AI$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AI$9))</f>
-        <v>0.11574147274962517</v>
+        <v>0.24111721814418247</v>
       </c>
       <c r="AJ21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AJ$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AJ$9))</f>
-        <v>0.1168158494489174</v>
+        <v>0.24335824028392483</v>
       </c>
       <c r="AK21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AK$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AK$9))</f>
-        <v>0.1176247495697499</v>
+        <v>0.24504550982431983</v>
       </c>
       <c r="AL21">
         <f>IF($G21="s-curve",$E21+($F21-$E21)*$I$2/(1+EXP($I$3*(COUNT($I$9:AL$9)+$I$4))),TREND($E21:$F21,$E$9:$F$9,AL$9))</f>
-        <v>0.118231275989074</v>
+        <v>0.24631065186894852</v>
       </c>
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.25">
@@ -67917,7 +68911,7 @@
         <v>n/a</v>
       </c>
       <c r="I41" s="22">
-        <f t="shared" ref="I41:I72" si="2">E41</f>
+        <f t="shared" ref="I41:I72" si="3">E41</f>
         <v>1</v>
       </c>
       <c r="J41">
@@ -68052,7 +69046,7 @@
         <v>n/a</v>
       </c>
       <c r="I42" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J42">
@@ -68187,7 +69181,7 @@
         <v>n/a</v>
       </c>
       <c r="I43" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J43">
@@ -68325,7 +69319,7 @@
         <v>n/a</v>
       </c>
       <c r="I44" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J44">
@@ -68466,7 +69460,7 @@
         <v>n/a</v>
       </c>
       <c r="I45" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J45">
@@ -68601,7 +69595,7 @@
         <v>n/a</v>
       </c>
       <c r="I46" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J46">
@@ -68736,7 +69730,7 @@
         <v>n/a</v>
       </c>
       <c r="I47" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J47">
@@ -68871,7 +69865,7 @@
         <v>n/a</v>
       </c>
       <c r="I48" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J48">
@@ -69006,7 +70000,7 @@
         <v>n/a</v>
       </c>
       <c r="I49" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J49">
@@ -69141,7 +70135,7 @@
         <v>n/a</v>
       </c>
       <c r="I50" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J50">
@@ -69279,7 +70273,7 @@
         <v>n/a</v>
       </c>
       <c r="I51" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J51">
@@ -69421,7 +70415,7 @@
         <v>s-curve</v>
       </c>
       <c r="I52" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.93664816809218165</v>
       </c>
       <c r="J52">
@@ -69556,7 +70550,7 @@
         <v>n/a</v>
       </c>
       <c r="I53" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J53">
@@ -69691,7 +70685,7 @@
         <v>n/a</v>
       </c>
       <c r="I54" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J54">
@@ -69827,7 +70821,7 @@
         <v>linear</v>
       </c>
       <c r="I55" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.3351831907818346E-2</v>
       </c>
       <c r="J55">
@@ -69962,7 +70956,7 @@
         <v>n/a</v>
       </c>
       <c r="I56" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J56">
@@ -70097,7 +71091,7 @@
         <v>n/a</v>
       </c>
       <c r="I57" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J57">
@@ -70235,7 +71229,7 @@
         <v>n/a</v>
       </c>
       <c r="I58" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J58">
@@ -70376,7 +71370,7 @@
         <v>n/a</v>
       </c>
       <c r="I59" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J59">
@@ -70511,7 +71505,7 @@
         <v>n/a</v>
       </c>
       <c r="I60" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J60">
@@ -70646,7 +71640,7 @@
         <v>n/a</v>
       </c>
       <c r="I61" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J61">
@@ -70781,7 +71775,7 @@
         <v>n/a</v>
       </c>
       <c r="I62" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J62">
@@ -70916,7 +71910,7 @@
         <v>n/a</v>
       </c>
       <c r="I63" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J63">
@@ -71051,7 +72045,7 @@
         <v>n/a</v>
       </c>
       <c r="I64" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J64">
@@ -71189,7 +72183,7 @@
         <v>n/a</v>
       </c>
       <c r="I65" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J65">
@@ -71330,7 +72324,7 @@
         <v>n/a</v>
       </c>
       <c r="I66" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J66">
@@ -71465,7 +72459,7 @@
         <v>n/a</v>
       </c>
       <c r="I67" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J67">
@@ -71600,7 +72594,7 @@
         <v>n/a</v>
       </c>
       <c r="I68" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J68">
@@ -71735,7 +72729,7 @@
         <v>n/a</v>
       </c>
       <c r="I69" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J69">
@@ -71870,7 +72864,7 @@
         <v>n/a</v>
       </c>
       <c r="I70" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J70">
@@ -72005,7 +72999,7 @@
         <v>n/a</v>
       </c>
       <c r="I71" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J71">
@@ -72143,7 +73137,7 @@
         <v>n/a</v>
       </c>
       <c r="I72" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J72">
@@ -72284,7 +73278,7 @@
         <v>n/a</v>
       </c>
       <c r="I73" s="22">
-        <f t="shared" ref="I73:I93" si="3">E73</f>
+        <f t="shared" ref="I73:I93" si="4">E73</f>
         <v>0</v>
       </c>
       <c r="J73">
@@ -72419,7 +73413,7 @@
         <v>n/a</v>
       </c>
       <c r="I74" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J74">
@@ -72554,7 +73548,7 @@
         <v>n/a</v>
       </c>
       <c r="I75" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J75">
@@ -72689,7 +73683,7 @@
         <v>n/a</v>
       </c>
       <c r="I76" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J76">
@@ -72824,7 +73818,7 @@
         <v>n/a</v>
       </c>
       <c r="I77" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J77">
@@ -72959,7 +73953,7 @@
         <v>n/a</v>
       </c>
       <c r="I78" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J78">
@@ -73097,7 +74091,7 @@
         <v>n/a</v>
       </c>
       <c r="I79" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J79">
@@ -73239,7 +74233,7 @@
         <v>s-curve</v>
       </c>
       <c r="I80" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J80">
@@ -73375,7 +74369,7 @@
         <v>n/a</v>
       </c>
       <c r="I81" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J81">
@@ -73510,7 +74504,7 @@
         <v>n/a</v>
       </c>
       <c r="I82" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="J82">
@@ -73646,7 +74640,7 @@
         <v>n/a</v>
       </c>
       <c r="I83" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J83">
@@ -73782,7 +74776,7 @@
         <v>n/a</v>
       </c>
       <c r="I84" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J84">
@@ -73918,7 +74912,7 @@
         <v>n/a</v>
       </c>
       <c r="I85" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J85">
@@ -74057,7 +75051,7 @@
         <v>n/a</v>
       </c>
       <c r="I86" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J86">
@@ -74198,7 +75192,7 @@
         <v>n/a</v>
       </c>
       <c r="I87" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J87">
@@ -74333,7 +75327,7 @@
         <v>n/a</v>
       </c>
       <c r="I88" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J88">
@@ -74468,7 +75462,7 @@
         <v>n/a</v>
       </c>
       <c r="I89" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J89">
@@ -74603,7 +75597,7 @@
         <v>n/a</v>
       </c>
       <c r="I90" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J90">
@@ -74738,7 +75732,7 @@
         <v>n/a</v>
       </c>
       <c r="I91" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J91">
@@ -74873,7 +75867,7 @@
         <v>n/a</v>
       </c>
       <c r="I92" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J92">
@@ -75011,7 +76005,7 @@
         <v>n/a</v>
       </c>
       <c r="I93" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J93">

</xml_diff>

<commit_message>
Add EPA HDV rules to BAU
</commit_message>
<xml_diff>
--- a/InputData/trans/TTS/Transportation Technology Shareweights.xlsx
+++ b/InputData/trans/TTS/Transportation Technology Shareweights.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\trans\TTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEC53A5-C5F7-4C86-A85B-F3095DE5179A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FE2570-F505-44B1-9FF4-BC2CA26D0CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="1004">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1838" uniqueCount="1005">
   <si>
     <t>Source:</t>
   </si>
@@ -3063,6 +3063,9 @@
   </si>
   <si>
     <t>2033, LDV PHEVs</t>
+  </si>
+  <si>
+    <t>2023, freight LDV BEVs</t>
   </si>
 </sst>
 </file>
@@ -4741,94 +4744,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0" formatCode="0.0000">
-                  <c:v>0.2</c:v>
+                  <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2579411882892142</c:v>
+                  <c:v>0.17745114499368292</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.27627957191928759</c:v>
+                  <c:v>0.19031199220093176</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.2996426865499332</c:v>
+                  <c:v>0.20876765729184479</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.32888715966126825</c:v>
+                  <c:v>0.23478791575173236</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.36469629744075793</c:v>
+                  <c:v>0.27057340516541462</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.40738008065427683</c:v>
+                  <c:v>0.31814369472520548</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.45665704065968565</c:v>
+                  <c:v>0.37860020816449586</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.51148861284062241</c:v>
+                  <c:v>0.45119213970807381</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.57005612372500036</c:v>
+                  <c:v>0.53264110228439376</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.62994387627499959</c:v>
+                  <c:v>0.61735889771560626</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.68851138715937765</c:v>
+                  <c:v>0.6988078602919261</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.74334295934031447</c:v>
+                  <c:v>0.77139979183550411</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.79261991934572329</c:v>
+                  <c:v>0.83185630527479459</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.83530370255924202</c:v>
+                  <c:v>0.87942659483458541</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.87111284033873182</c:v>
+                  <c:v>0.91521208424826761</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.90035731345006687</c:v>
+                  <c:v>0.94123234270815526</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.92372042808071253</c:v>
+                  <c:v>0.95968800779906827</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.94205881171078576</c:v>
+                  <c:v>0.97254885500631716</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.95625494622724738</c:v>
+                  <c:v>0.981400919704289</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.96712697743962805</c:v>
+                  <c:v>0.98744207306071796</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.97538491251428172</c:v>
+                  <c:v>0.99154096841313133</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.98161810407197958</c:v>
+                  <c:v>0.99431107671435792</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.98630077334741784</c:v>
+                  <c:v>0.99617816781320001</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.98980612042871075</c:v>
+                  <c:v>0.99743434612399795</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.99242316513444306</c:v>
+                  <c:v>0.99827847766930755</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.99437313027600394</c:v>
+                  <c:v>0.99884525804213542</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.99582389944515337</c:v>
+                  <c:v>0.99922560648475944</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.99690207724746327</c:v>
+                  <c:v>0.99948075254448077</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.99770269667543965</c:v>
+                  <c:v>0.9996518679097619</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5692,6 +5695,347 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$I$17:$AL$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0" formatCode="0.0000">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.17745114499368292</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19031199220093176</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.20876765729184479</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.23478791575173236</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.27057340516541462</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.31814369472520548</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.37860020816449586</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.45119213970807381</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.53264110228439376</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.61735889771560626</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.6988078602919261</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.77139979183550411</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.83185630527479459</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.87942659483458541</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.91521208424826761</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.94123234270815526</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.95968800779906827</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.97254885500631716</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.981400919704289</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.98744207306071796</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.99154096841313133</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.99431107671435792</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.99617816781320001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.99743434612399795</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.99827847766930755</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.99884525804213542</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.99922560648475944</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.99948075254448077</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.9996518679097619</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B905-4226-A18C-07289D02ECCA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1637983919"/>
+        <c:axId val="1637988239"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1637983919"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1637988239"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1637988239"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1637983919"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -5813,6 +6157,46 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -7916,6 +8300,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -8033,16 +8933,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8062,6 +8962,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7531E0B0-E8D0-FDE4-AA2E-6B666C6B162E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -10068,123 +11004,123 @@
       </c>
       <c r="B2">
         <f>Data!I17</f>
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="C2">
         <f>Data!J17</f>
-        <v>0.2579411882892142</v>
+        <v>0.17745114499368292</v>
       </c>
       <c r="D2">
         <f>Data!K17</f>
-        <v>0.27627957191928759</v>
+        <v>0.19031199220093176</v>
       </c>
       <c r="E2">
         <f>Data!L17</f>
-        <v>0.2996426865499332</v>
+        <v>0.20876765729184479</v>
       </c>
       <c r="F2">
         <f>Data!M17</f>
-        <v>0.32888715966126825</v>
+        <v>0.23478791575173236</v>
       </c>
       <c r="G2">
         <f>Data!N17</f>
-        <v>0.36469629744075793</v>
+        <v>0.27057340516541462</v>
       </c>
       <c r="H2">
         <f>Data!O17</f>
-        <v>0.40738008065427683</v>
+        <v>0.31814369472520548</v>
       </c>
       <c r="I2">
         <f>Data!P17</f>
-        <v>0.45665704065968565</v>
+        <v>0.37860020816449586</v>
       </c>
       <c r="J2">
         <f>Data!Q17</f>
-        <v>0.51148861284062241</v>
+        <v>0.45119213970807381</v>
       </c>
       <c r="K2">
         <f>Data!R17</f>
-        <v>0.57005612372500036</v>
+        <v>0.53264110228439376</v>
       </c>
       <c r="L2">
         <f>Data!S17</f>
-        <v>0.62994387627499959</v>
+        <v>0.61735889771560626</v>
       </c>
       <c r="M2">
         <f>Data!T17</f>
-        <v>0.68851138715937765</v>
+        <v>0.6988078602919261</v>
       </c>
       <c r="N2">
         <f>Data!U17</f>
-        <v>0.74334295934031447</v>
+        <v>0.77139979183550411</v>
       </c>
       <c r="O2">
         <f>Data!V17</f>
-        <v>0.79261991934572329</v>
+        <v>0.83185630527479459</v>
       </c>
       <c r="P2">
         <f>Data!W17</f>
-        <v>0.83530370255924202</v>
+        <v>0.87942659483458541</v>
       </c>
       <c r="Q2">
         <f>Data!X17</f>
-        <v>0.87111284033873182</v>
+        <v>0.91521208424826761</v>
       </c>
       <c r="R2">
         <f>Data!Y17</f>
-        <v>0.90035731345006687</v>
+        <v>0.94123234270815526</v>
       </c>
       <c r="S2">
         <f>Data!Z17</f>
-        <v>0.92372042808071253</v>
+        <v>0.95968800779906827</v>
       </c>
       <c r="T2">
         <f>Data!AA17</f>
-        <v>0.94205881171078576</v>
+        <v>0.97254885500631716</v>
       </c>
       <c r="U2">
         <f>Data!AB17</f>
-        <v>0.95625494622724738</v>
+        <v>0.981400919704289</v>
       </c>
       <c r="V2">
         <f>Data!AC17</f>
-        <v>0.96712697743962805</v>
+        <v>0.98744207306071796</v>
       </c>
       <c r="W2">
         <f>Data!AD17</f>
-        <v>0.97538491251428172</v>
+        <v>0.99154096841313133</v>
       </c>
       <c r="X2">
         <f>Data!AE17</f>
-        <v>0.98161810407197958</v>
+        <v>0.99431107671435792</v>
       </c>
       <c r="Y2">
         <f>Data!AF17</f>
-        <v>0.98630077334741784</v>
+        <v>0.99617816781320001</v>
       </c>
       <c r="Z2">
         <f>Data!AG17</f>
-        <v>0.98980612042871075</v>
+        <v>0.99743434612399795</v>
       </c>
       <c r="AA2">
         <f>Data!AH17</f>
-        <v>0.99242316513444306</v>
+        <v>0.99827847766930755</v>
       </c>
       <c r="AB2">
         <f>Data!AI17</f>
-        <v>0.99437313027600394</v>
+        <v>0.99884525804213542</v>
       </c>
       <c r="AC2">
         <f>Data!AJ17</f>
-        <v>0.99582389944515337</v>
+        <v>0.99922560648475944</v>
       </c>
       <c r="AD2">
         <f>Data!AK17</f>
-        <v>0.99690207724746327</v>
+        <v>0.99948075254448077</v>
       </c>
       <c r="AE2">
         <f>Data!AL17</f>
-        <v>0.99770269667543965</v>
+        <v>0.9996518679097619</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -64288,8 +65224,8 @@
   </sheetPr>
   <dimension ref="A1:AL93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64329,6 +65265,10 @@
         <v>1000</v>
       </c>
       <c r="U1" s="17"/>
+      <c r="W1" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="X1" s="17"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -64358,6 +65298,12 @@
       <c r="U2" s="19">
         <v>1</v>
       </c>
+      <c r="W2" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="X2" s="19">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -64387,6 +65333,12 @@
       <c r="U3" s="19">
         <v>-0.42</v>
       </c>
+      <c r="W3" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="X3" s="19">
+        <v>-0.4</v>
+      </c>
     </row>
     <row r="4" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -64416,13 +65368,19 @@
       <c r="U4" s="20">
         <v>-11</v>
       </c>
+      <c r="W4" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="X4" s="20">
+        <v>-10.5</v>
+      </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:38" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -64441,6 +65399,27 @@
       </c>
       <c r="O6" s="22">
         <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="R6" s="49" t="s">
+        <v>1001</v>
+      </c>
+      <c r="S6">
+        <v>0.05</v>
+      </c>
+      <c r="T6">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="U6">
+        <v>7.8E-2</v>
+      </c>
+      <c r="V6">
+        <v>0.09</v>
+      </c>
+      <c r="W6">
+        <v>0.12</v>
+      </c>
+      <c r="X6">
+        <v>0.15</v>
       </c>
     </row>
     <row r="7" spans="1:38" ht="30" x14ac:dyDescent="0.25">
@@ -64474,26 +65453,8 @@
       <c r="G8" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="N8" s="49" t="s">
-        <v>1001</v>
-      </c>
-      <c r="O8">
-        <v>0.05</v>
-      </c>
-      <c r="P8">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="Q8">
-        <v>7.8E-2</v>
-      </c>
-      <c r="R8">
-        <v>0.09</v>
-      </c>
-      <c r="S8">
-        <v>0.12</v>
-      </c>
-      <c r="T8">
-        <v>0.15</v>
+      <c r="N8" t="s">
+        <v>1004</v>
       </c>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
@@ -65246,7 +66207,7 @@
         <v>0.11799999999999999</v>
       </c>
       <c r="T14" s="15">
-        <f t="shared" ref="T14" si="2">T8</f>
+        <f>X6</f>
         <v>0.15</v>
       </c>
       <c r="U14">
@@ -65610,7 +66571,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="22">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="F17">
         <f>F10</f>
@@ -65622,123 +66583,123 @@
       </c>
       <c r="I17" s="22">
         <f t="shared" si="1"/>
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="J17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:J$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,J$9))</f>
-        <v>0.2579411882892142</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:J$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,J$9))</f>
+        <v>0.17745114499368292</v>
       </c>
       <c r="K17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:K$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,K$9))</f>
-        <v>0.27627957191928759</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:K$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,K$9))</f>
+        <v>0.19031199220093176</v>
       </c>
       <c r="L17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:L$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,L$9))</f>
-        <v>0.2996426865499332</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:L$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,L$9))</f>
+        <v>0.20876765729184479</v>
       </c>
       <c r="M17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:M$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,M$9))</f>
-        <v>0.32888715966126825</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:M$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,M$9))</f>
+        <v>0.23478791575173236</v>
       </c>
       <c r="N17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:N$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,N$9))</f>
-        <v>0.36469629744075793</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:N$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,N$9))</f>
+        <v>0.27057340516541462</v>
       </c>
       <c r="O17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:O$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,O$9))</f>
-        <v>0.40738008065427683</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:O$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,O$9))</f>
+        <v>0.31814369472520548</v>
       </c>
       <c r="P17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:P$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,P$9))</f>
-        <v>0.45665704065968565</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:P$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,P$9))</f>
+        <v>0.37860020816449586</v>
       </c>
       <c r="Q17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:Q$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,Q$9))</f>
-        <v>0.51148861284062241</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:Q$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,Q$9))</f>
+        <v>0.45119213970807381</v>
       </c>
       <c r="R17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:R$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,R$9))</f>
-        <v>0.57005612372500036</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:R$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,R$9))</f>
+        <v>0.53264110228439376</v>
       </c>
       <c r="S17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:S$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,S$9))</f>
-        <v>0.62994387627499959</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:S$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,S$9))</f>
+        <v>0.61735889771560626</v>
       </c>
       <c r="T17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:T$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,T$9))</f>
-        <v>0.68851138715937765</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:T$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,T$9))</f>
+        <v>0.6988078602919261</v>
       </c>
       <c r="U17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:U$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,U$9))</f>
-        <v>0.74334295934031447</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:U$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,U$9))</f>
+        <v>0.77139979183550411</v>
       </c>
       <c r="V17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:V$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,V$9))</f>
-        <v>0.79261991934572329</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:V$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,V$9))</f>
+        <v>0.83185630527479459</v>
       </c>
       <c r="W17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:W$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,W$9))</f>
-        <v>0.83530370255924202</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:W$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,W$9))</f>
+        <v>0.87942659483458541</v>
       </c>
       <c r="X17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:X$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,X$9))</f>
-        <v>0.87111284033873182</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:X$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,X$9))</f>
+        <v>0.91521208424826761</v>
       </c>
       <c r="Y17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:Y$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,Y$9))</f>
-        <v>0.90035731345006687</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:Y$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,Y$9))</f>
+        <v>0.94123234270815526</v>
       </c>
       <c r="Z17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:Z$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,Z$9))</f>
-        <v>0.92372042808071253</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:Z$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,Z$9))</f>
+        <v>0.95968800779906827</v>
       </c>
       <c r="AA17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:AA$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,AA$9))</f>
-        <v>0.94205881171078576</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:AA$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,AA$9))</f>
+        <v>0.97254885500631716</v>
       </c>
       <c r="AB17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:AB$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,AB$9))</f>
-        <v>0.95625494622724738</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:AB$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,AB$9))</f>
+        <v>0.981400919704289</v>
       </c>
       <c r="AC17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:AC$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,AC$9))</f>
-        <v>0.96712697743962805</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:AC$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,AC$9))</f>
+        <v>0.98744207306071796</v>
       </c>
       <c r="AD17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:AD$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,AD$9))</f>
-        <v>0.97538491251428172</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:AD$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,AD$9))</f>
+        <v>0.99154096841313133</v>
       </c>
       <c r="AE17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:AE$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,AE$9))</f>
-        <v>0.98161810407197958</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:AE$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,AE$9))</f>
+        <v>0.99431107671435792</v>
       </c>
       <c r="AF17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:AF$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,AF$9))</f>
-        <v>0.98630077334741784</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:AF$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,AF$9))</f>
+        <v>0.99617816781320001</v>
       </c>
       <c r="AG17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:AG$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,AG$9))</f>
-        <v>0.98980612042871075</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:AG$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,AG$9))</f>
+        <v>0.99743434612399795</v>
       </c>
       <c r="AH17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:AH$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,AH$9))</f>
-        <v>0.99242316513444306</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:AH$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,AH$9))</f>
+        <v>0.99827847766930755</v>
       </c>
       <c r="AI17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:AI$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,AI$9))</f>
-        <v>0.99437313027600394</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:AI$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,AI$9))</f>
+        <v>0.99884525804213542</v>
       </c>
       <c r="AJ17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:AJ$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,AJ$9))</f>
-        <v>0.99582389944515337</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:AJ$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,AJ$9))</f>
+        <v>0.99922560648475944</v>
       </c>
       <c r="AK17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:AK$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,AK$9))</f>
-        <v>0.99690207724746327</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:AK$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,AK$9))</f>
+        <v>0.99948075254448077</v>
       </c>
       <c r="AL17">
-        <f>IF($G17="s-curve",$E17+($F17-$E17)*$O$2/(1+EXP($O$3*(COUNT($I$9:AL$9)+$O$4))),TREND($E17:$F17,$E$9:$F$9,AL$9))</f>
-        <v>0.99770269667543965</v>
+        <f>IF($G17="s-curve",$E17+($F17-$E17)*$X$2/(1+EXP($X$3*(COUNT($I$9:AL$9)+$X$4))),TREND($E17:$F17,$E$9:$F$9,AL$9))</f>
+        <v>0.9996518679097619</v>
       </c>
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.25">
@@ -66019,7 +66980,7 @@
       <c r="E20" s="22">
         <v>1</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="29">
         <v>1</v>
       </c>
       <c r="G20" s="7" t="str">
@@ -68911,7 +69872,7 @@
         <v>n/a</v>
       </c>
       <c r="I41" s="22">
-        <f t="shared" ref="I41:I72" si="3">E41</f>
+        <f t="shared" ref="I41:I72" si="2">E41</f>
         <v>1</v>
       </c>
       <c r="J41">
@@ -69046,7 +70007,7 @@
         <v>n/a</v>
       </c>
       <c r="I42" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J42">
@@ -69181,7 +70142,7 @@
         <v>n/a</v>
       </c>
       <c r="I43" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J43">
@@ -69319,7 +70280,7 @@
         <v>n/a</v>
       </c>
       <c r="I44" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J44">
@@ -69460,7 +70421,7 @@
         <v>n/a</v>
       </c>
       <c r="I45" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J45">
@@ -69595,7 +70556,7 @@
         <v>n/a</v>
       </c>
       <c r="I46" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J46">
@@ -69730,7 +70691,7 @@
         <v>n/a</v>
       </c>
       <c r="I47" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J47">
@@ -69865,7 +70826,7 @@
         <v>n/a</v>
       </c>
       <c r="I48" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J48">
@@ -70000,7 +70961,7 @@
         <v>n/a</v>
       </c>
       <c r="I49" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J49">
@@ -70135,7 +71096,7 @@
         <v>n/a</v>
       </c>
       <c r="I50" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J50">
@@ -70273,7 +71234,7 @@
         <v>n/a</v>
       </c>
       <c r="I51" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J51">
@@ -70415,7 +71376,7 @@
         <v>s-curve</v>
       </c>
       <c r="I52" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.93664816809218165</v>
       </c>
       <c r="J52">
@@ -70550,7 +71511,7 @@
         <v>n/a</v>
       </c>
       <c r="I53" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J53">
@@ -70685,7 +71646,7 @@
         <v>n/a</v>
       </c>
       <c r="I54" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J54">
@@ -70821,7 +71782,7 @@
         <v>linear</v>
       </c>
       <c r="I55" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>6.3351831907818346E-2</v>
       </c>
       <c r="J55">
@@ -70956,7 +71917,7 @@
         <v>n/a</v>
       </c>
       <c r="I56" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J56">
@@ -71091,7 +72052,7 @@
         <v>n/a</v>
       </c>
       <c r="I57" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J57">
@@ -71229,7 +72190,7 @@
         <v>n/a</v>
       </c>
       <c r="I58" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J58">
@@ -71370,7 +72331,7 @@
         <v>n/a</v>
       </c>
       <c r="I59" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J59">
@@ -71505,7 +72466,7 @@
         <v>n/a</v>
       </c>
       <c r="I60" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J60">
@@ -71640,7 +72601,7 @@
         <v>n/a</v>
       </c>
       <c r="I61" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J61">
@@ -71775,7 +72736,7 @@
         <v>n/a</v>
       </c>
       <c r="I62" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J62">
@@ -71910,7 +72871,7 @@
         <v>n/a</v>
       </c>
       <c r="I63" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J63">
@@ -72045,7 +73006,7 @@
         <v>n/a</v>
       </c>
       <c r="I64" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J64">
@@ -72183,7 +73144,7 @@
         <v>n/a</v>
       </c>
       <c r="I65" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J65">
@@ -72324,7 +73285,7 @@
         <v>n/a</v>
       </c>
       <c r="I66" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J66">
@@ -72459,7 +73420,7 @@
         <v>n/a</v>
       </c>
       <c r="I67" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J67">
@@ -72594,7 +73555,7 @@
         <v>n/a</v>
       </c>
       <c r="I68" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J68">
@@ -72729,7 +73690,7 @@
         <v>n/a</v>
       </c>
       <c r="I69" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J69">
@@ -72864,7 +73825,7 @@
         <v>n/a</v>
       </c>
       <c r="I70" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J70">
@@ -72999,7 +73960,7 @@
         <v>n/a</v>
       </c>
       <c r="I71" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J71">
@@ -73137,7 +74098,7 @@
         <v>n/a</v>
       </c>
       <c r="I72" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J72">
@@ -73278,7 +74239,7 @@
         <v>n/a</v>
       </c>
       <c r="I73" s="22">
-        <f t="shared" ref="I73:I93" si="4">E73</f>
+        <f t="shared" ref="I73:I93" si="3">E73</f>
         <v>0</v>
       </c>
       <c r="J73">
@@ -73413,7 +74374,7 @@
         <v>n/a</v>
       </c>
       <c r="I74" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J74">
@@ -73548,7 +74509,7 @@
         <v>n/a</v>
       </c>
       <c r="I75" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J75">
@@ -73683,7 +74644,7 @@
         <v>n/a</v>
       </c>
       <c r="I76" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J76">
@@ -73818,7 +74779,7 @@
         <v>n/a</v>
       </c>
       <c r="I77" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J77">
@@ -73953,7 +74914,7 @@
         <v>n/a</v>
       </c>
       <c r="I78" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J78">
@@ -74091,7 +75052,7 @@
         <v>n/a</v>
       </c>
       <c r="I79" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J79">
@@ -74233,7 +75194,7 @@
         <v>s-curve</v>
       </c>
       <c r="I80" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J80">
@@ -74369,7 +75330,7 @@
         <v>n/a</v>
       </c>
       <c r="I81" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J81">
@@ -74504,7 +75465,7 @@
         <v>n/a</v>
       </c>
       <c r="I82" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="J82">
@@ -74640,7 +75601,7 @@
         <v>n/a</v>
       </c>
       <c r="I83" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J83">
@@ -74776,7 +75737,7 @@
         <v>n/a</v>
       </c>
       <c r="I84" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J84">
@@ -74912,7 +75873,7 @@
         <v>n/a</v>
       </c>
       <c r="I85" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J85">
@@ -75051,7 +76012,7 @@
         <v>n/a</v>
       </c>
       <c r="I86" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J86">
@@ -75192,7 +76153,7 @@
         <v>n/a</v>
       </c>
       <c r="I87" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J87">
@@ -75327,7 +76288,7 @@
         <v>n/a</v>
       </c>
       <c r="I88" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J88">
@@ -75462,7 +76423,7 @@
         <v>n/a</v>
       </c>
       <c r="I89" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J89">
@@ -75597,7 +76558,7 @@
         <v>n/a</v>
       </c>
       <c r="I90" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J90">
@@ -75732,7 +76693,7 @@
         <v>n/a</v>
       </c>
       <c r="I91" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J91">
@@ -75867,7 +76828,7 @@
         <v>n/a</v>
       </c>
       <c r="I92" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J92">
@@ -76005,7 +76966,7 @@
         <v>n/a</v>
       </c>
       <c r="I93" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J93">

</xml_diff>